<commit_message>
hyperparameters tuning for neural prophet
</commit_message>
<xml_diff>
--- a/holidays.xlsx
+++ b/holidays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namtrantuan\Desktop\passenger_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0E5BE0-3A4B-4686-8D3D-C1A8FD9561B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C4ECAD-CAF9-42D0-9600-B3FF316BD9D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C81195CF-3238-4C84-B228-279AE06B6B57}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="covid" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">covid!$A$1:$B$477</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">covid!$A$1:$B$999</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,9 +45,6 @@
     <t>ds</t>
   </si>
   <si>
-    <t>holiday</t>
-  </si>
-  <si>
     <t>Lunar</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>Summer</t>
+  </si>
+  <si>
+    <t>holiday</t>
   </si>
 </sst>
 </file>
@@ -410,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9708BE-FF7E-456D-97C7-E4E782A5149C}">
   <dimension ref="A1:B999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="B477" sqref="B477"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -424,7 +424,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4240,7 +4240,7 @@
         <v>44941</v>
       </c>
       <c r="B478" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>44942</v>
       </c>
       <c r="B479" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.2">
@@ -4256,7 +4256,7 @@
         <v>44943</v>
       </c>
       <c r="B480" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.2">
@@ -4264,7 +4264,7 @@
         <v>44944</v>
       </c>
       <c r="B481" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.2">
@@ -4272,7 +4272,7 @@
         <v>44945</v>
       </c>
       <c r="B482" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.2">
@@ -4280,7 +4280,7 @@
         <v>44946</v>
       </c>
       <c r="B483" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
@@ -4288,7 +4288,7 @@
         <v>44948</v>
       </c>
       <c r="B484" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.2">
@@ -4296,7 +4296,7 @@
         <v>44949</v>
       </c>
       <c r="B485" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.2">
@@ -4304,7 +4304,7 @@
         <v>44950</v>
       </c>
       <c r="B486" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.2">
@@ -4312,7 +4312,7 @@
         <v>44951</v>
       </c>
       <c r="B487" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.2">
@@ -4320,7 +4320,7 @@
         <v>44952</v>
       </c>
       <c r="B488" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.2">
@@ -4328,7 +4328,7 @@
         <v>44953</v>
       </c>
       <c r="B489" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.2">
@@ -4336,7 +4336,7 @@
         <v>44954</v>
       </c>
       <c r="B490" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.2">
@@ -4344,7 +4344,7 @@
         <v>44955</v>
       </c>
       <c r="B491" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.2">
@@ -4352,7 +4352,7 @@
         <v>44956</v>
       </c>
       <c r="B492" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>44957</v>
       </c>
       <c r="B493" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.2">
@@ -4368,7 +4368,7 @@
         <v>44587</v>
       </c>
       <c r="B494" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.2">
@@ -4376,7 +4376,7 @@
         <v>44588</v>
       </c>
       <c r="B495" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.2">
@@ -4384,7 +4384,7 @@
         <v>44589</v>
       </c>
       <c r="B496" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.2">
@@ -4392,7 +4392,7 @@
         <v>44590</v>
       </c>
       <c r="B497" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.2">
@@ -4400,7 +4400,7 @@
         <v>44591</v>
       </c>
       <c r="B498" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.2">
@@ -4408,7 +4408,7 @@
         <v>44593</v>
       </c>
       <c r="B499" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.2">
@@ -4416,7 +4416,7 @@
         <v>44594</v>
       </c>
       <c r="B500" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.2">
@@ -4424,7 +4424,7 @@
         <v>44595</v>
       </c>
       <c r="B501" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.2">
@@ -4432,7 +4432,7 @@
         <v>44596</v>
       </c>
       <c r="B502" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.2">
@@ -4440,7 +4440,7 @@
         <v>44597</v>
       </c>
       <c r="B503" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.2">
@@ -4448,7 +4448,7 @@
         <v>44598</v>
       </c>
       <c r="B504" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
@@ -4456,7 +4456,7 @@
         <v>44599</v>
       </c>
       <c r="B505" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
@@ -4464,7 +4464,7 @@
         <v>44600</v>
       </c>
       <c r="B506" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
@@ -4472,7 +4472,7 @@
         <v>44601</v>
       </c>
       <c r="B507" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.2">
@@ -4480,7 +4480,7 @@
         <v>44602</v>
       </c>
       <c r="B508" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.2">
@@ -4488,7 +4488,7 @@
         <v>42047</v>
       </c>
       <c r="B509" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
@@ -4496,7 +4496,7 @@
         <v>42048</v>
       </c>
       <c r="B510" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.2">
@@ -4504,7 +4504,7 @@
         <v>42049</v>
       </c>
       <c r="B511" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
@@ -4512,7 +4512,7 @@
         <v>42050</v>
       </c>
       <c r="B512" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
@@ -4520,7 +4520,7 @@
         <v>42051</v>
       </c>
       <c r="B513" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
@@ -4528,7 +4528,7 @@
         <v>42052</v>
       </c>
       <c r="B514" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.2">
@@ -4536,7 +4536,7 @@
         <v>42055</v>
       </c>
       <c r="B515" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.2">
@@ -4544,7 +4544,7 @@
         <v>42056</v>
       </c>
       <c r="B516" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.2">
@@ -4552,7 +4552,7 @@
         <v>42057</v>
       </c>
       <c r="B517" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.2">
@@ -4560,7 +4560,7 @@
         <v>42058</v>
       </c>
       <c r="B518" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.2">
@@ -4568,7 +4568,7 @@
         <v>42059</v>
       </c>
       <c r="B519" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.2">
@@ -4576,7 +4576,7 @@
         <v>42060</v>
       </c>
       <c r="B520" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.2">
@@ -4584,7 +4584,7 @@
         <v>42061</v>
       </c>
       <c r="B521" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
@@ -4592,7 +4592,7 @@
         <v>42062</v>
       </c>
       <c r="B522" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
@@ -4600,7 +4600,7 @@
         <v>42063</v>
       </c>
       <c r="B523" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
@@ -4608,7 +4608,7 @@
         <v>42064</v>
       </c>
       <c r="B524" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.2">
@@ -4616,7 +4616,7 @@
         <v>42065</v>
       </c>
       <c r="B525" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.2">
@@ -4624,7 +4624,7 @@
         <v>42402</v>
       </c>
       <c r="B526" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.2">
@@ -4632,7 +4632,7 @@
         <v>42403</v>
       </c>
       <c r="B527" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.2">
@@ -4640,7 +4640,7 @@
         <v>42404</v>
       </c>
       <c r="B528" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.2">
@@ -4648,7 +4648,7 @@
         <v>42405</v>
       </c>
       <c r="B529" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.2">
@@ -4656,7 +4656,7 @@
         <v>42406</v>
       </c>
       <c r="B530" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.2">
@@ -4664,7 +4664,7 @@
         <v>42409</v>
       </c>
       <c r="B531" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>42410</v>
       </c>
       <c r="B532" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.2">
@@ -4680,7 +4680,7 @@
         <v>42411</v>
       </c>
       <c r="B533" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.2">
@@ -4688,7 +4688,7 @@
         <v>42412</v>
       </c>
       <c r="B534" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.2">
@@ -4696,7 +4696,7 @@
         <v>42413</v>
       </c>
       <c r="B535" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.2">
@@ -4704,7 +4704,7 @@
         <v>42414</v>
       </c>
       <c r="B536" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.2">
@@ -4712,7 +4712,7 @@
         <v>42415</v>
       </c>
       <c r="B537" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.2">
@@ -4720,7 +4720,7 @@
         <v>42416</v>
       </c>
       <c r="B538" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.2">
@@ -4728,7 +4728,7 @@
         <v>42756</v>
       </c>
       <c r="B539" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.2">
@@ -4736,7 +4736,7 @@
         <v>42757</v>
       </c>
       <c r="B540" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.2">
@@ -4744,7 +4744,7 @@
         <v>42758</v>
       </c>
       <c r="B541" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.2">
@@ -4752,7 +4752,7 @@
         <v>42759</v>
       </c>
       <c r="B542" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.2">
@@ -4760,7 +4760,7 @@
         <v>42760</v>
       </c>
       <c r="B543" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.2">
@@ -4768,7 +4768,7 @@
         <v>42761</v>
       </c>
       <c r="B544" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.2">
@@ -4776,7 +4776,7 @@
         <v>42764</v>
       </c>
       <c r="B545" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.2">
@@ -4784,7 +4784,7 @@
         <v>42765</v>
       </c>
       <c r="B546" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.2">
@@ -4792,7 +4792,7 @@
         <v>42766</v>
       </c>
       <c r="B547" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.2">
@@ -4800,7 +4800,7 @@
         <v>42767</v>
       </c>
       <c r="B548" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.2">
@@ -4808,7 +4808,7 @@
         <v>42768</v>
       </c>
       <c r="B549" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.2">
@@ -4816,7 +4816,7 @@
         <v>42769</v>
       </c>
       <c r="B550" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.2">
@@ -4824,7 +4824,7 @@
         <v>42770</v>
       </c>
       <c r="B551" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.2">
@@ -4832,7 +4832,7 @@
         <v>42771</v>
       </c>
       <c r="B552" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.2">
@@ -4840,7 +4840,7 @@
         <v>42772</v>
       </c>
       <c r="B553" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.2">
@@ -4848,7 +4848,7 @@
         <v>43140</v>
       </c>
       <c r="B554" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.2">
@@ -4857,7 +4857,7 @@
         <v>43141</v>
       </c>
       <c r="B555" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.2">
@@ -4866,7 +4866,7 @@
         <v>43142</v>
       </c>
       <c r="B556" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.2">
@@ -4875,7 +4875,7 @@
         <v>43143</v>
       </c>
       <c r="B557" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
         <v>43144</v>
       </c>
       <c r="B558" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.2">
@@ -4893,7 +4893,7 @@
         <v>43145</v>
       </c>
       <c r="B559" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.2">
@@ -4901,7 +4901,7 @@
         <v>43148</v>
       </c>
       <c r="B560" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.2">
@@ -4910,7 +4910,7 @@
         <v>43149</v>
       </c>
       <c r="B561" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.2">
@@ -4919,7 +4919,7 @@
         <v>43150</v>
       </c>
       <c r="B562" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.2">
@@ -4928,7 +4928,7 @@
         <v>43151</v>
       </c>
       <c r="B563" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.2">
@@ -4937,7 +4937,7 @@
         <v>43152</v>
       </c>
       <c r="B564" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.2">
@@ -4946,7 +4946,7 @@
         <v>43153</v>
       </c>
       <c r="B565" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.2">
@@ -4955,7 +4955,7 @@
         <v>43154</v>
       </c>
       <c r="B566" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.2">
@@ -4964,7 +4964,7 @@
         <v>43155</v>
       </c>
       <c r="B567" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.2">
@@ -4973,7 +4973,7 @@
         <v>43156</v>
       </c>
       <c r="B568" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.2">
@@ -4982,7 +4982,7 @@
         <v>43157</v>
       </c>
       <c r="B569" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.2">
@@ -4991,7 +4991,7 @@
         <v>43158</v>
       </c>
       <c r="B570" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.2">
@@ -5000,7 +5000,7 @@
         <v>43159</v>
       </c>
       <c r="B571" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.2">
@@ -5008,7 +5008,7 @@
         <v>43494</v>
       </c>
       <c r="B572" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.2">
@@ -5016,7 +5016,7 @@
         <v>43495</v>
       </c>
       <c r="B573" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.2">
@@ -5024,7 +5024,7 @@
         <v>43496</v>
       </c>
       <c r="B574" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.2">
@@ -5032,7 +5032,7 @@
         <v>43497</v>
       </c>
       <c r="B575" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.2">
@@ -5040,7 +5040,7 @@
         <v>43498</v>
       </c>
       <c r="B576" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.2">
@@ -5048,7 +5048,7 @@
         <v>43499</v>
       </c>
       <c r="B577" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.2">
@@ -5056,7 +5056,7 @@
         <v>43500</v>
       </c>
       <c r="B578" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.2">
@@ -5064,7 +5064,7 @@
         <v>43502</v>
       </c>
       <c r="B579" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.2">
@@ -5072,7 +5072,7 @@
         <v>43503</v>
       </c>
       <c r="B580" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.2">
@@ -5080,7 +5080,7 @@
         <v>43504</v>
       </c>
       <c r="B581" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.2">
@@ -5088,7 +5088,7 @@
         <v>43505</v>
       </c>
       <c r="B582" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.2">
@@ -5096,7 +5096,7 @@
         <v>43506</v>
       </c>
       <c r="B583" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.2">
@@ -5104,7 +5104,7 @@
         <v>43507</v>
       </c>
       <c r="B584" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.2">
@@ -5112,7 +5112,7 @@
         <v>43508</v>
       </c>
       <c r="B585" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.2">
@@ -5120,7 +5120,7 @@
         <v>43509</v>
       </c>
       <c r="B586" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.2">
@@ -5128,7 +5128,7 @@
         <v>43510</v>
       </c>
       <c r="B587" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.2">
@@ -5136,7 +5136,7 @@
         <v>43511</v>
       </c>
       <c r="B588" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.2">
@@ -5144,7 +5144,7 @@
         <v>43512</v>
       </c>
       <c r="B589" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.2">
@@ -5153,7 +5153,7 @@
         <v>42118</v>
       </c>
       <c r="B590" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.2">
@@ -5162,7 +5162,7 @@
         <v>42119</v>
       </c>
       <c r="B591" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.2">
@@ -5171,7 +5171,7 @@
         <v>42120</v>
       </c>
       <c r="B592" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.2">
@@ -5180,7 +5180,7 @@
         <v>42121</v>
       </c>
       <c r="B593" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.2">
@@ -5189,7 +5189,7 @@
         <v>42122</v>
       </c>
       <c r="B594" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.2">
@@ -5198,7 +5198,7 @@
         <v>42123</v>
       </c>
       <c r="B595" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.2">
@@ -5206,7 +5206,7 @@
         <v>42124</v>
       </c>
       <c r="B596" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.2">
@@ -5215,7 +5215,7 @@
         <v>42125</v>
       </c>
       <c r="B597" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.2">
@@ -5224,7 +5224,7 @@
         <v>42126</v>
       </c>
       <c r="B598" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.2">
@@ -5233,7 +5233,7 @@
         <v>42127</v>
       </c>
       <c r="B599" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.2">
@@ -5242,7 +5242,7 @@
         <v>42128</v>
       </c>
       <c r="B600" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.2">
@@ -5251,7 +5251,7 @@
         <v>42484</v>
       </c>
       <c r="B601" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.2">
@@ -5260,7 +5260,7 @@
         <v>42485</v>
       </c>
       <c r="B602" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.2">
@@ -5269,7 +5269,7 @@
         <v>42486</v>
       </c>
       <c r="B603" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.2">
@@ -5278,7 +5278,7 @@
         <v>42487</v>
       </c>
       <c r="B604" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.2">
@@ -5287,7 +5287,7 @@
         <v>42488</v>
       </c>
       <c r="B605" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.2">
@@ -5296,7 +5296,7 @@
         <v>42489</v>
       </c>
       <c r="B606" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.2">
@@ -5305,7 +5305,7 @@
         <v>42490</v>
       </c>
       <c r="B607" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.2">
@@ -5314,7 +5314,7 @@
         <v>42491</v>
       </c>
       <c r="B608" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.2">
@@ -5323,7 +5323,7 @@
         <v>42492</v>
       </c>
       <c r="B609" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.2">
@@ -5332,7 +5332,7 @@
         <v>42493</v>
       </c>
       <c r="B610" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.2">
@@ -5340,7 +5340,7 @@
         <v>42494</v>
       </c>
       <c r="B611" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.2">
@@ -5349,7 +5349,7 @@
         <v>42851</v>
       </c>
       <c r="B612" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.2">
@@ -5358,7 +5358,7 @@
         <v>42852</v>
       </c>
       <c r="B613" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.2">
@@ -5367,7 +5367,7 @@
         <v>42853</v>
       </c>
       <c r="B614" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.2">
@@ -5376,7 +5376,7 @@
         <v>42854</v>
       </c>
       <c r="B615" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.2">
@@ -5385,7 +5385,7 @@
         <v>42855</v>
       </c>
       <c r="B616" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.2">
@@ -5394,7 +5394,7 @@
         <v>42856</v>
       </c>
       <c r="B617" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.2">
@@ -5403,7 +5403,7 @@
         <v>42857</v>
       </c>
       <c r="B618" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.2">
@@ -5412,7 +5412,7 @@
         <v>42858</v>
       </c>
       <c r="B619" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.2">
@@ -5420,7 +5420,7 @@
         <v>42859</v>
       </c>
       <c r="B620" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.2">
@@ -5428,7 +5428,7 @@
         <v>43217</v>
       </c>
       <c r="B621" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.2">
@@ -5437,7 +5437,7 @@
         <v>43218</v>
       </c>
       <c r="B622" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.2">
@@ -5446,7 +5446,7 @@
         <v>43219</v>
       </c>
       <c r="B623" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.2">
@@ -5455,7 +5455,7 @@
         <v>43220</v>
       </c>
       <c r="B624" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.2">
@@ -5464,7 +5464,7 @@
         <v>43221</v>
       </c>
       <c r="B625" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.2">
@@ -5473,7 +5473,7 @@
         <v>43222</v>
       </c>
       <c r="B626" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.2">
@@ -5481,7 +5481,7 @@
         <v>43581</v>
       </c>
       <c r="B627" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.2">
@@ -5490,7 +5490,7 @@
         <v>43582</v>
       </c>
       <c r="B628" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.2">
@@ -5499,7 +5499,7 @@
         <v>43583</v>
       </c>
       <c r="B629" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.2">
@@ -5508,7 +5508,7 @@
         <v>43584</v>
       </c>
       <c r="B630" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.2">
@@ -5517,7 +5517,7 @@
         <v>43585</v>
       </c>
       <c r="B631" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.2">
@@ -5526,7 +5526,7 @@
         <v>43586</v>
       </c>
       <c r="B632" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.2">
@@ -5535,7 +5535,7 @@
         <v>43587</v>
       </c>
       <c r="B633" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.2">
@@ -5543,7 +5543,7 @@
         <v>45046</v>
       </c>
       <c r="B634" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.2">
@@ -5551,7 +5551,7 @@
         <v>45047</v>
       </c>
       <c r="B635" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.2">
@@ -5559,7 +5559,7 @@
         <v>42180</v>
       </c>
       <c r="B636" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.2">
@@ -5567,7 +5567,7 @@
         <v>42181</v>
       </c>
       <c r="B637" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.2">
@@ -5575,7 +5575,7 @@
         <v>42182</v>
       </c>
       <c r="B638" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.2">
@@ -5583,7 +5583,7 @@
         <v>42183</v>
       </c>
       <c r="B639" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.2">
@@ -5591,7 +5591,7 @@
         <v>42184</v>
       </c>
       <c r="B640" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.2">
@@ -5599,7 +5599,7 @@
         <v>42185</v>
       </c>
       <c r="B641" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.2">
@@ -5607,7 +5607,7 @@
         <v>42186</v>
       </c>
       <c r="B642" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.2">
@@ -5615,7 +5615,7 @@
         <v>42187</v>
       </c>
       <c r="B643" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.2">
@@ -5623,7 +5623,7 @@
         <v>42188</v>
       </c>
       <c r="B644" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.2">
@@ -5631,7 +5631,7 @@
         <v>42189</v>
       </c>
       <c r="B645" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.2">
@@ -5639,7 +5639,7 @@
         <v>42190</v>
       </c>
       <c r="B646" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.2">
@@ -5647,7 +5647,7 @@
         <v>42191</v>
       </c>
       <c r="B647" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.2">
@@ -5655,7 +5655,7 @@
         <v>42192</v>
       </c>
       <c r="B648" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.2">
@@ -5663,7 +5663,7 @@
         <v>42193</v>
       </c>
       <c r="B649" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.2">
@@ -5671,7 +5671,7 @@
         <v>42194</v>
       </c>
       <c r="B650" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.2">
@@ -5679,7 +5679,7 @@
         <v>42195</v>
       </c>
       <c r="B651" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.2">
@@ -5687,7 +5687,7 @@
         <v>42196</v>
       </c>
       <c r="B652" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
@@ -5695,7 +5695,7 @@
         <v>42197</v>
       </c>
       <c r="B653" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.2">
@@ -5703,7 +5703,7 @@
         <v>42198</v>
       </c>
       <c r="B654" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
@@ -5711,7 +5711,7 @@
         <v>42199</v>
       </c>
       <c r="B655" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
@@ -5719,7 +5719,7 @@
         <v>42200</v>
       </c>
       <c r="B656" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
@@ -5727,7 +5727,7 @@
         <v>42201</v>
       </c>
       <c r="B657" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.2">
@@ -5735,7 +5735,7 @@
         <v>42202</v>
       </c>
       <c r="B658" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.2">
@@ -5743,7 +5743,7 @@
         <v>42203</v>
       </c>
       <c r="B659" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.2">
@@ -5751,7 +5751,7 @@
         <v>42204</v>
       </c>
       <c r="B660" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.2">
@@ -5759,7 +5759,7 @@
         <v>42205</v>
       </c>
       <c r="B661" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.2">
@@ -5767,7 +5767,7 @@
         <v>42206</v>
       </c>
       <c r="B662" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.2">
@@ -5775,7 +5775,7 @@
         <v>42207</v>
       </c>
       <c r="B663" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.2">
@@ -5783,7 +5783,7 @@
         <v>42208</v>
       </c>
       <c r="B664" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.2">
@@ -5791,7 +5791,7 @@
         <v>42209</v>
       </c>
       <c r="B665" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.2">
@@ -5799,7 +5799,7 @@
         <v>42210</v>
       </c>
       <c r="B666" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.2">
@@ -5807,7 +5807,7 @@
         <v>42211</v>
       </c>
       <c r="B667" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.2">
@@ -5815,7 +5815,7 @@
         <v>42212</v>
       </c>
       <c r="B668" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.2">
@@ -5823,7 +5823,7 @@
         <v>42213</v>
       </c>
       <c r="B669" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.2">
@@ -5831,7 +5831,7 @@
         <v>42214</v>
       </c>
       <c r="B670" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.2">
@@ -5839,7 +5839,7 @@
         <v>42215</v>
       </c>
       <c r="B671" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.2">
@@ -5847,7 +5847,7 @@
         <v>42216</v>
       </c>
       <c r="B672" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.2">
@@ -5855,7 +5855,7 @@
         <v>42217</v>
       </c>
       <c r="B673" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.2">
@@ -5863,7 +5863,7 @@
         <v>42218</v>
       </c>
       <c r="B674" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.2">
@@ -5871,7 +5871,7 @@
         <v>42219</v>
       </c>
       <c r="B675" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.2">
@@ -5879,7 +5879,7 @@
         <v>42220</v>
       </c>
       <c r="B676" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.2">
@@ -5887,7 +5887,7 @@
         <v>42221</v>
       </c>
       <c r="B677" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.2">
@@ -5895,7 +5895,7 @@
         <v>42222</v>
       </c>
       <c r="B678" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.2">
@@ -5903,7 +5903,7 @@
         <v>42223</v>
       </c>
       <c r="B679" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.2">
@@ -5911,7 +5911,7 @@
         <v>42224</v>
       </c>
       <c r="B680" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.2">
@@ -5919,7 +5919,7 @@
         <v>42225</v>
       </c>
       <c r="B681" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.2">
@@ -5927,7 +5927,7 @@
         <v>42546</v>
       </c>
       <c r="B682" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.2">
@@ -5935,7 +5935,7 @@
         <v>42547</v>
       </c>
       <c r="B683" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.2">
@@ -5943,7 +5943,7 @@
         <v>42548</v>
       </c>
       <c r="B684" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.2">
@@ -5951,7 +5951,7 @@
         <v>42549</v>
       </c>
       <c r="B685" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.2">
@@ -5959,7 +5959,7 @@
         <v>42550</v>
       </c>
       <c r="B686" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.2">
@@ -5967,7 +5967,7 @@
         <v>42551</v>
       </c>
       <c r="B687" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
@@ -5975,7 +5975,7 @@
         <v>42552</v>
       </c>
       <c r="B688" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.2">
@@ -5983,7 +5983,7 @@
         <v>42553</v>
       </c>
       <c r="B689" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.2">
@@ -5991,7 +5991,7 @@
         <v>42554</v>
       </c>
       <c r="B690" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.2">
@@ -5999,7 +5999,7 @@
         <v>42555</v>
       </c>
       <c r="B691" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.2">
@@ -6007,7 +6007,7 @@
         <v>42556</v>
       </c>
       <c r="B692" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.2">
@@ -6015,7 +6015,7 @@
         <v>42557</v>
       </c>
       <c r="B693" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.2">
@@ -6023,7 +6023,7 @@
         <v>42558</v>
       </c>
       <c r="B694" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.2">
@@ -6031,7 +6031,7 @@
         <v>42559</v>
       </c>
       <c r="B695" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.2">
@@ -6039,7 +6039,7 @@
         <v>42560</v>
       </c>
       <c r="B696" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.2">
@@ -6047,7 +6047,7 @@
         <v>42561</v>
       </c>
       <c r="B697" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.2">
@@ -6055,7 +6055,7 @@
         <v>42562</v>
       </c>
       <c r="B698" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.2">
@@ -6063,7 +6063,7 @@
         <v>42563</v>
       </c>
       <c r="B699" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.2">
@@ -6071,7 +6071,7 @@
         <v>42564</v>
       </c>
       <c r="B700" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.2">
@@ -6079,7 +6079,7 @@
         <v>42565</v>
       </c>
       <c r="B701" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.2">
@@ -6087,7 +6087,7 @@
         <v>42566</v>
       </c>
       <c r="B702" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.2">
@@ -6095,7 +6095,7 @@
         <v>42567</v>
       </c>
       <c r="B703" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.2">
@@ -6103,7 +6103,7 @@
         <v>42568</v>
       </c>
       <c r="B704" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.2">
@@ -6111,7 +6111,7 @@
         <v>42569</v>
       </c>
       <c r="B705" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.2">
@@ -6119,7 +6119,7 @@
         <v>42570</v>
       </c>
       <c r="B706" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.2">
@@ -6127,7 +6127,7 @@
         <v>42571</v>
       </c>
       <c r="B707" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.2">
@@ -6135,7 +6135,7 @@
         <v>42572</v>
       </c>
       <c r="B708" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.2">
@@ -6143,7 +6143,7 @@
         <v>42573</v>
       </c>
       <c r="B709" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
@@ -6151,7 +6151,7 @@
         <v>42574</v>
       </c>
       <c r="B710" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
@@ -6159,7 +6159,7 @@
         <v>42575</v>
       </c>
       <c r="B711" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
@@ -6167,7 +6167,7 @@
         <v>42576</v>
       </c>
       <c r="B712" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.2">
@@ -6175,7 +6175,7 @@
         <v>42577</v>
       </c>
       <c r="B713" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.2">
@@ -6183,7 +6183,7 @@
         <v>42578</v>
       </c>
       <c r="B714" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.2">
@@ -6191,7 +6191,7 @@
         <v>42579</v>
       </c>
       <c r="B715" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.2">
@@ -6199,7 +6199,7 @@
         <v>42580</v>
       </c>
       <c r="B716" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.2">
@@ -6207,7 +6207,7 @@
         <v>42581</v>
       </c>
       <c r="B717" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
@@ -6215,7 +6215,7 @@
         <v>42582</v>
       </c>
       <c r="B718" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.2">
@@ -6223,7 +6223,7 @@
         <v>42583</v>
       </c>
       <c r="B719" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
@@ -6231,7 +6231,7 @@
         <v>42584</v>
       </c>
       <c r="B720" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.2">
@@ -6239,7 +6239,7 @@
         <v>42585</v>
       </c>
       <c r="B721" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
@@ -6247,7 +6247,7 @@
         <v>42586</v>
       </c>
       <c r="B722" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">
@@ -6255,7 +6255,7 @@
         <v>42587</v>
       </c>
       <c r="B723" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.2">
@@ -6263,7 +6263,7 @@
         <v>42588</v>
       </c>
       <c r="B724" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.2">
@@ -6271,7 +6271,7 @@
         <v>42589</v>
       </c>
       <c r="B725" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.2">
@@ -6279,7 +6279,7 @@
         <v>42590</v>
       </c>
       <c r="B726" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.2">
@@ -6287,7 +6287,7 @@
         <v>42911</v>
       </c>
       <c r="B727" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.2">
@@ -6295,7 +6295,7 @@
         <v>42912</v>
       </c>
       <c r="B728" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
@@ -6303,7 +6303,7 @@
         <v>42913</v>
       </c>
       <c r="B729" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
@@ -6311,7 +6311,7 @@
         <v>42914</v>
       </c>
       <c r="B730" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
@@ -6319,7 +6319,7 @@
         <v>42915</v>
       </c>
       <c r="B731" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.2">
@@ -6327,7 +6327,7 @@
         <v>42916</v>
       </c>
       <c r="B732" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.2">
@@ -6335,7 +6335,7 @@
         <v>42917</v>
       </c>
       <c r="B733" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.2">
@@ -6343,7 +6343,7 @@
         <v>42918</v>
       </c>
       <c r="B734" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.2">
@@ -6351,7 +6351,7 @@
         <v>42919</v>
       </c>
       <c r="B735" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.2">
@@ -6359,7 +6359,7 @@
         <v>42920</v>
       </c>
       <c r="B736" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.2">
@@ -6367,7 +6367,7 @@
         <v>42921</v>
       </c>
       <c r="B737" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.2">
@@ -6375,7 +6375,7 @@
         <v>42922</v>
       </c>
       <c r="B738" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.2">
@@ -6383,7 +6383,7 @@
         <v>42923</v>
       </c>
       <c r="B739" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
@@ -6391,7 +6391,7 @@
         <v>42924</v>
       </c>
       <c r="B740" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
@@ -6399,7 +6399,7 @@
         <v>42925</v>
       </c>
       <c r="B741" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
@@ -6407,7 +6407,7 @@
         <v>42926</v>
       </c>
       <c r="B742" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
@@ -6415,7 +6415,7 @@
         <v>42927</v>
       </c>
       <c r="B743" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
@@ -6423,7 +6423,7 @@
         <v>42928</v>
       </c>
       <c r="B744" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
@@ -6431,7 +6431,7 @@
         <v>42929</v>
       </c>
       <c r="B745" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
@@ -6439,7 +6439,7 @@
         <v>42930</v>
       </c>
       <c r="B746" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.2">
@@ -6447,7 +6447,7 @@
         <v>42931</v>
       </c>
       <c r="B747" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.2">
@@ -6455,7 +6455,7 @@
         <v>42932</v>
       </c>
       <c r="B748" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.2">
@@ -6463,7 +6463,7 @@
         <v>42933</v>
       </c>
       <c r="B749" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.2">
@@ -6471,7 +6471,7 @@
         <v>42934</v>
       </c>
       <c r="B750" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.2">
@@ -6479,7 +6479,7 @@
         <v>42935</v>
       </c>
       <c r="B751" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.2">
@@ -6487,7 +6487,7 @@
         <v>42936</v>
       </c>
       <c r="B752" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.2">
@@ -6495,7 +6495,7 @@
         <v>42937</v>
       </c>
       <c r="B753" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.2">
@@ -6503,7 +6503,7 @@
         <v>42938</v>
       </c>
       <c r="B754" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.2">
@@ -6511,7 +6511,7 @@
         <v>42939</v>
       </c>
       <c r="B755" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.2">
@@ -6519,7 +6519,7 @@
         <v>42940</v>
       </c>
       <c r="B756" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.2">
@@ -6527,7 +6527,7 @@
         <v>42941</v>
       </c>
       <c r="B757" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.2">
@@ -6535,7 +6535,7 @@
         <v>42942</v>
       </c>
       <c r="B758" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.2">
@@ -6543,7 +6543,7 @@
         <v>42943</v>
       </c>
       <c r="B759" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.2">
@@ -6551,7 +6551,7 @@
         <v>42944</v>
       </c>
       <c r="B760" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.2">
@@ -6559,7 +6559,7 @@
         <v>42945</v>
       </c>
       <c r="B761" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.2">
@@ -6567,7 +6567,7 @@
         <v>42946</v>
       </c>
       <c r="B762" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.2">
@@ -6575,7 +6575,7 @@
         <v>43276</v>
       </c>
       <c r="B763" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.2">
@@ -6583,7 +6583,7 @@
         <v>43277</v>
       </c>
       <c r="B764" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.2">
@@ -6591,7 +6591,7 @@
         <v>43278</v>
       </c>
       <c r="B765" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.2">
@@ -6599,7 +6599,7 @@
         <v>43279</v>
       </c>
       <c r="B766" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.2">
@@ -6607,7 +6607,7 @@
         <v>43280</v>
       </c>
       <c r="B767" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.2">
@@ -6615,7 +6615,7 @@
         <v>43281</v>
       </c>
       <c r="B768" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.2">
@@ -6623,7 +6623,7 @@
         <v>43282</v>
       </c>
       <c r="B769" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.2">
@@ -6631,7 +6631,7 @@
         <v>43283</v>
       </c>
       <c r="B770" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.2">
@@ -6639,7 +6639,7 @@
         <v>43284</v>
       </c>
       <c r="B771" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.2">
@@ -6647,7 +6647,7 @@
         <v>43285</v>
       </c>
       <c r="B772" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.2">
@@ -6655,7 +6655,7 @@
         <v>43286</v>
       </c>
       <c r="B773" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.2">
@@ -6663,7 +6663,7 @@
         <v>43287</v>
       </c>
       <c r="B774" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.2">
@@ -6671,7 +6671,7 @@
         <v>43288</v>
       </c>
       <c r="B775" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.2">
@@ -6679,7 +6679,7 @@
         <v>43289</v>
       </c>
       <c r="B776" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.2">
@@ -6687,7 +6687,7 @@
         <v>43290</v>
       </c>
       <c r="B777" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.2">
@@ -6695,7 +6695,7 @@
         <v>43291</v>
       </c>
       <c r="B778" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.2">
@@ -6703,7 +6703,7 @@
         <v>43292</v>
       </c>
       <c r="B779" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.2">
@@ -6711,7 +6711,7 @@
         <v>43293</v>
       </c>
       <c r="B780" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.2">
@@ -6719,7 +6719,7 @@
         <v>43294</v>
       </c>
       <c r="B781" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.2">
@@ -6727,7 +6727,7 @@
         <v>43295</v>
       </c>
       <c r="B782" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.2">
@@ -6735,7 +6735,7 @@
         <v>43296</v>
       </c>
       <c r="B783" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.2">
@@ -6743,7 +6743,7 @@
         <v>43297</v>
       </c>
       <c r="B784" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.2">
@@ -6751,7 +6751,7 @@
         <v>43298</v>
       </c>
       <c r="B785" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.2">
@@ -6759,7 +6759,7 @@
         <v>43299</v>
       </c>
       <c r="B786" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.2">
@@ -6767,7 +6767,7 @@
         <v>43300</v>
       </c>
       <c r="B787" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.2">
@@ -6775,7 +6775,7 @@
         <v>43301</v>
       </c>
       <c r="B788" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.2">
@@ -6783,7 +6783,7 @@
         <v>43302</v>
       </c>
       <c r="B789" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.2">
@@ -6791,7 +6791,7 @@
         <v>43303</v>
       </c>
       <c r="B790" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.2">
@@ -6799,7 +6799,7 @@
         <v>43304</v>
       </c>
       <c r="B791" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.2">
@@ -6807,7 +6807,7 @@
         <v>43305</v>
       </c>
       <c r="B792" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.2">
@@ -6815,7 +6815,7 @@
         <v>43306</v>
       </c>
       <c r="B793" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.2">
@@ -6823,7 +6823,7 @@
         <v>43307</v>
       </c>
       <c r="B794" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.2">
@@ -6831,7 +6831,7 @@
         <v>43308</v>
       </c>
       <c r="B795" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.2">
@@ -6839,7 +6839,7 @@
         <v>43309</v>
       </c>
       <c r="B796" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.2">
@@ -6847,7 +6847,7 @@
         <v>43310</v>
       </c>
       <c r="B797" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.2">
@@ -6855,7 +6855,7 @@
         <v>43311</v>
       </c>
       <c r="B798" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.2">
@@ -6863,7 +6863,7 @@
         <v>43312</v>
       </c>
       <c r="B799" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.2">
@@ -6871,7 +6871,7 @@
         <v>43641</v>
       </c>
       <c r="B800" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.2">
@@ -6879,7 +6879,7 @@
         <v>43642</v>
       </c>
       <c r="B801" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.2">
@@ -6887,7 +6887,7 @@
         <v>43643</v>
       </c>
       <c r="B802" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.2">
@@ -6895,7 +6895,7 @@
         <v>43644</v>
       </c>
       <c r="B803" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.2">
@@ -6903,7 +6903,7 @@
         <v>43645</v>
       </c>
       <c r="B804" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.2">
@@ -6911,7 +6911,7 @@
         <v>43646</v>
       </c>
       <c r="B805" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.2">
@@ -6919,7 +6919,7 @@
         <v>43647</v>
       </c>
       <c r="B806" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
@@ -6927,7 +6927,7 @@
         <v>43648</v>
       </c>
       <c r="B807" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.2">
@@ -6935,7 +6935,7 @@
         <v>43649</v>
       </c>
       <c r="B808" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
@@ -6943,7 +6943,7 @@
         <v>43650</v>
       </c>
       <c r="B809" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.2">
@@ -6951,7 +6951,7 @@
         <v>43651</v>
       </c>
       <c r="B810" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.2">
@@ -6959,7 +6959,7 @@
         <v>43652</v>
       </c>
       <c r="B811" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.2">
@@ -6967,7 +6967,7 @@
         <v>43653</v>
       </c>
       <c r="B812" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.2">
@@ -6975,7 +6975,7 @@
         <v>43654</v>
       </c>
       <c r="B813" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.2">
@@ -6983,7 +6983,7 @@
         <v>43655</v>
       </c>
       <c r="B814" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.2">
@@ -6991,7 +6991,7 @@
         <v>43656</v>
       </c>
       <c r="B815" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.2">
@@ -6999,7 +6999,7 @@
         <v>43657</v>
       </c>
       <c r="B816" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.2">
@@ -7007,7 +7007,7 @@
         <v>43658</v>
       </c>
       <c r="B817" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.2">
@@ -7015,7 +7015,7 @@
         <v>43659</v>
       </c>
       <c r="B818" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.2">
@@ -7023,7 +7023,7 @@
         <v>43660</v>
       </c>
       <c r="B819" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.2">
@@ -7031,7 +7031,7 @@
         <v>43661</v>
       </c>
       <c r="B820" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.2">
@@ -7039,7 +7039,7 @@
         <v>43662</v>
       </c>
       <c r="B821" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.2">
@@ -7047,7 +7047,7 @@
         <v>43663</v>
       </c>
       <c r="B822" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.2">
@@ -7055,7 +7055,7 @@
         <v>43664</v>
       </c>
       <c r="B823" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
@@ -7063,7 +7063,7 @@
         <v>43665</v>
       </c>
       <c r="B824" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.2">
@@ -7071,7 +7071,7 @@
         <v>43666</v>
       </c>
       <c r="B825" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
@@ -7079,7 +7079,7 @@
         <v>43667</v>
       </c>
       <c r="B826" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.2">
@@ -7087,7 +7087,7 @@
         <v>43668</v>
       </c>
       <c r="B827" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.2">
@@ -7095,7 +7095,7 @@
         <v>43669</v>
       </c>
       <c r="B828" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.2">
@@ -7103,7 +7103,7 @@
         <v>43670</v>
       </c>
       <c r="B829" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.2">
@@ -7111,7 +7111,7 @@
         <v>43671</v>
       </c>
       <c r="B830" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.2">
@@ -7119,7 +7119,7 @@
         <v>43672</v>
       </c>
       <c r="B831" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
@@ -7127,7 +7127,7 @@
         <v>43673</v>
       </c>
       <c r="B832" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.2">
@@ -7135,7 +7135,7 @@
         <v>43674</v>
       </c>
       <c r="B833" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
@@ -7143,7 +7143,7 @@
         <v>43675</v>
       </c>
       <c r="B834" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
@@ -7151,7 +7151,7 @@
         <v>43676</v>
       </c>
       <c r="B835" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
@@ -7159,7 +7159,7 @@
         <v>44737</v>
       </c>
       <c r="B836" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.2">
@@ -7167,7 +7167,7 @@
         <v>44738</v>
       </c>
       <c r="B837" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.2">
@@ -7175,7 +7175,7 @@
         <v>44739</v>
       </c>
       <c r="B838" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.2">
@@ -7183,7 +7183,7 @@
         <v>44740</v>
       </c>
       <c r="B839" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
@@ -7191,7 +7191,7 @@
         <v>44741</v>
       </c>
       <c r="B840" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.2">
@@ -7199,7 +7199,7 @@
         <v>44742</v>
       </c>
       <c r="B841" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
@@ -7207,7 +7207,7 @@
         <v>44743</v>
       </c>
       <c r="B842" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.2">
@@ -7215,7 +7215,7 @@
         <v>44744</v>
       </c>
       <c r="B843" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.2">
@@ -7223,7 +7223,7 @@
         <v>44745</v>
       </c>
       <c r="B844" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.2">
@@ -7231,7 +7231,7 @@
         <v>44746</v>
       </c>
       <c r="B845" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
@@ -7239,7 +7239,7 @@
         <v>44747</v>
       </c>
       <c r="B846" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.2">
@@ -7247,7 +7247,7 @@
         <v>44748</v>
       </c>
       <c r="B847" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
@@ -7255,7 +7255,7 @@
         <v>44749</v>
       </c>
       <c r="B848" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
@@ -7263,7 +7263,7 @@
         <v>44750</v>
       </c>
       <c r="B849" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
@@ -7271,7 +7271,7 @@
         <v>44751</v>
       </c>
       <c r="B850" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
@@ -7279,7 +7279,7 @@
         <v>44752</v>
       </c>
       <c r="B851" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
@@ -7287,7 +7287,7 @@
         <v>44753</v>
       </c>
       <c r="B852" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
@@ -7295,7 +7295,7 @@
         <v>44754</v>
       </c>
       <c r="B853" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
@@ -7303,7 +7303,7 @@
         <v>44755</v>
       </c>
       <c r="B854" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
@@ -7311,7 +7311,7 @@
         <v>44756</v>
       </c>
       <c r="B855" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
@@ -7319,7 +7319,7 @@
         <v>44757</v>
       </c>
       <c r="B856" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
@@ -7327,7 +7327,7 @@
         <v>44758</v>
       </c>
       <c r="B857" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
@@ -7335,7 +7335,7 @@
         <v>44759</v>
       </c>
       <c r="B858" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
@@ -7343,7 +7343,7 @@
         <v>44760</v>
       </c>
       <c r="B859" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
@@ -7351,7 +7351,7 @@
         <v>44761</v>
       </c>
       <c r="B860" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
@@ -7359,7 +7359,7 @@
         <v>44762</v>
       </c>
       <c r="B861" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
@@ -7367,7 +7367,7 @@
         <v>44763</v>
       </c>
       <c r="B862" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
@@ -7375,7 +7375,7 @@
         <v>44764</v>
       </c>
       <c r="B863" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
@@ -7383,7 +7383,7 @@
         <v>44765</v>
       </c>
       <c r="B864" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
@@ -7391,7 +7391,7 @@
         <v>44766</v>
       </c>
       <c r="B865" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
@@ -7399,7 +7399,7 @@
         <v>44767</v>
       </c>
       <c r="B866" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
@@ -7407,7 +7407,7 @@
         <v>44768</v>
       </c>
       <c r="B867" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
@@ -7415,7 +7415,7 @@
         <v>44769</v>
       </c>
       <c r="B868" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
@@ -7423,7 +7423,7 @@
         <v>44770</v>
       </c>
       <c r="B869" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
@@ -7431,7 +7431,7 @@
         <v>44771</v>
       </c>
       <c r="B870" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
@@ -7439,7 +7439,7 @@
         <v>44772</v>
       </c>
       <c r="B871" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
@@ -7447,7 +7447,7 @@
         <v>44773</v>
       </c>
       <c r="B872" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
@@ -7455,7 +7455,7 @@
         <v>44677</v>
       </c>
       <c r="B873" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
@@ -7464,7 +7464,7 @@
         <v>44678</v>
       </c>
       <c r="B874" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
@@ -7473,7 +7473,7 @@
         <v>44679</v>
       </c>
       <c r="B875" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
@@ -7482,7 +7482,7 @@
         <v>44680</v>
       </c>
       <c r="B876" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
@@ -7491,7 +7491,7 @@
         <v>44681</v>
       </c>
       <c r="B877" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
@@ -7500,7 +7500,7 @@
         <v>44682</v>
       </c>
       <c r="B878" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
@@ -7509,7 +7509,7 @@
         <v>44683</v>
       </c>
       <c r="B879" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
@@ -7517,7 +7517,7 @@
         <v>44312</v>
       </c>
       <c r="B880" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
@@ -7526,7 +7526,7 @@
         <v>44313</v>
       </c>
       <c r="B881" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
@@ -7535,7 +7535,7 @@
         <v>44314</v>
       </c>
       <c r="B882" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
@@ -7544,7 +7544,7 @@
         <v>44315</v>
       </c>
       <c r="B883" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
@@ -7553,7 +7553,7 @@
         <v>44316</v>
       </c>
       <c r="B884" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
@@ -7562,7 +7562,7 @@
         <v>44317</v>
       </c>
       <c r="B885" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
@@ -7571,7 +7571,7 @@
         <v>44318</v>
       </c>
       <c r="B886" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
@@ -7579,7 +7579,7 @@
         <v>43947</v>
       </c>
       <c r="B887" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
@@ -7588,7 +7588,7 @@
         <v>43948</v>
       </c>
       <c r="B888" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
@@ -7597,7 +7597,7 @@
         <v>43949</v>
       </c>
       <c r="B889" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
@@ -7606,7 +7606,7 @@
         <v>43950</v>
       </c>
       <c r="B890" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
@@ -7615,7 +7615,7 @@
         <v>43951</v>
       </c>
       <c r="B891" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
@@ -7624,7 +7624,7 @@
         <v>43952</v>
       </c>
       <c r="B892" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
@@ -7633,7 +7633,7 @@
         <v>43953</v>
       </c>
       <c r="B893" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
@@ -7641,7 +7641,7 @@
         <v>44007</v>
       </c>
       <c r="B894" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
@@ -7649,7 +7649,7 @@
         <v>44008</v>
       </c>
       <c r="B895" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
@@ -7657,7 +7657,7 @@
         <v>44009</v>
       </c>
       <c r="B896" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
@@ -7665,7 +7665,7 @@
         <v>44010</v>
       </c>
       <c r="B897" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.2">
@@ -7673,7 +7673,7 @@
         <v>44011</v>
       </c>
       <c r="B898" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
@@ -7681,7 +7681,7 @@
         <v>44012</v>
       </c>
       <c r="B899" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
@@ -7689,7 +7689,7 @@
         <v>44013</v>
       </c>
       <c r="B900" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
@@ -7697,7 +7697,7 @@
         <v>44014</v>
       </c>
       <c r="B901" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
@@ -7705,7 +7705,7 @@
         <v>44015</v>
       </c>
       <c r="B902" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
@@ -7713,7 +7713,7 @@
         <v>44016</v>
       </c>
       <c r="B903" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
@@ -7721,7 +7721,7 @@
         <v>44017</v>
       </c>
       <c r="B904" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
@@ -7729,7 +7729,7 @@
         <v>44018</v>
       </c>
       <c r="B905" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
@@ -7737,7 +7737,7 @@
         <v>44019</v>
       </c>
       <c r="B906" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
@@ -7745,7 +7745,7 @@
         <v>44020</v>
       </c>
       <c r="B907" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
@@ -7753,7 +7753,7 @@
         <v>44021</v>
       </c>
       <c r="B908" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.2">
@@ -7761,7 +7761,7 @@
         <v>44022</v>
       </c>
       <c r="B909" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
@@ -7769,7 +7769,7 @@
         <v>44023</v>
       </c>
       <c r="B910" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
@@ -7777,7 +7777,7 @@
         <v>44024</v>
       </c>
       <c r="B911" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
@@ -7785,7 +7785,7 @@
         <v>44025</v>
       </c>
       <c r="B912" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
@@ -7793,7 +7793,7 @@
         <v>44026</v>
       </c>
       <c r="B913" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.2">
@@ -7801,7 +7801,7 @@
         <v>44027</v>
       </c>
       <c r="B914" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
@@ -7809,7 +7809,7 @@
         <v>44028</v>
       </c>
       <c r="B915" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
@@ -7817,7 +7817,7 @@
         <v>44029</v>
       </c>
       <c r="B916" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
@@ -7825,7 +7825,7 @@
         <v>44030</v>
       </c>
       <c r="B917" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
@@ -7833,7 +7833,7 @@
         <v>44031</v>
       </c>
       <c r="B918" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.2">
@@ -7841,7 +7841,7 @@
         <v>44032</v>
       </c>
       <c r="B919" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
@@ -7849,7 +7849,7 @@
         <v>44033</v>
       </c>
       <c r="B920" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
@@ -7857,7 +7857,7 @@
         <v>44034</v>
       </c>
       <c r="B921" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
@@ -7865,7 +7865,7 @@
         <v>44035</v>
       </c>
       <c r="B922" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
@@ -7873,7 +7873,7 @@
         <v>44036</v>
       </c>
       <c r="B923" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
@@ -7881,7 +7881,7 @@
         <v>44037</v>
       </c>
       <c r="B924" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
@@ -7889,7 +7889,7 @@
         <v>44038</v>
       </c>
       <c r="B925" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
@@ -7897,7 +7897,7 @@
         <v>44039</v>
       </c>
       <c r="B926" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
@@ -7905,7 +7905,7 @@
         <v>44040</v>
       </c>
       <c r="B927" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
@@ -7913,7 +7913,7 @@
         <v>44041</v>
       </c>
       <c r="B928" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
@@ -7921,7 +7921,7 @@
         <v>44042</v>
       </c>
       <c r="B929" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
@@ -7929,7 +7929,7 @@
         <v>44043</v>
       </c>
       <c r="B930" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
@@ -7937,7 +7937,7 @@
         <v>44372</v>
       </c>
       <c r="B931" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
@@ -7945,7 +7945,7 @@
         <v>44373</v>
       </c>
       <c r="B932" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
@@ -7953,7 +7953,7 @@
         <v>44374</v>
       </c>
       <c r="B933" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
@@ -7961,7 +7961,7 @@
         <v>44375</v>
       </c>
       <c r="B934" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
@@ -7969,7 +7969,7 @@
         <v>44376</v>
       </c>
       <c r="B935" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
@@ -7977,7 +7977,7 @@
         <v>44377</v>
       </c>
       <c r="B936" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
@@ -7985,7 +7985,7 @@
         <v>44378</v>
       </c>
       <c r="B937" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
@@ -7993,7 +7993,7 @@
         <v>44379</v>
       </c>
       <c r="B938" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
@@ -8001,7 +8001,7 @@
         <v>44380</v>
       </c>
       <c r="B939" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
@@ -8009,7 +8009,7 @@
         <v>44381</v>
       </c>
       <c r="B940" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
@@ -8017,7 +8017,7 @@
         <v>44382</v>
       </c>
       <c r="B941" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
@@ -8025,7 +8025,7 @@
         <v>44383</v>
       </c>
       <c r="B942" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
@@ -8033,7 +8033,7 @@
         <v>44384</v>
       </c>
       <c r="B943" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
@@ -8041,7 +8041,7 @@
         <v>44385</v>
       </c>
       <c r="B944" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
@@ -8049,7 +8049,7 @@
         <v>44386</v>
       </c>
       <c r="B945" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
@@ -8057,7 +8057,7 @@
         <v>44387</v>
       </c>
       <c r="B946" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
@@ -8065,7 +8065,7 @@
         <v>44388</v>
       </c>
       <c r="B947" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
@@ -8073,7 +8073,7 @@
         <v>44389</v>
       </c>
       <c r="B948" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
@@ -8081,7 +8081,7 @@
         <v>44390</v>
       </c>
       <c r="B949" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
@@ -8089,7 +8089,7 @@
         <v>44391</v>
       </c>
       <c r="B950" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
@@ -8097,7 +8097,7 @@
         <v>44392</v>
       </c>
       <c r="B951" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
@@ -8105,7 +8105,7 @@
         <v>44393</v>
       </c>
       <c r="B952" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
@@ -8113,7 +8113,7 @@
         <v>44394</v>
       </c>
       <c r="B953" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
@@ -8121,7 +8121,7 @@
         <v>44395</v>
       </c>
       <c r="B954" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
@@ -8129,7 +8129,7 @@
         <v>44396</v>
       </c>
       <c r="B955" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
@@ -8137,7 +8137,7 @@
         <v>44397</v>
       </c>
       <c r="B956" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
@@ -8145,7 +8145,7 @@
         <v>44398</v>
       </c>
       <c r="B957" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
@@ -8153,7 +8153,7 @@
         <v>44399</v>
       </c>
       <c r="B958" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
@@ -8161,7 +8161,7 @@
         <v>44400</v>
       </c>
       <c r="B959" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
@@ -8169,7 +8169,7 @@
         <v>44401</v>
       </c>
       <c r="B960" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
@@ -8177,7 +8177,7 @@
         <v>44402</v>
       </c>
       <c r="B961" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
@@ -8185,7 +8185,7 @@
         <v>44403</v>
       </c>
       <c r="B962" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
@@ -8193,7 +8193,7 @@
         <v>44404</v>
       </c>
       <c r="B963" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
@@ -8201,7 +8201,7 @@
         <v>44405</v>
       </c>
       <c r="B964" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
@@ -8209,7 +8209,7 @@
         <v>44406</v>
       </c>
       <c r="B965" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
@@ -8217,7 +8217,7 @@
         <v>44407</v>
       </c>
       <c r="B966" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
@@ -8225,7 +8225,7 @@
         <v>44408</v>
       </c>
       <c r="B967" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
@@ -8233,7 +8233,7 @@
         <v>43848</v>
       </c>
       <c r="B968" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
@@ -8241,7 +8241,7 @@
         <v>43849</v>
       </c>
       <c r="B969" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
@@ -8249,7 +8249,7 @@
         <v>43850</v>
       </c>
       <c r="B970" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
@@ -8257,7 +8257,7 @@
         <v>43851</v>
       </c>
       <c r="B971" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.2">
@@ -8265,7 +8265,7 @@
         <v>43852</v>
       </c>
       <c r="B972" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
@@ -8273,7 +8273,7 @@
         <v>43853</v>
       </c>
       <c r="B973" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
@@ -8281,7 +8281,7 @@
         <v>43855</v>
       </c>
       <c r="B974" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
@@ -8289,7 +8289,7 @@
         <v>43856</v>
       </c>
       <c r="B975" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
@@ -8297,7 +8297,7 @@
         <v>43857</v>
       </c>
       <c r="B976" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
@@ -8305,7 +8305,7 @@
         <v>43858</v>
       </c>
       <c r="B977" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
@@ -8313,7 +8313,7 @@
         <v>43859</v>
       </c>
       <c r="B978" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
@@ -8321,7 +8321,7 @@
         <v>43860</v>
       </c>
       <c r="B979" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
@@ -8329,7 +8329,7 @@
         <v>43861</v>
       </c>
       <c r="B980" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
@@ -8337,7 +8337,7 @@
         <v>43862</v>
       </c>
       <c r="B981" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
@@ -8345,7 +8345,7 @@
         <v>43863</v>
       </c>
       <c r="B982" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
@@ -8353,7 +8353,7 @@
         <v>43864</v>
       </c>
       <c r="B983" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
@@ -8361,7 +8361,7 @@
         <v>44232</v>
       </c>
       <c r="B984" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
@@ -8369,7 +8369,7 @@
         <v>44233</v>
       </c>
       <c r="B985" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
@@ -8377,7 +8377,7 @@
         <v>44234</v>
       </c>
       <c r="B986" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
@@ -8385,7 +8385,7 @@
         <v>44235</v>
       </c>
       <c r="B987" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
@@ -8393,7 +8393,7 @@
         <v>44236</v>
       </c>
       <c r="B988" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
@@ -8401,7 +8401,7 @@
         <v>44237</v>
       </c>
       <c r="B989" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
@@ -8409,7 +8409,7 @@
         <v>44239</v>
       </c>
       <c r="B990" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
@@ -8417,7 +8417,7 @@
         <v>44240</v>
       </c>
       <c r="B991" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
@@ -8425,7 +8425,7 @@
         <v>44241</v>
       </c>
       <c r="B992" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
@@ -8433,7 +8433,7 @@
         <v>44242</v>
       </c>
       <c r="B993" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
@@ -8441,7 +8441,7 @@
         <v>44243</v>
       </c>
       <c r="B994" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
@@ -8449,7 +8449,7 @@
         <v>44244</v>
       </c>
       <c r="B995" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
@@ -8457,7 +8457,7 @@
         <v>44245</v>
       </c>
       <c r="B996" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
@@ -8465,7 +8465,7 @@
         <v>44246</v>
       </c>
       <c r="B997" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
@@ -8473,7 +8473,7 @@
         <v>44247</v>
       </c>
       <c r="B998" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
@@ -8481,7 +8481,7 @@
         <v>44248</v>
       </c>
       <c r="B999" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add capacity as lagged regressors
</commit_message>
<xml_diff>
--- a/holidays.xlsx
+++ b/holidays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namtrantuan\Desktop\passenger_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C4ECAD-CAF9-42D0-9600-B3FF316BD9D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EEDCFB-0462-415E-9283-A5E485E69197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C81195CF-3238-4C84-B228-279AE06B6B57}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="covid" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">covid!$A$1:$B$999</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">covid!$A$1:$B$1000</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="9">
   <si>
     <t>covid_1</t>
   </si>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9708BE-FF7E-456D-97C7-E4E782A5149C}">
-  <dimension ref="A1:B999"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484" s="1">
-        <v>44948</v>
+        <v>44947</v>
       </c>
       <c r="B484" t="s">
         <v>5</v>
@@ -4293,7 +4293,7 @@
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A485" s="1">
-        <v>44949</v>
+        <v>44948</v>
       </c>
       <c r="B485" t="s">
         <v>5</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A486" s="1">
-        <v>44950</v>
+        <v>44949</v>
       </c>
       <c r="B486" t="s">
         <v>5</v>
@@ -4309,7 +4309,7 @@
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A487" s="1">
-        <v>44951</v>
+        <v>44950</v>
       </c>
       <c r="B487" t="s">
         <v>5</v>
@@ -4317,7 +4317,7 @@
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A488" s="1">
-        <v>44952</v>
+        <v>44951</v>
       </c>
       <c r="B488" t="s">
         <v>5</v>
@@ -4325,7 +4325,7 @@
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A489" s="1">
-        <v>44953</v>
+        <v>44952</v>
       </c>
       <c r="B489" t="s">
         <v>5</v>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A490" s="1">
-        <v>44954</v>
+        <v>44953</v>
       </c>
       <c r="B490" t="s">
         <v>5</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A491" s="1">
-        <v>44955</v>
+        <v>44954</v>
       </c>
       <c r="B491" t="s">
         <v>5</v>
@@ -4349,7 +4349,7 @@
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A492" s="1">
-        <v>44956</v>
+        <v>44955</v>
       </c>
       <c r="B492" t="s">
         <v>5</v>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A493" s="1">
-        <v>44957</v>
+        <v>44956</v>
       </c>
       <c r="B493" t="s">
         <v>5</v>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A494" s="1">
-        <v>44587</v>
+        <v>44957</v>
       </c>
       <c r="B494" t="s">
         <v>5</v>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A495" s="1">
-        <v>44588</v>
+        <v>44587</v>
       </c>
       <c r="B495" t="s">
         <v>5</v>
@@ -4381,7 +4381,7 @@
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A496" s="1">
-        <v>44589</v>
+        <v>44588</v>
       </c>
       <c r="B496" t="s">
         <v>5</v>
@@ -4389,7 +4389,7 @@
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A497" s="1">
-        <v>44590</v>
+        <v>44589</v>
       </c>
       <c r="B497" t="s">
         <v>5</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A498" s="1">
-        <v>44591</v>
+        <v>44590</v>
       </c>
       <c r="B498" t="s">
         <v>5</v>
@@ -4405,7 +4405,7 @@
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A499" s="1">
-        <v>44593</v>
+        <v>44591</v>
       </c>
       <c r="B499" t="s">
         <v>5</v>
@@ -4413,7 +4413,7 @@
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A500" s="1">
-        <v>44594</v>
+        <v>44593</v>
       </c>
       <c r="B500" t="s">
         <v>5</v>
@@ -4421,7 +4421,7 @@
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A501" s="1">
-        <v>44595</v>
+        <v>44594</v>
       </c>
       <c r="B501" t="s">
         <v>5</v>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A502" s="1">
-        <v>44596</v>
+        <v>44595</v>
       </c>
       <c r="B502" t="s">
         <v>5</v>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A503" s="1">
-        <v>44597</v>
+        <v>44596</v>
       </c>
       <c r="B503" t="s">
         <v>5</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A504" s="1">
-        <v>44598</v>
+        <v>44597</v>
       </c>
       <c r="B504" t="s">
         <v>5</v>
@@ -4453,7 +4453,7 @@
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A505" s="1">
-        <v>44599</v>
+        <v>44598</v>
       </c>
       <c r="B505" t="s">
         <v>5</v>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A506" s="1">
-        <v>44600</v>
+        <v>44599</v>
       </c>
       <c r="B506" t="s">
         <v>5</v>
@@ -4469,7 +4469,7 @@
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A507" s="1">
-        <v>44601</v>
+        <v>44600</v>
       </c>
       <c r="B507" t="s">
         <v>5</v>
@@ -4477,7 +4477,7 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A508" s="1">
-        <v>44602</v>
+        <v>44601</v>
       </c>
       <c r="B508" t="s">
         <v>5</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A509" s="1">
-        <v>42047</v>
+        <v>44602</v>
       </c>
       <c r="B509" t="s">
         <v>5</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" s="1">
-        <v>42048</v>
+        <v>42047</v>
       </c>
       <c r="B510" t="s">
         <v>5</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" s="1">
-        <v>42049</v>
+        <v>42048</v>
       </c>
       <c r="B511" t="s">
         <v>5</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A512" s="1">
-        <v>42050</v>
+        <v>42049</v>
       </c>
       <c r="B512" t="s">
         <v>5</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A513" s="1">
-        <v>42051</v>
+        <v>42050</v>
       </c>
       <c r="B513" t="s">
         <v>5</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A514" s="1">
-        <v>42052</v>
+        <v>42051</v>
       </c>
       <c r="B514" t="s">
         <v>5</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A515" s="1">
-        <v>42055</v>
+        <v>42052</v>
       </c>
       <c r="B515" t="s">
         <v>5</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A516" s="1">
-        <v>42056</v>
+        <v>42055</v>
       </c>
       <c r="B516" t="s">
         <v>5</v>
@@ -4549,7 +4549,7 @@
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A517" s="1">
-        <v>42057</v>
+        <v>42056</v>
       </c>
       <c r="B517" t="s">
         <v>5</v>
@@ -4557,7 +4557,7 @@
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A518" s="1">
-        <v>42058</v>
+        <v>42057</v>
       </c>
       <c r="B518" t="s">
         <v>5</v>
@@ -4565,7 +4565,7 @@
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A519" s="1">
-        <v>42059</v>
+        <v>42058</v>
       </c>
       <c r="B519" t="s">
         <v>5</v>
@@ -4573,7 +4573,7 @@
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A520" s="1">
-        <v>42060</v>
+        <v>42059</v>
       </c>
       <c r="B520" t="s">
         <v>5</v>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A521" s="1">
-        <v>42061</v>
+        <v>42060</v>
       </c>
       <c r="B521" t="s">
         <v>5</v>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A522" s="1">
-        <v>42062</v>
+        <v>42061</v>
       </c>
       <c r="B522" t="s">
         <v>5</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A523" s="1">
-        <v>42063</v>
+        <v>42062</v>
       </c>
       <c r="B523" t="s">
         <v>5</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A524" s="1">
-        <v>42064</v>
+        <v>42063</v>
       </c>
       <c r="B524" t="s">
         <v>5</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A525" s="1">
-        <v>42065</v>
+        <v>42064</v>
       </c>
       <c r="B525" t="s">
         <v>5</v>
@@ -4621,7 +4621,7 @@
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A526" s="1">
-        <v>42402</v>
+        <v>42065</v>
       </c>
       <c r="B526" t="s">
         <v>5</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A527" s="1">
-        <v>42403</v>
+        <v>42402</v>
       </c>
       <c r="B527" t="s">
         <v>5</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A528" s="1">
-        <v>42404</v>
+        <v>42403</v>
       </c>
       <c r="B528" t="s">
         <v>5</v>
@@ -4645,7 +4645,7 @@
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A529" s="1">
-        <v>42405</v>
+        <v>42404</v>
       </c>
       <c r="B529" t="s">
         <v>5</v>
@@ -4653,7 +4653,7 @@
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A530" s="1">
-        <v>42406</v>
+        <v>42405</v>
       </c>
       <c r="B530" t="s">
         <v>5</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A531" s="1">
-        <v>42409</v>
+        <v>42406</v>
       </c>
       <c r="B531" t="s">
         <v>5</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A532" s="1">
-        <v>42410</v>
+        <v>42409</v>
       </c>
       <c r="B532" t="s">
         <v>5</v>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A533" s="1">
-        <v>42411</v>
+        <v>42410</v>
       </c>
       <c r="B533" t="s">
         <v>5</v>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A534" s="1">
-        <v>42412</v>
+        <v>42411</v>
       </c>
       <c r="B534" t="s">
         <v>5</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A535" s="1">
-        <v>42413</v>
+        <v>42412</v>
       </c>
       <c r="B535" t="s">
         <v>5</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A536" s="1">
-        <v>42414</v>
+        <v>42413</v>
       </c>
       <c r="B536" t="s">
         <v>5</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A537" s="1">
-        <v>42415</v>
+        <v>42414</v>
       </c>
       <c r="B537" t="s">
         <v>5</v>
@@ -4717,7 +4717,7 @@
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A538" s="1">
-        <v>42416</v>
+        <v>42415</v>
       </c>
       <c r="B538" t="s">
         <v>5</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A539" s="1">
-        <v>42756</v>
+        <v>42416</v>
       </c>
       <c r="B539" t="s">
         <v>5</v>
@@ -4733,7 +4733,7 @@
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A540" s="1">
-        <v>42757</v>
+        <v>42756</v>
       </c>
       <c r="B540" t="s">
         <v>5</v>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A541" s="1">
-        <v>42758</v>
+        <v>42757</v>
       </c>
       <c r="B541" t="s">
         <v>5</v>
@@ -4749,7 +4749,7 @@
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A542" s="1">
-        <v>42759</v>
+        <v>42758</v>
       </c>
       <c r="B542" t="s">
         <v>5</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A543" s="1">
-        <v>42760</v>
+        <v>42759</v>
       </c>
       <c r="B543" t="s">
         <v>5</v>
@@ -4765,7 +4765,7 @@
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A544" s="1">
-        <v>42761</v>
+        <v>42760</v>
       </c>
       <c r="B544" t="s">
         <v>5</v>
@@ -4773,7 +4773,7 @@
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A545" s="1">
-        <v>42764</v>
+        <v>42761</v>
       </c>
       <c r="B545" t="s">
         <v>5</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A546" s="1">
-        <v>42765</v>
+        <v>42764</v>
       </c>
       <c r="B546" t="s">
         <v>5</v>
@@ -4789,7 +4789,7 @@
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A547" s="1">
-        <v>42766</v>
+        <v>42765</v>
       </c>
       <c r="B547" t="s">
         <v>5</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A548" s="1">
-        <v>42767</v>
+        <v>42766</v>
       </c>
       <c r="B548" t="s">
         <v>5</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A549" s="1">
-        <v>42768</v>
+        <v>42767</v>
       </c>
       <c r="B549" t="s">
         <v>5</v>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A550" s="1">
-        <v>42769</v>
+        <v>42768</v>
       </c>
       <c r="B550" t="s">
         <v>5</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A551" s="1">
-        <v>42770</v>
+        <v>42769</v>
       </c>
       <c r="B551" t="s">
         <v>5</v>
@@ -4829,7 +4829,7 @@
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A552" s="1">
-        <v>42771</v>
+        <v>42770</v>
       </c>
       <c r="B552" t="s">
         <v>5</v>
@@ -4837,7 +4837,7 @@
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A553" s="1">
-        <v>42772</v>
+        <v>42771</v>
       </c>
       <c r="B553" t="s">
         <v>5</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A554" s="1">
-        <v>43140</v>
+        <v>42772</v>
       </c>
       <c r="B554" t="s">
         <v>5</v>
@@ -4853,8 +4853,7 @@
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A555" s="1">
-        <f>A554+1</f>
-        <v>43141</v>
+        <v>43140</v>
       </c>
       <c r="B555" t="s">
         <v>5</v>
@@ -4862,8 +4861,8 @@
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A556" s="1">
-        <f t="shared" ref="A556:A571" si="0">A555+1</f>
-        <v>43142</v>
+        <f>A555+1</f>
+        <v>43141</v>
       </c>
       <c r="B556" t="s">
         <v>5</v>
@@ -4871,8 +4870,8 @@
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A557" s="1">
-        <f t="shared" si="0"/>
-        <v>43143</v>
+        <f t="shared" ref="A557:A572" si="0">A556+1</f>
+        <v>43142</v>
       </c>
       <c r="B557" t="s">
         <v>5</v>
@@ -4881,7 +4880,7 @@
     <row r="558" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A558" s="1">
         <f t="shared" si="0"/>
-        <v>43144</v>
+        <v>43143</v>
       </c>
       <c r="B558" t="s">
         <v>5</v>
@@ -4890,7 +4889,7 @@
     <row r="559" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A559" s="1">
         <f t="shared" si="0"/>
-        <v>43145</v>
+        <v>43144</v>
       </c>
       <c r="B559" t="s">
         <v>5</v>
@@ -4898,7 +4897,8 @@
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A560" s="1">
-        <v>43148</v>
+        <f t="shared" si="0"/>
+        <v>43145</v>
       </c>
       <c r="B560" t="s">
         <v>5</v>
@@ -4906,8 +4906,7 @@
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A561" s="1">
-        <f t="shared" si="0"/>
-        <v>43149</v>
+        <v>43148</v>
       </c>
       <c r="B561" t="s">
         <v>5</v>
@@ -4916,7 +4915,7 @@
     <row r="562" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A562" s="1">
         <f t="shared" si="0"/>
-        <v>43150</v>
+        <v>43149</v>
       </c>
       <c r="B562" t="s">
         <v>5</v>
@@ -4925,7 +4924,7 @@
     <row r="563" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A563" s="1">
         <f t="shared" si="0"/>
-        <v>43151</v>
+        <v>43150</v>
       </c>
       <c r="B563" t="s">
         <v>5</v>
@@ -4934,7 +4933,7 @@
     <row r="564" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A564" s="1">
         <f t="shared" si="0"/>
-        <v>43152</v>
+        <v>43151</v>
       </c>
       <c r="B564" t="s">
         <v>5</v>
@@ -4943,7 +4942,7 @@
     <row r="565" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A565" s="1">
         <f t="shared" si="0"/>
-        <v>43153</v>
+        <v>43152</v>
       </c>
       <c r="B565" t="s">
         <v>5</v>
@@ -4952,7 +4951,7 @@
     <row r="566" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A566" s="1">
         <f t="shared" si="0"/>
-        <v>43154</v>
+        <v>43153</v>
       </c>
       <c r="B566" t="s">
         <v>5</v>
@@ -4961,7 +4960,7 @@
     <row r="567" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A567" s="1">
         <f t="shared" si="0"/>
-        <v>43155</v>
+        <v>43154</v>
       </c>
       <c r="B567" t="s">
         <v>5</v>
@@ -4970,7 +4969,7 @@
     <row r="568" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A568" s="1">
         <f t="shared" si="0"/>
-        <v>43156</v>
+        <v>43155</v>
       </c>
       <c r="B568" t="s">
         <v>5</v>
@@ -4979,7 +4978,7 @@
     <row r="569" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A569" s="1">
         <f t="shared" si="0"/>
-        <v>43157</v>
+        <v>43156</v>
       </c>
       <c r="B569" t="s">
         <v>5</v>
@@ -4988,7 +4987,7 @@
     <row r="570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A570" s="1">
         <f t="shared" si="0"/>
-        <v>43158</v>
+        <v>43157</v>
       </c>
       <c r="B570" t="s">
         <v>5</v>
@@ -4997,7 +4996,7 @@
     <row r="571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A571" s="1">
         <f t="shared" si="0"/>
-        <v>43159</v>
+        <v>43158</v>
       </c>
       <c r="B571" t="s">
         <v>5</v>
@@ -5005,7 +5004,8 @@
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A572" s="1">
-        <v>43494</v>
+        <f t="shared" si="0"/>
+        <v>43159</v>
       </c>
       <c r="B572" t="s">
         <v>5</v>
@@ -5013,7 +5013,7 @@
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A573" s="1">
-        <v>43495</v>
+        <v>43494</v>
       </c>
       <c r="B573" t="s">
         <v>5</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A574" s="1">
-        <v>43496</v>
+        <v>43495</v>
       </c>
       <c r="B574" t="s">
         <v>5</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A575" s="1">
-        <v>43497</v>
+        <v>43496</v>
       </c>
       <c r="B575" t="s">
         <v>5</v>
@@ -5037,7 +5037,7 @@
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A576" s="1">
-        <v>43498</v>
+        <v>43497</v>
       </c>
       <c r="B576" t="s">
         <v>5</v>
@@ -5045,7 +5045,7 @@
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A577" s="1">
-        <v>43499</v>
+        <v>43498</v>
       </c>
       <c r="B577" t="s">
         <v>5</v>
@@ -5053,7 +5053,7 @@
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A578" s="1">
-        <v>43500</v>
+        <v>43499</v>
       </c>
       <c r="B578" t="s">
         <v>5</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A579" s="1">
-        <v>43502</v>
+        <v>43500</v>
       </c>
       <c r="B579" t="s">
         <v>5</v>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A580" s="1">
-        <v>43503</v>
+        <v>43502</v>
       </c>
       <c r="B580" t="s">
         <v>5</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A581" s="1">
-        <v>43504</v>
+        <v>43503</v>
       </c>
       <c r="B581" t="s">
         <v>5</v>
@@ -5085,7 +5085,7 @@
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A582" s="1">
-        <v>43505</v>
+        <v>43504</v>
       </c>
       <c r="B582" t="s">
         <v>5</v>
@@ -5093,7 +5093,7 @@
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A583" s="1">
-        <v>43506</v>
+        <v>43505</v>
       </c>
       <c r="B583" t="s">
         <v>5</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A584" s="1">
-        <v>43507</v>
+        <v>43506</v>
       </c>
       <c r="B584" t="s">
         <v>5</v>
@@ -5109,7 +5109,7 @@
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A585" s="1">
-        <v>43508</v>
+        <v>43507</v>
       </c>
       <c r="B585" t="s">
         <v>5</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A586" s="1">
-        <v>43509</v>
+        <v>43508</v>
       </c>
       <c r="B586" t="s">
         <v>5</v>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A587" s="1">
-        <v>43510</v>
+        <v>43509</v>
       </c>
       <c r="B587" t="s">
         <v>5</v>
@@ -5133,7 +5133,7 @@
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A588" s="1">
-        <v>43511</v>
+        <v>43510</v>
       </c>
       <c r="B588" t="s">
         <v>5</v>
@@ -5141,7 +5141,7 @@
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A589" s="1">
-        <v>43512</v>
+        <v>43511</v>
       </c>
       <c r="B589" t="s">
         <v>5</v>
@@ -5149,17 +5149,16 @@
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A590" s="1">
-        <f t="shared" ref="A590:A594" si="1">A591-1</f>
-        <v>42118</v>
+        <v>43512</v>
       </c>
       <c r="B590" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A591" s="1">
-        <f t="shared" si="1"/>
-        <v>42119</v>
+        <f t="shared" ref="A591:A595" si="1">A592-1</f>
+        <v>42118</v>
       </c>
       <c r="B591" t="s">
         <v>6</v>
@@ -5168,7 +5167,7 @@
     <row r="592" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A592" s="1">
         <f t="shared" si="1"/>
-        <v>42120</v>
+        <v>42119</v>
       </c>
       <c r="B592" t="s">
         <v>6</v>
@@ -5177,7 +5176,7 @@
     <row r="593" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A593" s="1">
         <f t="shared" si="1"/>
-        <v>42121</v>
+        <v>42120</v>
       </c>
       <c r="B593" t="s">
         <v>6</v>
@@ -5186,7 +5185,7 @@
     <row r="594" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A594" s="1">
         <f t="shared" si="1"/>
-        <v>42122</v>
+        <v>42121</v>
       </c>
       <c r="B594" t="s">
         <v>6</v>
@@ -5194,8 +5193,8 @@
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A595" s="1">
-        <f>A596-1</f>
-        <v>42123</v>
+        <f t="shared" si="1"/>
+        <v>42122</v>
       </c>
       <c r="B595" t="s">
         <v>6</v>
@@ -5203,7 +5202,8 @@
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A596" s="1">
-        <v>42124</v>
+        <f>A597-1</f>
+        <v>42123</v>
       </c>
       <c r="B596" t="s">
         <v>6</v>
@@ -5211,8 +5211,7 @@
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A597" s="1">
-        <f>A596+1</f>
-        <v>42125</v>
+        <v>42124</v>
       </c>
       <c r="B597" t="s">
         <v>6</v>
@@ -5220,8 +5219,8 @@
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A598" s="1">
-        <f t="shared" ref="A598:A600" si="2">A597+1</f>
-        <v>42126</v>
+        <f>A597+1</f>
+        <v>42125</v>
       </c>
       <c r="B598" t="s">
         <v>6</v>
@@ -5229,8 +5228,8 @@
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A599" s="1">
-        <f t="shared" si="2"/>
-        <v>42127</v>
+        <f t="shared" ref="A599:A601" si="2">A598+1</f>
+        <v>42126</v>
       </c>
       <c r="B599" t="s">
         <v>6</v>
@@ -5239,7 +5238,7 @@
     <row r="600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A600" s="1">
         <f t="shared" si="2"/>
-        <v>42128</v>
+        <v>42127</v>
       </c>
       <c r="B600" t="s">
         <v>6</v>
@@ -5247,8 +5246,8 @@
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" s="1">
-        <f t="shared" ref="A601:A609" si="3">A602-1</f>
-        <v>42484</v>
+        <f t="shared" si="2"/>
+        <v>42128</v>
       </c>
       <c r="B601" t="s">
         <v>6</v>
@@ -5256,8 +5255,8 @@
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A602" s="1">
-        <f t="shared" si="3"/>
-        <v>42485</v>
+        <f t="shared" ref="A602:A610" si="3">A603-1</f>
+        <v>42484</v>
       </c>
       <c r="B602" t="s">
         <v>6</v>
@@ -5266,7 +5265,7 @@
     <row r="603" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A603" s="1">
         <f t="shared" si="3"/>
-        <v>42486</v>
+        <v>42485</v>
       </c>
       <c r="B603" t="s">
         <v>6</v>
@@ -5275,7 +5274,7 @@
     <row r="604" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A604" s="1">
         <f t="shared" si="3"/>
-        <v>42487</v>
+        <v>42486</v>
       </c>
       <c r="B604" t="s">
         <v>6</v>
@@ -5284,7 +5283,7 @@
     <row r="605" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A605" s="1">
         <f t="shared" si="3"/>
-        <v>42488</v>
+        <v>42487</v>
       </c>
       <c r="B605" t="s">
         <v>6</v>
@@ -5293,7 +5292,7 @@
     <row r="606" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A606" s="1">
         <f t="shared" si="3"/>
-        <v>42489</v>
+        <v>42488</v>
       </c>
       <c r="B606" t="s">
         <v>6</v>
@@ -5302,7 +5301,7 @@
     <row r="607" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A607" s="1">
         <f t="shared" si="3"/>
-        <v>42490</v>
+        <v>42489</v>
       </c>
       <c r="B607" t="s">
         <v>6</v>
@@ -5311,7 +5310,7 @@
     <row r="608" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A608" s="1">
         <f t="shared" si="3"/>
-        <v>42491</v>
+        <v>42490</v>
       </c>
       <c r="B608" t="s">
         <v>6</v>
@@ -5320,7 +5319,7 @@
     <row r="609" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A609" s="1">
         <f t="shared" si="3"/>
-        <v>42492</v>
+        <v>42491</v>
       </c>
       <c r="B609" t="s">
         <v>6</v>
@@ -5328,8 +5327,8 @@
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A610" s="1">
-        <f>A611-1</f>
-        <v>42493</v>
+        <f t="shared" si="3"/>
+        <v>42492</v>
       </c>
       <c r="B610" t="s">
         <v>6</v>
@@ -5337,7 +5336,8 @@
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A611" s="1">
-        <v>42494</v>
+        <f>A612-1</f>
+        <v>42493</v>
       </c>
       <c r="B611" t="s">
         <v>6</v>
@@ -5345,8 +5345,7 @@
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A612" s="1">
-        <f t="shared" ref="A612:A618" si="4">A613-1</f>
-        <v>42851</v>
+        <v>42494</v>
       </c>
       <c r="B612" t="s">
         <v>6</v>
@@ -5354,8 +5353,8 @@
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A613" s="1">
-        <f t="shared" si="4"/>
-        <v>42852</v>
+        <f t="shared" ref="A613:A619" si="4">A614-1</f>
+        <v>42851</v>
       </c>
       <c r="B613" t="s">
         <v>6</v>
@@ -5364,7 +5363,7 @@
     <row r="614" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A614" s="1">
         <f t="shared" si="4"/>
-        <v>42853</v>
+        <v>42852</v>
       </c>
       <c r="B614" t="s">
         <v>6</v>
@@ -5373,7 +5372,7 @@
     <row r="615" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A615" s="1">
         <f t="shared" si="4"/>
-        <v>42854</v>
+        <v>42853</v>
       </c>
       <c r="B615" t="s">
         <v>6</v>
@@ -5382,7 +5381,7 @@
     <row r="616" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A616" s="1">
         <f t="shared" si="4"/>
-        <v>42855</v>
+        <v>42854</v>
       </c>
       <c r="B616" t="s">
         <v>6</v>
@@ -5391,7 +5390,7 @@
     <row r="617" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A617" s="1">
         <f t="shared" si="4"/>
-        <v>42856</v>
+        <v>42855</v>
       </c>
       <c r="B617" t="s">
         <v>6</v>
@@ -5400,7 +5399,7 @@
     <row r="618" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A618" s="1">
         <f t="shared" si="4"/>
-        <v>42857</v>
+        <v>42856</v>
       </c>
       <c r="B618" t="s">
         <v>6</v>
@@ -5408,8 +5407,8 @@
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A619" s="1">
-        <f>A620-1</f>
-        <v>42858</v>
+        <f t="shared" si="4"/>
+        <v>42857</v>
       </c>
       <c r="B619" t="s">
         <v>6</v>
@@ -5417,7 +5416,8 @@
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A620" s="1">
-        <v>42859</v>
+        <f>A621-1</f>
+        <v>42858</v>
       </c>
       <c r="B620" t="s">
         <v>6</v>
@@ -5425,7 +5425,7 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A621" s="1">
-        <v>43217</v>
+        <v>42859</v>
       </c>
       <c r="B621" t="s">
         <v>6</v>
@@ -5433,8 +5433,7 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A622" s="1">
-        <f>A621+1</f>
-        <v>43218</v>
+        <v>43217</v>
       </c>
       <c r="B622" t="s">
         <v>6</v>
@@ -5442,8 +5441,8 @@
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A623" s="1">
-        <f t="shared" ref="A623:A626" si="5">A622+1</f>
-        <v>43219</v>
+        <f>A622+1</f>
+        <v>43218</v>
       </c>
       <c r="B623" t="s">
         <v>6</v>
@@ -5451,8 +5450,8 @@
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A624" s="1">
-        <f t="shared" si="5"/>
-        <v>43220</v>
+        <f t="shared" ref="A624:A627" si="5">A623+1</f>
+        <v>43219</v>
       </c>
       <c r="B624" t="s">
         <v>6</v>
@@ -5461,7 +5460,7 @@
     <row r="625" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A625" s="1">
         <f t="shared" si="5"/>
-        <v>43221</v>
+        <v>43220</v>
       </c>
       <c r="B625" t="s">
         <v>6</v>
@@ -5470,7 +5469,7 @@
     <row r="626" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A626" s="1">
         <f t="shared" si="5"/>
-        <v>43222</v>
+        <v>43221</v>
       </c>
       <c r="B626" t="s">
         <v>6</v>
@@ -5478,7 +5477,8 @@
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A627" s="1">
-        <v>43581</v>
+        <f t="shared" si="5"/>
+        <v>43222</v>
       </c>
       <c r="B627" t="s">
         <v>6</v>
@@ -5486,8 +5486,7 @@
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A628" s="1">
-        <f>A627+1</f>
-        <v>43582</v>
+        <v>43581</v>
       </c>
       <c r="B628" t="s">
         <v>6</v>
@@ -5495,8 +5494,8 @@
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A629" s="1">
-        <f t="shared" ref="A629:A633" si="6">A628+1</f>
-        <v>43583</v>
+        <f>A628+1</f>
+        <v>43582</v>
       </c>
       <c r="B629" t="s">
         <v>6</v>
@@ -5504,8 +5503,8 @@
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A630" s="1">
-        <f t="shared" si="6"/>
-        <v>43584</v>
+        <f t="shared" ref="A630:A634" si="6">A629+1</f>
+        <v>43583</v>
       </c>
       <c r="B630" t="s">
         <v>6</v>
@@ -5514,7 +5513,7 @@
     <row r="631" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A631" s="1">
         <f t="shared" si="6"/>
-        <v>43585</v>
+        <v>43584</v>
       </c>
       <c r="B631" t="s">
         <v>6</v>
@@ -5523,7 +5522,7 @@
     <row r="632" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A632" s="1">
         <f t="shared" si="6"/>
-        <v>43586</v>
+        <v>43585</v>
       </c>
       <c r="B632" t="s">
         <v>6</v>
@@ -5532,7 +5531,7 @@
     <row r="633" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A633" s="1">
         <f t="shared" si="6"/>
-        <v>43587</v>
+        <v>43586</v>
       </c>
       <c r="B633" t="s">
         <v>6</v>
@@ -5540,7 +5539,8 @@
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A634" s="1">
-        <v>45046</v>
+        <f t="shared" si="6"/>
+        <v>43587</v>
       </c>
       <c r="B634" t="s">
         <v>6</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A635" s="1">
-        <v>45047</v>
+        <v>45046</v>
       </c>
       <c r="B635" t="s">
         <v>6</v>
@@ -5556,15 +5556,15 @@
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A636" s="1">
-        <v>42180</v>
+        <v>45047</v>
       </c>
       <c r="B636" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A637" s="1">
-        <v>42181</v>
+        <v>42180</v>
       </c>
       <c r="B637" t="s">
         <v>7</v>
@@ -5572,7 +5572,7 @@
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A638" s="1">
-        <v>42182</v>
+        <v>42181</v>
       </c>
       <c r="B638" t="s">
         <v>7</v>
@@ -5580,7 +5580,7 @@
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A639" s="1">
-        <v>42183</v>
+        <v>42182</v>
       </c>
       <c r="B639" t="s">
         <v>7</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A640" s="1">
-        <v>42184</v>
+        <v>42183</v>
       </c>
       <c r="B640" t="s">
         <v>7</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A641" s="1">
-        <v>42185</v>
+        <v>42184</v>
       </c>
       <c r="B641" t="s">
         <v>7</v>
@@ -5604,7 +5604,7 @@
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A642" s="1">
-        <v>42186</v>
+        <v>42185</v>
       </c>
       <c r="B642" t="s">
         <v>7</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A643" s="1">
-        <v>42187</v>
+        <v>42186</v>
       </c>
       <c r="B643" t="s">
         <v>7</v>
@@ -5620,7 +5620,7 @@
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A644" s="1">
-        <v>42188</v>
+        <v>42187</v>
       </c>
       <c r="B644" t="s">
         <v>7</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A645" s="1">
-        <v>42189</v>
+        <v>42188</v>
       </c>
       <c r="B645" t="s">
         <v>7</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A646" s="1">
-        <v>42190</v>
+        <v>42189</v>
       </c>
       <c r="B646" t="s">
         <v>7</v>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A647" s="1">
-        <v>42191</v>
+        <v>42190</v>
       </c>
       <c r="B647" t="s">
         <v>7</v>
@@ -5652,7 +5652,7 @@
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A648" s="1">
-        <v>42192</v>
+        <v>42191</v>
       </c>
       <c r="B648" t="s">
         <v>7</v>
@@ -5660,7 +5660,7 @@
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A649" s="1">
-        <v>42193</v>
+        <v>42192</v>
       </c>
       <c r="B649" t="s">
         <v>7</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A650" s="1">
-        <v>42194</v>
+        <v>42193</v>
       </c>
       <c r="B650" t="s">
         <v>7</v>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A651" s="1">
-        <v>42195</v>
+        <v>42194</v>
       </c>
       <c r="B651" t="s">
         <v>7</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A652" s="1">
-        <v>42196</v>
+        <v>42195</v>
       </c>
       <c r="B652" t="s">
         <v>7</v>
@@ -5692,7 +5692,7 @@
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A653" s="1">
-        <v>42197</v>
+        <v>42196</v>
       </c>
       <c r="B653" t="s">
         <v>7</v>
@@ -5700,7 +5700,7 @@
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A654" s="1">
-        <v>42198</v>
+        <v>42197</v>
       </c>
       <c r="B654" t="s">
         <v>7</v>
@@ -5708,7 +5708,7 @@
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A655" s="1">
-        <v>42199</v>
+        <v>42198</v>
       </c>
       <c r="B655" t="s">
         <v>7</v>
@@ -5716,7 +5716,7 @@
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A656" s="1">
-        <v>42200</v>
+        <v>42199</v>
       </c>
       <c r="B656" t="s">
         <v>7</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A657" s="1">
-        <v>42201</v>
+        <v>42200</v>
       </c>
       <c r="B657" t="s">
         <v>7</v>
@@ -5732,7 +5732,7 @@
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A658" s="1">
-        <v>42202</v>
+        <v>42201</v>
       </c>
       <c r="B658" t="s">
         <v>7</v>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A659" s="1">
-        <v>42203</v>
+        <v>42202</v>
       </c>
       <c r="B659" t="s">
         <v>7</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A660" s="1">
-        <v>42204</v>
+        <v>42203</v>
       </c>
       <c r="B660" t="s">
         <v>7</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A661" s="1">
-        <v>42205</v>
+        <v>42204</v>
       </c>
       <c r="B661" t="s">
         <v>7</v>
@@ -5764,7 +5764,7 @@
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A662" s="1">
-        <v>42206</v>
+        <v>42205</v>
       </c>
       <c r="B662" t="s">
         <v>7</v>
@@ -5772,7 +5772,7 @@
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A663" s="1">
-        <v>42207</v>
+        <v>42206</v>
       </c>
       <c r="B663" t="s">
         <v>7</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A664" s="1">
-        <v>42208</v>
+        <v>42207</v>
       </c>
       <c r="B664" t="s">
         <v>7</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A665" s="1">
-        <v>42209</v>
+        <v>42208</v>
       </c>
       <c r="B665" t="s">
         <v>7</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A666" s="1">
-        <v>42210</v>
+        <v>42209</v>
       </c>
       <c r="B666" t="s">
         <v>7</v>
@@ -5804,7 +5804,7 @@
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A667" s="1">
-        <v>42211</v>
+        <v>42210</v>
       </c>
       <c r="B667" t="s">
         <v>7</v>
@@ -5812,7 +5812,7 @@
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A668" s="1">
-        <v>42212</v>
+        <v>42211</v>
       </c>
       <c r="B668" t="s">
         <v>7</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A669" s="1">
-        <v>42213</v>
+        <v>42212</v>
       </c>
       <c r="B669" t="s">
         <v>7</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A670" s="1">
-        <v>42214</v>
+        <v>42213</v>
       </c>
       <c r="B670" t="s">
         <v>7</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A671" s="1">
-        <v>42215</v>
+        <v>42214</v>
       </c>
       <c r="B671" t="s">
         <v>7</v>
@@ -5844,7 +5844,7 @@
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A672" s="1">
-        <v>42216</v>
+        <v>42215</v>
       </c>
       <c r="B672" t="s">
         <v>7</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A673" s="1">
-        <v>42217</v>
+        <v>42216</v>
       </c>
       <c r="B673" t="s">
         <v>7</v>
@@ -5860,7 +5860,7 @@
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A674" s="1">
-        <v>42218</v>
+        <v>42217</v>
       </c>
       <c r="B674" t="s">
         <v>7</v>
@@ -5868,7 +5868,7 @@
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A675" s="1">
-        <v>42219</v>
+        <v>42218</v>
       </c>
       <c r="B675" t="s">
         <v>7</v>
@@ -5876,7 +5876,7 @@
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A676" s="1">
-        <v>42220</v>
+        <v>42219</v>
       </c>
       <c r="B676" t="s">
         <v>7</v>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A677" s="1">
-        <v>42221</v>
+        <v>42220</v>
       </c>
       <c r="B677" t="s">
         <v>7</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A678" s="1">
-        <v>42222</v>
+        <v>42221</v>
       </c>
       <c r="B678" t="s">
         <v>7</v>
@@ -5900,7 +5900,7 @@
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A679" s="1">
-        <v>42223</v>
+        <v>42222</v>
       </c>
       <c r="B679" t="s">
         <v>7</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A680" s="1">
-        <v>42224</v>
+        <v>42223</v>
       </c>
       <c r="B680" t="s">
         <v>7</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A681" s="1">
-        <v>42225</v>
+        <v>42224</v>
       </c>
       <c r="B681" t="s">
         <v>7</v>
@@ -5924,7 +5924,7 @@
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A682" s="1">
-        <v>42546</v>
+        <v>42225</v>
       </c>
       <c r="B682" t="s">
         <v>7</v>
@@ -5932,7 +5932,7 @@
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A683" s="1">
-        <v>42547</v>
+        <v>42546</v>
       </c>
       <c r="B683" t="s">
         <v>7</v>
@@ -5940,7 +5940,7 @@
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A684" s="1">
-        <v>42548</v>
+        <v>42547</v>
       </c>
       <c r="B684" t="s">
         <v>7</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A685" s="1">
-        <v>42549</v>
+        <v>42548</v>
       </c>
       <c r="B685" t="s">
         <v>7</v>
@@ -5956,7 +5956,7 @@
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A686" s="1">
-        <v>42550</v>
+        <v>42549</v>
       </c>
       <c r="B686" t="s">
         <v>7</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A687" s="1">
-        <v>42551</v>
+        <v>42550</v>
       </c>
       <c r="B687" t="s">
         <v>7</v>
@@ -5972,7 +5972,7 @@
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A688" s="1">
-        <v>42552</v>
+        <v>42551</v>
       </c>
       <c r="B688" t="s">
         <v>7</v>
@@ -5980,7 +5980,7 @@
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A689" s="1">
-        <v>42553</v>
+        <v>42552</v>
       </c>
       <c r="B689" t="s">
         <v>7</v>
@@ -5988,7 +5988,7 @@
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A690" s="1">
-        <v>42554</v>
+        <v>42553</v>
       </c>
       <c r="B690" t="s">
         <v>7</v>
@@ -5996,7 +5996,7 @@
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A691" s="1">
-        <v>42555</v>
+        <v>42554</v>
       </c>
       <c r="B691" t="s">
         <v>7</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A692" s="1">
-        <v>42556</v>
+        <v>42555</v>
       </c>
       <c r="B692" t="s">
         <v>7</v>
@@ -6012,7 +6012,7 @@
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A693" s="1">
-        <v>42557</v>
+        <v>42556</v>
       </c>
       <c r="B693" t="s">
         <v>7</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A694" s="1">
-        <v>42558</v>
+        <v>42557</v>
       </c>
       <c r="B694" t="s">
         <v>7</v>
@@ -6028,7 +6028,7 @@
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A695" s="1">
-        <v>42559</v>
+        <v>42558</v>
       </c>
       <c r="B695" t="s">
         <v>7</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A696" s="1">
-        <v>42560</v>
+        <v>42559</v>
       </c>
       <c r="B696" t="s">
         <v>7</v>
@@ -6044,7 +6044,7 @@
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A697" s="1">
-        <v>42561</v>
+        <v>42560</v>
       </c>
       <c r="B697" t="s">
         <v>7</v>
@@ -6052,7 +6052,7 @@
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A698" s="1">
-        <v>42562</v>
+        <v>42561</v>
       </c>
       <c r="B698" t="s">
         <v>7</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A699" s="1">
-        <v>42563</v>
+        <v>42562</v>
       </c>
       <c r="B699" t="s">
         <v>7</v>
@@ -6068,7 +6068,7 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A700" s="1">
-        <v>42564</v>
+        <v>42563</v>
       </c>
       <c r="B700" t="s">
         <v>7</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A701" s="1">
-        <v>42565</v>
+        <v>42564</v>
       </c>
       <c r="B701" t="s">
         <v>7</v>
@@ -6084,7 +6084,7 @@
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A702" s="1">
-        <v>42566</v>
+        <v>42565</v>
       </c>
       <c r="B702" t="s">
         <v>7</v>
@@ -6092,7 +6092,7 @@
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A703" s="1">
-        <v>42567</v>
+        <v>42566</v>
       </c>
       <c r="B703" t="s">
         <v>7</v>
@@ -6100,7 +6100,7 @@
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A704" s="1">
-        <v>42568</v>
+        <v>42567</v>
       </c>
       <c r="B704" t="s">
         <v>7</v>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A705" s="1">
-        <v>42569</v>
+        <v>42568</v>
       </c>
       <c r="B705" t="s">
         <v>7</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A706" s="1">
-        <v>42570</v>
+        <v>42569</v>
       </c>
       <c r="B706" t="s">
         <v>7</v>
@@ -6124,7 +6124,7 @@
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A707" s="1">
-        <v>42571</v>
+        <v>42570</v>
       </c>
       <c r="B707" t="s">
         <v>7</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A708" s="1">
-        <v>42572</v>
+        <v>42571</v>
       </c>
       <c r="B708" t="s">
         <v>7</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A709" s="1">
-        <v>42573</v>
+        <v>42572</v>
       </c>
       <c r="B709" t="s">
         <v>7</v>
@@ -6148,7 +6148,7 @@
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A710" s="1">
-        <v>42574</v>
+        <v>42573</v>
       </c>
       <c r="B710" t="s">
         <v>7</v>
@@ -6156,7 +6156,7 @@
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A711" s="1">
-        <v>42575</v>
+        <v>42574</v>
       </c>
       <c r="B711" t="s">
         <v>7</v>
@@ -6164,7 +6164,7 @@
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A712" s="1">
-        <v>42576</v>
+        <v>42575</v>
       </c>
       <c r="B712" t="s">
         <v>7</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A713" s="1">
-        <v>42577</v>
+        <v>42576</v>
       </c>
       <c r="B713" t="s">
         <v>7</v>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A714" s="1">
-        <v>42578</v>
+        <v>42577</v>
       </c>
       <c r="B714" t="s">
         <v>7</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A715" s="1">
-        <v>42579</v>
+        <v>42578</v>
       </c>
       <c r="B715" t="s">
         <v>7</v>
@@ -6196,7 +6196,7 @@
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A716" s="1">
-        <v>42580</v>
+        <v>42579</v>
       </c>
       <c r="B716" t="s">
         <v>7</v>
@@ -6204,7 +6204,7 @@
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A717" s="1">
-        <v>42581</v>
+        <v>42580</v>
       </c>
       <c r="B717" t="s">
         <v>7</v>
@@ -6212,7 +6212,7 @@
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A718" s="1">
-        <v>42582</v>
+        <v>42581</v>
       </c>
       <c r="B718" t="s">
         <v>7</v>
@@ -6220,7 +6220,7 @@
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A719" s="1">
-        <v>42583</v>
+        <v>42582</v>
       </c>
       <c r="B719" t="s">
         <v>7</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A720" s="1">
-        <v>42584</v>
+        <v>42583</v>
       </c>
       <c r="B720" t="s">
         <v>7</v>
@@ -6236,7 +6236,7 @@
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A721" s="1">
-        <v>42585</v>
+        <v>42584</v>
       </c>
       <c r="B721" t="s">
         <v>7</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" s="1">
-        <v>42586</v>
+        <v>42585</v>
       </c>
       <c r="B722" t="s">
         <v>7</v>
@@ -6252,7 +6252,7 @@
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A723" s="1">
-        <v>42587</v>
+        <v>42586</v>
       </c>
       <c r="B723" t="s">
         <v>7</v>
@@ -6260,7 +6260,7 @@
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A724" s="1">
-        <v>42588</v>
+        <v>42587</v>
       </c>
       <c r="B724" t="s">
         <v>7</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A725" s="1">
-        <v>42589</v>
+        <v>42588</v>
       </c>
       <c r="B725" t="s">
         <v>7</v>
@@ -6276,7 +6276,7 @@
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A726" s="1">
-        <v>42590</v>
+        <v>42589</v>
       </c>
       <c r="B726" t="s">
         <v>7</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A727" s="1">
-        <v>42911</v>
+        <v>42590</v>
       </c>
       <c r="B727" t="s">
         <v>7</v>
@@ -6292,7 +6292,7 @@
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A728" s="1">
-        <v>42912</v>
+        <v>42911</v>
       </c>
       <c r="B728" t="s">
         <v>7</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A729" s="1">
-        <v>42913</v>
+        <v>42912</v>
       </c>
       <c r="B729" t="s">
         <v>7</v>
@@ -6308,7 +6308,7 @@
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A730" s="1">
-        <v>42914</v>
+        <v>42913</v>
       </c>
       <c r="B730" t="s">
         <v>7</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A731" s="1">
-        <v>42915</v>
+        <v>42914</v>
       </c>
       <c r="B731" t="s">
         <v>7</v>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A732" s="1">
-        <v>42916</v>
+        <v>42915</v>
       </c>
       <c r="B732" t="s">
         <v>7</v>
@@ -6332,7 +6332,7 @@
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A733" s="1">
-        <v>42917</v>
+        <v>42916</v>
       </c>
       <c r="B733" t="s">
         <v>7</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A734" s="1">
-        <v>42918</v>
+        <v>42917</v>
       </c>
       <c r="B734" t="s">
         <v>7</v>
@@ -6348,7 +6348,7 @@
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A735" s="1">
-        <v>42919</v>
+        <v>42918</v>
       </c>
       <c r="B735" t="s">
         <v>7</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A736" s="1">
-        <v>42920</v>
+        <v>42919</v>
       </c>
       <c r="B736" t="s">
         <v>7</v>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A737" s="1">
-        <v>42921</v>
+        <v>42920</v>
       </c>
       <c r="B737" t="s">
         <v>7</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A738" s="1">
-        <v>42922</v>
+        <v>42921</v>
       </c>
       <c r="B738" t="s">
         <v>7</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A739" s="1">
-        <v>42923</v>
+        <v>42922</v>
       </c>
       <c r="B739" t="s">
         <v>7</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A740" s="1">
-        <v>42924</v>
+        <v>42923</v>
       </c>
       <c r="B740" t="s">
         <v>7</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A741" s="1">
-        <v>42925</v>
+        <v>42924</v>
       </c>
       <c r="B741" t="s">
         <v>7</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A742" s="1">
-        <v>42926</v>
+        <v>42925</v>
       </c>
       <c r="B742" t="s">
         <v>7</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A743" s="1">
-        <v>42927</v>
+        <v>42926</v>
       </c>
       <c r="B743" t="s">
         <v>7</v>
@@ -6420,7 +6420,7 @@
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A744" s="1">
-        <v>42928</v>
+        <v>42927</v>
       </c>
       <c r="B744" t="s">
         <v>7</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A745" s="1">
-        <v>42929</v>
+        <v>42928</v>
       </c>
       <c r="B745" t="s">
         <v>7</v>
@@ -6436,7 +6436,7 @@
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A746" s="1">
-        <v>42930</v>
+        <v>42929</v>
       </c>
       <c r="B746" t="s">
         <v>7</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A747" s="1">
-        <v>42931</v>
+        <v>42930</v>
       </c>
       <c r="B747" t="s">
         <v>7</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A748" s="1">
-        <v>42932</v>
+        <v>42931</v>
       </c>
       <c r="B748" t="s">
         <v>7</v>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A749" s="1">
-        <v>42933</v>
+        <v>42932</v>
       </c>
       <c r="B749" t="s">
         <v>7</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A750" s="1">
-        <v>42934</v>
+        <v>42933</v>
       </c>
       <c r="B750" t="s">
         <v>7</v>
@@ -6476,7 +6476,7 @@
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A751" s="1">
-        <v>42935</v>
+        <v>42934</v>
       </c>
       <c r="B751" t="s">
         <v>7</v>
@@ -6484,7 +6484,7 @@
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A752" s="1">
-        <v>42936</v>
+        <v>42935</v>
       </c>
       <c r="B752" t="s">
         <v>7</v>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A753" s="1">
-        <v>42937</v>
+        <v>42936</v>
       </c>
       <c r="B753" t="s">
         <v>7</v>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A754" s="1">
-        <v>42938</v>
+        <v>42937</v>
       </c>
       <c r="B754" t="s">
         <v>7</v>
@@ -6508,7 +6508,7 @@
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A755" s="1">
-        <v>42939</v>
+        <v>42938</v>
       </c>
       <c r="B755" t="s">
         <v>7</v>
@@ -6516,7 +6516,7 @@
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A756" s="1">
-        <v>42940</v>
+        <v>42939</v>
       </c>
       <c r="B756" t="s">
         <v>7</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A757" s="1">
-        <v>42941</v>
+        <v>42940</v>
       </c>
       <c r="B757" t="s">
         <v>7</v>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A758" s="1">
-        <v>42942</v>
+        <v>42941</v>
       </c>
       <c r="B758" t="s">
         <v>7</v>
@@ -6540,7 +6540,7 @@
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A759" s="1">
-        <v>42943</v>
+        <v>42942</v>
       </c>
       <c r="B759" t="s">
         <v>7</v>
@@ -6548,7 +6548,7 @@
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A760" s="1">
-        <v>42944</v>
+        <v>42943</v>
       </c>
       <c r="B760" t="s">
         <v>7</v>
@@ -6556,7 +6556,7 @@
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A761" s="1">
-        <v>42945</v>
+        <v>42944</v>
       </c>
       <c r="B761" t="s">
         <v>7</v>
@@ -6564,7 +6564,7 @@
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A762" s="1">
-        <v>42946</v>
+        <v>42945</v>
       </c>
       <c r="B762" t="s">
         <v>7</v>
@@ -6572,7 +6572,7 @@
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A763" s="1">
-        <v>43276</v>
+        <v>42946</v>
       </c>
       <c r="B763" t="s">
         <v>7</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A764" s="1">
-        <v>43277</v>
+        <v>43276</v>
       </c>
       <c r="B764" t="s">
         <v>7</v>
@@ -6588,7 +6588,7 @@
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A765" s="1">
-        <v>43278</v>
+        <v>43277</v>
       </c>
       <c r="B765" t="s">
         <v>7</v>
@@ -6596,7 +6596,7 @@
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A766" s="1">
-        <v>43279</v>
+        <v>43278</v>
       </c>
       <c r="B766" t="s">
         <v>7</v>
@@ -6604,7 +6604,7 @@
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A767" s="1">
-        <v>43280</v>
+        <v>43279</v>
       </c>
       <c r="B767" t="s">
         <v>7</v>
@@ -6612,7 +6612,7 @@
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A768" s="1">
-        <v>43281</v>
+        <v>43280</v>
       </c>
       <c r="B768" t="s">
         <v>7</v>
@@ -6620,7 +6620,7 @@
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A769" s="1">
-        <v>43282</v>
+        <v>43281</v>
       </c>
       <c r="B769" t="s">
         <v>7</v>
@@ -6628,7 +6628,7 @@
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A770" s="1">
-        <v>43283</v>
+        <v>43282</v>
       </c>
       <c r="B770" t="s">
         <v>7</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A771" s="1">
-        <v>43284</v>
+        <v>43283</v>
       </c>
       <c r="B771" t="s">
         <v>7</v>
@@ -6644,7 +6644,7 @@
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A772" s="1">
-        <v>43285</v>
+        <v>43284</v>
       </c>
       <c r="B772" t="s">
         <v>7</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A773" s="1">
-        <v>43286</v>
+        <v>43285</v>
       </c>
       <c r="B773" t="s">
         <v>7</v>
@@ -6660,7 +6660,7 @@
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A774" s="1">
-        <v>43287</v>
+        <v>43286</v>
       </c>
       <c r="B774" t="s">
         <v>7</v>
@@ -6668,7 +6668,7 @@
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A775" s="1">
-        <v>43288</v>
+        <v>43287</v>
       </c>
       <c r="B775" t="s">
         <v>7</v>
@@ -6676,7 +6676,7 @@
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A776" s="1">
-        <v>43289</v>
+        <v>43288</v>
       </c>
       <c r="B776" t="s">
         <v>7</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A777" s="1">
-        <v>43290</v>
+        <v>43289</v>
       </c>
       <c r="B777" t="s">
         <v>7</v>
@@ -6692,7 +6692,7 @@
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A778" s="1">
-        <v>43291</v>
+        <v>43290</v>
       </c>
       <c r="B778" t="s">
         <v>7</v>
@@ -6700,7 +6700,7 @@
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A779" s="1">
-        <v>43292</v>
+        <v>43291</v>
       </c>
       <c r="B779" t="s">
         <v>7</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A780" s="1">
-        <v>43293</v>
+        <v>43292</v>
       </c>
       <c r="B780" t="s">
         <v>7</v>
@@ -6716,7 +6716,7 @@
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A781" s="1">
-        <v>43294</v>
+        <v>43293</v>
       </c>
       <c r="B781" t="s">
         <v>7</v>
@@ -6724,7 +6724,7 @@
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A782" s="1">
-        <v>43295</v>
+        <v>43294</v>
       </c>
       <c r="B782" t="s">
         <v>7</v>
@@ -6732,7 +6732,7 @@
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A783" s="1">
-        <v>43296</v>
+        <v>43295</v>
       </c>
       <c r="B783" t="s">
         <v>7</v>
@@ -6740,7 +6740,7 @@
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A784" s="1">
-        <v>43297</v>
+        <v>43296</v>
       </c>
       <c r="B784" t="s">
         <v>7</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A785" s="1">
-        <v>43298</v>
+        <v>43297</v>
       </c>
       <c r="B785" t="s">
         <v>7</v>
@@ -6756,7 +6756,7 @@
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A786" s="1">
-        <v>43299</v>
+        <v>43298</v>
       </c>
       <c r="B786" t="s">
         <v>7</v>
@@ -6764,7 +6764,7 @@
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A787" s="1">
-        <v>43300</v>
+        <v>43299</v>
       </c>
       <c r="B787" t="s">
         <v>7</v>
@@ -6772,7 +6772,7 @@
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A788" s="1">
-        <v>43301</v>
+        <v>43300</v>
       </c>
       <c r="B788" t="s">
         <v>7</v>
@@ -6780,7 +6780,7 @@
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A789" s="1">
-        <v>43302</v>
+        <v>43301</v>
       </c>
       <c r="B789" t="s">
         <v>7</v>
@@ -6788,7 +6788,7 @@
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A790" s="1">
-        <v>43303</v>
+        <v>43302</v>
       </c>
       <c r="B790" t="s">
         <v>7</v>
@@ -6796,7 +6796,7 @@
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A791" s="1">
-        <v>43304</v>
+        <v>43303</v>
       </c>
       <c r="B791" t="s">
         <v>7</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A792" s="1">
-        <v>43305</v>
+        <v>43304</v>
       </c>
       <c r="B792" t="s">
         <v>7</v>
@@ -6812,7 +6812,7 @@
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A793" s="1">
-        <v>43306</v>
+        <v>43305</v>
       </c>
       <c r="B793" t="s">
         <v>7</v>
@@ -6820,7 +6820,7 @@
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A794" s="1">
-        <v>43307</v>
+        <v>43306</v>
       </c>
       <c r="B794" t="s">
         <v>7</v>
@@ -6828,7 +6828,7 @@
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A795" s="1">
-        <v>43308</v>
+        <v>43307</v>
       </c>
       <c r="B795" t="s">
         <v>7</v>
@@ -6836,7 +6836,7 @@
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A796" s="1">
-        <v>43309</v>
+        <v>43308</v>
       </c>
       <c r="B796" t="s">
         <v>7</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A797" s="1">
-        <v>43310</v>
+        <v>43309</v>
       </c>
       <c r="B797" t="s">
         <v>7</v>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A798" s="1">
-        <v>43311</v>
+        <v>43310</v>
       </c>
       <c r="B798" t="s">
         <v>7</v>
@@ -6860,7 +6860,7 @@
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A799" s="1">
-        <v>43312</v>
+        <v>43311</v>
       </c>
       <c r="B799" t="s">
         <v>7</v>
@@ -6868,7 +6868,7 @@
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A800" s="1">
-        <v>43641</v>
+        <v>43312</v>
       </c>
       <c r="B800" t="s">
         <v>7</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A801" s="1">
-        <v>43642</v>
+        <v>43641</v>
       </c>
       <c r="B801" t="s">
         <v>7</v>
@@ -6884,7 +6884,7 @@
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A802" s="1">
-        <v>43643</v>
+        <v>43642</v>
       </c>
       <c r="B802" t="s">
         <v>7</v>
@@ -6892,7 +6892,7 @@
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A803" s="1">
-        <v>43644</v>
+        <v>43643</v>
       </c>
       <c r="B803" t="s">
         <v>7</v>
@@ -6900,7 +6900,7 @@
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A804" s="1">
-        <v>43645</v>
+        <v>43644</v>
       </c>
       <c r="B804" t="s">
         <v>7</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A805" s="1">
-        <v>43646</v>
+        <v>43645</v>
       </c>
       <c r="B805" t="s">
         <v>7</v>
@@ -6916,7 +6916,7 @@
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A806" s="1">
-        <v>43647</v>
+        <v>43646</v>
       </c>
       <c r="B806" t="s">
         <v>7</v>
@@ -6924,7 +6924,7 @@
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A807" s="1">
-        <v>43648</v>
+        <v>43647</v>
       </c>
       <c r="B807" t="s">
         <v>7</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A808" s="1">
-        <v>43649</v>
+        <v>43648</v>
       </c>
       <c r="B808" t="s">
         <v>7</v>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A809" s="1">
-        <v>43650</v>
+        <v>43649</v>
       </c>
       <c r="B809" t="s">
         <v>7</v>
@@ -6948,7 +6948,7 @@
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A810" s="1">
-        <v>43651</v>
+        <v>43650</v>
       </c>
       <c r="B810" t="s">
         <v>7</v>
@@ -6956,7 +6956,7 @@
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A811" s="1">
-        <v>43652</v>
+        <v>43651</v>
       </c>
       <c r="B811" t="s">
         <v>7</v>
@@ -6964,7 +6964,7 @@
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A812" s="1">
-        <v>43653</v>
+        <v>43652</v>
       </c>
       <c r="B812" t="s">
         <v>7</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A813" s="1">
-        <v>43654</v>
+        <v>43653</v>
       </c>
       <c r="B813" t="s">
         <v>7</v>
@@ -6980,7 +6980,7 @@
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A814" s="1">
-        <v>43655</v>
+        <v>43654</v>
       </c>
       <c r="B814" t="s">
         <v>7</v>
@@ -6988,7 +6988,7 @@
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A815" s="1">
-        <v>43656</v>
+        <v>43655</v>
       </c>
       <c r="B815" t="s">
         <v>7</v>
@@ -6996,7 +6996,7 @@
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A816" s="1">
-        <v>43657</v>
+        <v>43656</v>
       </c>
       <c r="B816" t="s">
         <v>7</v>
@@ -7004,7 +7004,7 @@
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A817" s="1">
-        <v>43658</v>
+        <v>43657</v>
       </c>
       <c r="B817" t="s">
         <v>7</v>
@@ -7012,7 +7012,7 @@
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A818" s="1">
-        <v>43659</v>
+        <v>43658</v>
       </c>
       <c r="B818" t="s">
         <v>7</v>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A819" s="1">
-        <v>43660</v>
+        <v>43659</v>
       </c>
       <c r="B819" t="s">
         <v>7</v>
@@ -7028,7 +7028,7 @@
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A820" s="1">
-        <v>43661</v>
+        <v>43660</v>
       </c>
       <c r="B820" t="s">
         <v>7</v>
@@ -7036,7 +7036,7 @@
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A821" s="1">
-        <v>43662</v>
+        <v>43661</v>
       </c>
       <c r="B821" t="s">
         <v>7</v>
@@ -7044,7 +7044,7 @@
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A822" s="1">
-        <v>43663</v>
+        <v>43662</v>
       </c>
       <c r="B822" t="s">
         <v>7</v>
@@ -7052,7 +7052,7 @@
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A823" s="1">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="B823" t="s">
         <v>7</v>
@@ -7060,7 +7060,7 @@
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A824" s="1">
-        <v>43665</v>
+        <v>43664</v>
       </c>
       <c r="B824" t="s">
         <v>7</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A825" s="1">
-        <v>43666</v>
+        <v>43665</v>
       </c>
       <c r="B825" t="s">
         <v>7</v>
@@ -7076,7 +7076,7 @@
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A826" s="1">
-        <v>43667</v>
+        <v>43666</v>
       </c>
       <c r="B826" t="s">
         <v>7</v>
@@ -7084,7 +7084,7 @@
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A827" s="1">
-        <v>43668</v>
+        <v>43667</v>
       </c>
       <c r="B827" t="s">
         <v>7</v>
@@ -7092,7 +7092,7 @@
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A828" s="1">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="B828" t="s">
         <v>7</v>
@@ -7100,7 +7100,7 @@
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A829" s="1">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="B829" t="s">
         <v>7</v>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A830" s="1">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="B830" t="s">
         <v>7</v>
@@ -7116,7 +7116,7 @@
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A831" s="1">
-        <v>43672</v>
+        <v>43671</v>
       </c>
       <c r="B831" t="s">
         <v>7</v>
@@ -7124,7 +7124,7 @@
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A832" s="1">
-        <v>43673</v>
+        <v>43672</v>
       </c>
       <c r="B832" t="s">
         <v>7</v>
@@ -7132,7 +7132,7 @@
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A833" s="1">
-        <v>43674</v>
+        <v>43673</v>
       </c>
       <c r="B833" t="s">
         <v>7</v>
@@ -7140,7 +7140,7 @@
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="1">
-        <v>43675</v>
+        <v>43674</v>
       </c>
       <c r="B834" t="s">
         <v>7</v>
@@ -7148,7 +7148,7 @@
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="1">
-        <v>43676</v>
+        <v>43675</v>
       </c>
       <c r="B835" t="s">
         <v>7</v>
@@ -7156,7 +7156,7 @@
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="1">
-        <v>44737</v>
+        <v>43676</v>
       </c>
       <c r="B836" t="s">
         <v>7</v>
@@ -7164,7 +7164,7 @@
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A837" s="1">
-        <v>44738</v>
+        <v>44737</v>
       </c>
       <c r="B837" t="s">
         <v>7</v>
@@ -7172,7 +7172,7 @@
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A838" s="1">
-        <v>44739</v>
+        <v>44738</v>
       </c>
       <c r="B838" t="s">
         <v>7</v>
@@ -7180,7 +7180,7 @@
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A839" s="1">
-        <v>44740</v>
+        <v>44739</v>
       </c>
       <c r="B839" t="s">
         <v>7</v>
@@ -7188,7 +7188,7 @@
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="1">
-        <v>44741</v>
+        <v>44740</v>
       </c>
       <c r="B840" t="s">
         <v>7</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A841" s="1">
-        <v>44742</v>
+        <v>44741</v>
       </c>
       <c r="B841" t="s">
         <v>7</v>
@@ -7204,7 +7204,7 @@
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="1">
-        <v>44743</v>
+        <v>44742</v>
       </c>
       <c r="B842" t="s">
         <v>7</v>
@@ -7212,7 +7212,7 @@
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A843" s="1">
-        <v>44744</v>
+        <v>44743</v>
       </c>
       <c r="B843" t="s">
         <v>7</v>
@@ -7220,7 +7220,7 @@
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A844" s="1">
-        <v>44745</v>
+        <v>44744</v>
       </c>
       <c r="B844" t="s">
         <v>7</v>
@@ -7228,7 +7228,7 @@
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A845" s="1">
-        <v>44746</v>
+        <v>44745</v>
       </c>
       <c r="B845" t="s">
         <v>7</v>
@@ -7236,7 +7236,7 @@
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="1">
-        <v>44747</v>
+        <v>44746</v>
       </c>
       <c r="B846" t="s">
         <v>7</v>
@@ -7244,7 +7244,7 @@
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A847" s="1">
-        <v>44748</v>
+        <v>44747</v>
       </c>
       <c r="B847" t="s">
         <v>7</v>
@@ -7252,7 +7252,7 @@
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A848" s="1">
-        <v>44749</v>
+        <v>44748</v>
       </c>
       <c r="B848" t="s">
         <v>7</v>
@@ -7260,7 +7260,7 @@
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A849" s="1">
-        <v>44750</v>
+        <v>44749</v>
       </c>
       <c r="B849" t="s">
         <v>7</v>
@@ -7268,7 +7268,7 @@
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="1">
-        <v>44751</v>
+        <v>44750</v>
       </c>
       <c r="B850" t="s">
         <v>7</v>
@@ -7276,7 +7276,7 @@
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="1">
-        <v>44752</v>
+        <v>44751</v>
       </c>
       <c r="B851" t="s">
         <v>7</v>
@@ -7284,7 +7284,7 @@
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="1">
-        <v>44753</v>
+        <v>44752</v>
       </c>
       <c r="B852" t="s">
         <v>7</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="1">
-        <v>44754</v>
+        <v>44753</v>
       </c>
       <c r="B853" t="s">
         <v>7</v>
@@ -7300,7 +7300,7 @@
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="1">
-        <v>44755</v>
+        <v>44754</v>
       </c>
       <c r="B854" t="s">
         <v>7</v>
@@ -7308,7 +7308,7 @@
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="1">
-        <v>44756</v>
+        <v>44755</v>
       </c>
       <c r="B855" t="s">
         <v>7</v>
@@ -7316,7 +7316,7 @@
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="1">
-        <v>44757</v>
+        <v>44756</v>
       </c>
       <c r="B856" t="s">
         <v>7</v>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A857" s="1">
-        <v>44758</v>
+        <v>44757</v>
       </c>
       <c r="B857" t="s">
         <v>7</v>
@@ -7332,7 +7332,7 @@
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="1">
-        <v>44759</v>
+        <v>44758</v>
       </c>
       <c r="B858" t="s">
         <v>7</v>
@@ -7340,7 +7340,7 @@
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="1">
-        <v>44760</v>
+        <v>44759</v>
       </c>
       <c r="B859" t="s">
         <v>7</v>
@@ -7348,7 +7348,7 @@
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="1">
-        <v>44761</v>
+        <v>44760</v>
       </c>
       <c r="B860" t="s">
         <v>7</v>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="1">
-        <v>44762</v>
+        <v>44761</v>
       </c>
       <c r="B861" t="s">
         <v>7</v>
@@ -7364,7 +7364,7 @@
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="1">
-        <v>44763</v>
+        <v>44762</v>
       </c>
       <c r="B862" t="s">
         <v>7</v>
@@ -7372,7 +7372,7 @@
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="1">
-        <v>44764</v>
+        <v>44763</v>
       </c>
       <c r="B863" t="s">
         <v>7</v>
@@ -7380,7 +7380,7 @@
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="1">
-        <v>44765</v>
+        <v>44764</v>
       </c>
       <c r="B864" t="s">
         <v>7</v>
@@ -7388,7 +7388,7 @@
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="1">
-        <v>44766</v>
+        <v>44765</v>
       </c>
       <c r="B865" t="s">
         <v>7</v>
@@ -7396,7 +7396,7 @@
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="1">
-        <v>44767</v>
+        <v>44766</v>
       </c>
       <c r="B866" t="s">
         <v>7</v>
@@ -7404,7 +7404,7 @@
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="1">
-        <v>44768</v>
+        <v>44767</v>
       </c>
       <c r="B867" t="s">
         <v>7</v>
@@ -7412,7 +7412,7 @@
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="1">
-        <v>44769</v>
+        <v>44768</v>
       </c>
       <c r="B868" t="s">
         <v>7</v>
@@ -7420,7 +7420,7 @@
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="1">
-        <v>44770</v>
+        <v>44769</v>
       </c>
       <c r="B869" t="s">
         <v>7</v>
@@ -7428,7 +7428,7 @@
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="1">
-        <v>44771</v>
+        <v>44770</v>
       </c>
       <c r="B870" t="s">
         <v>7</v>
@@ -7436,7 +7436,7 @@
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="1">
-        <v>44772</v>
+        <v>44771</v>
       </c>
       <c r="B871" t="s">
         <v>7</v>
@@ -7444,7 +7444,7 @@
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="1">
-        <v>44773</v>
+        <v>44772</v>
       </c>
       <c r="B872" t="s">
         <v>7</v>
@@ -7452,16 +7452,15 @@
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="1">
-        <v>44677</v>
+        <v>44773</v>
       </c>
       <c r="B873" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="1">
-        <f>A873+1</f>
-        <v>44678</v>
+        <v>44677</v>
       </c>
       <c r="B874" t="s">
         <v>6</v>
@@ -7469,8 +7468,8 @@
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="1">
-        <f t="shared" ref="A875:A879" si="7">A874+1</f>
-        <v>44679</v>
+        <f>A874+1</f>
+        <v>44678</v>
       </c>
       <c r="B875" t="s">
         <v>6</v>
@@ -7478,8 +7477,8 @@
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="1">
-        <f t="shared" si="7"/>
-        <v>44680</v>
+        <f t="shared" ref="A876:A880" si="7">A875+1</f>
+        <v>44679</v>
       </c>
       <c r="B876" t="s">
         <v>6</v>
@@ -7488,7 +7487,7 @@
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="1">
         <f t="shared" si="7"/>
-        <v>44681</v>
+        <v>44680</v>
       </c>
       <c r="B877" t="s">
         <v>6</v>
@@ -7497,7 +7496,7 @@
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="1">
         <f t="shared" si="7"/>
-        <v>44682</v>
+        <v>44681</v>
       </c>
       <c r="B878" t="s">
         <v>6</v>
@@ -7506,7 +7505,7 @@
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="1">
         <f t="shared" si="7"/>
-        <v>44683</v>
+        <v>44682</v>
       </c>
       <c r="B879" t="s">
         <v>6</v>
@@ -7514,7 +7513,8 @@
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="1">
-        <v>44312</v>
+        <f t="shared" si="7"/>
+        <v>44683</v>
       </c>
       <c r="B880" t="s">
         <v>6</v>
@@ -7522,8 +7522,7 @@
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="1">
-        <f>A880+1</f>
-        <v>44313</v>
+        <v>44312</v>
       </c>
       <c r="B881" t="s">
         <v>6</v>
@@ -7531,8 +7530,8 @@
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="1">
-        <f t="shared" ref="A882:A886" si="8">A881+1</f>
-        <v>44314</v>
+        <f>A881+1</f>
+        <v>44313</v>
       </c>
       <c r="B882" t="s">
         <v>6</v>
@@ -7540,8 +7539,8 @@
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="1">
-        <f t="shared" si="8"/>
-        <v>44315</v>
+        <f t="shared" ref="A883:A887" si="8">A882+1</f>
+        <v>44314</v>
       </c>
       <c r="B883" t="s">
         <v>6</v>
@@ -7550,7 +7549,7 @@
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="1">
         <f t="shared" si="8"/>
-        <v>44316</v>
+        <v>44315</v>
       </c>
       <c r="B884" t="s">
         <v>6</v>
@@ -7559,7 +7558,7 @@
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="1">
         <f t="shared" si="8"/>
-        <v>44317</v>
+        <v>44316</v>
       </c>
       <c r="B885" t="s">
         <v>6</v>
@@ -7568,7 +7567,7 @@
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="1">
         <f t="shared" si="8"/>
-        <v>44318</v>
+        <v>44317</v>
       </c>
       <c r="B886" t="s">
         <v>6</v>
@@ -7576,7 +7575,8 @@
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="1">
-        <v>43947</v>
+        <f t="shared" si="8"/>
+        <v>44318</v>
       </c>
       <c r="B887" t="s">
         <v>6</v>
@@ -7584,8 +7584,7 @@
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="1">
-        <f>A887+1</f>
-        <v>43948</v>
+        <v>43947</v>
       </c>
       <c r="B888" t="s">
         <v>6</v>
@@ -7593,8 +7592,8 @@
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="1">
-        <f t="shared" ref="A889:A893" si="9">A888+1</f>
-        <v>43949</v>
+        <f>A888+1</f>
+        <v>43948</v>
       </c>
       <c r="B889" t="s">
         <v>6</v>
@@ -7602,8 +7601,8 @@
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="1">
-        <f t="shared" si="9"/>
-        <v>43950</v>
+        <f t="shared" ref="A890:A894" si="9">A889+1</f>
+        <v>43949</v>
       </c>
       <c r="B890" t="s">
         <v>6</v>
@@ -7612,7 +7611,7 @@
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="1">
         <f t="shared" si="9"/>
-        <v>43951</v>
+        <v>43950</v>
       </c>
       <c r="B891" t="s">
         <v>6</v>
@@ -7621,7 +7620,7 @@
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="1">
         <f t="shared" si="9"/>
-        <v>43952</v>
+        <v>43951</v>
       </c>
       <c r="B892" t="s">
         <v>6</v>
@@ -7630,7 +7629,7 @@
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A893" s="1">
         <f t="shared" si="9"/>
-        <v>43953</v>
+        <v>43952</v>
       </c>
       <c r="B893" t="s">
         <v>6</v>
@@ -7638,15 +7637,16 @@
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="1">
-        <v>44007</v>
+        <f t="shared" si="9"/>
+        <v>43953</v>
       </c>
       <c r="B894" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="1">
-        <v>44008</v>
+        <v>44007</v>
       </c>
       <c r="B895" t="s">
         <v>7</v>
@@ -7654,7 +7654,7 @@
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="1">
-        <v>44009</v>
+        <v>44008</v>
       </c>
       <c r="B896" t="s">
         <v>7</v>
@@ -7662,7 +7662,7 @@
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="1">
-        <v>44010</v>
+        <v>44009</v>
       </c>
       <c r="B897" t="s">
         <v>7</v>
@@ -7670,7 +7670,7 @@
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A898" s="1">
-        <v>44011</v>
+        <v>44010</v>
       </c>
       <c r="B898" t="s">
         <v>7</v>
@@ -7678,7 +7678,7 @@
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="1">
-        <v>44012</v>
+        <v>44011</v>
       </c>
       <c r="B899" t="s">
         <v>7</v>
@@ -7686,7 +7686,7 @@
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="1">
-        <v>44013</v>
+        <v>44012</v>
       </c>
       <c r="B900" t="s">
         <v>7</v>
@@ -7694,7 +7694,7 @@
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="1">
-        <v>44014</v>
+        <v>44013</v>
       </c>
       <c r="B901" t="s">
         <v>7</v>
@@ -7702,7 +7702,7 @@
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="1">
-        <v>44015</v>
+        <v>44014</v>
       </c>
       <c r="B902" t="s">
         <v>7</v>
@@ -7710,7 +7710,7 @@
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="1">
-        <v>44016</v>
+        <v>44015</v>
       </c>
       <c r="B903" t="s">
         <v>7</v>
@@ -7718,7 +7718,7 @@
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="1">
-        <v>44017</v>
+        <v>44016</v>
       </c>
       <c r="B904" t="s">
         <v>7</v>
@@ -7726,7 +7726,7 @@
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="1">
-        <v>44018</v>
+        <v>44017</v>
       </c>
       <c r="B905" t="s">
         <v>7</v>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="1">
-        <v>44019</v>
+        <v>44018</v>
       </c>
       <c r="B906" t="s">
         <v>7</v>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="1">
-        <v>44020</v>
+        <v>44019</v>
       </c>
       <c r="B907" t="s">
         <v>7</v>
@@ -7750,7 +7750,7 @@
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="1">
-        <v>44021</v>
+        <v>44020</v>
       </c>
       <c r="B908" t="s">
         <v>7</v>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A909" s="1">
-        <v>44022</v>
+        <v>44021</v>
       </c>
       <c r="B909" t="s">
         <v>7</v>
@@ -7766,7 +7766,7 @@
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="1">
-        <v>44023</v>
+        <v>44022</v>
       </c>
       <c r="B910" t="s">
         <v>7</v>
@@ -7774,7 +7774,7 @@
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="1">
-        <v>44024</v>
+        <v>44023</v>
       </c>
       <c r="B911" t="s">
         <v>7</v>
@@ -7782,7 +7782,7 @@
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="1">
-        <v>44025</v>
+        <v>44024</v>
       </c>
       <c r="B912" t="s">
         <v>7</v>
@@ -7790,7 +7790,7 @@
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="1">
-        <v>44026</v>
+        <v>44025</v>
       </c>
       <c r="B913" t="s">
         <v>7</v>
@@ -7798,7 +7798,7 @@
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A914" s="1">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B914" t="s">
         <v>7</v>
@@ -7806,7 +7806,7 @@
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="1">
-        <v>44028</v>
+        <v>44027</v>
       </c>
       <c r="B915" t="s">
         <v>7</v>
@@ -7814,7 +7814,7 @@
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="1">
-        <v>44029</v>
+        <v>44028</v>
       </c>
       <c r="B916" t="s">
         <v>7</v>
@@ -7822,7 +7822,7 @@
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="1">
-        <v>44030</v>
+        <v>44029</v>
       </c>
       <c r="B917" t="s">
         <v>7</v>
@@ -7830,7 +7830,7 @@
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="1">
-        <v>44031</v>
+        <v>44030</v>
       </c>
       <c r="B918" t="s">
         <v>7</v>
@@ -7838,7 +7838,7 @@
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A919" s="1">
-        <v>44032</v>
+        <v>44031</v>
       </c>
       <c r="B919" t="s">
         <v>7</v>
@@ -7846,7 +7846,7 @@
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="1">
-        <v>44033</v>
+        <v>44032</v>
       </c>
       <c r="B920" t="s">
         <v>7</v>
@@ -7854,7 +7854,7 @@
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="1">
-        <v>44034</v>
+        <v>44033</v>
       </c>
       <c r="B921" t="s">
         <v>7</v>
@@ -7862,7 +7862,7 @@
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="1">
-        <v>44035</v>
+        <v>44034</v>
       </c>
       <c r="B922" t="s">
         <v>7</v>
@@ -7870,7 +7870,7 @@
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="1">
-        <v>44036</v>
+        <v>44035</v>
       </c>
       <c r="B923" t="s">
         <v>7</v>
@@ -7878,7 +7878,7 @@
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="1">
-        <v>44037</v>
+        <v>44036</v>
       </c>
       <c r="B924" t="s">
         <v>7</v>
@@ -7886,7 +7886,7 @@
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="1">
-        <v>44038</v>
+        <v>44037</v>
       </c>
       <c r="B925" t="s">
         <v>7</v>
@@ -7894,7 +7894,7 @@
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="1">
-        <v>44039</v>
+        <v>44038</v>
       </c>
       <c r="B926" t="s">
         <v>7</v>
@@ -7902,7 +7902,7 @@
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="1">
-        <v>44040</v>
+        <v>44039</v>
       </c>
       <c r="B927" t="s">
         <v>7</v>
@@ -7910,7 +7910,7 @@
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="1">
-        <v>44041</v>
+        <v>44040</v>
       </c>
       <c r="B928" t="s">
         <v>7</v>
@@ -7918,7 +7918,7 @@
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="1">
-        <v>44042</v>
+        <v>44041</v>
       </c>
       <c r="B929" t="s">
         <v>7</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="1">
-        <v>44043</v>
+        <v>44042</v>
       </c>
       <c r="B930" t="s">
         <v>7</v>
@@ -7934,7 +7934,7 @@
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="1">
-        <v>44372</v>
+        <v>44043</v>
       </c>
       <c r="B931" t="s">
         <v>7</v>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="1">
-        <v>44373</v>
+        <v>44372</v>
       </c>
       <c r="B932" t="s">
         <v>7</v>
@@ -7950,7 +7950,7 @@
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A933" s="1">
-        <v>44374</v>
+        <v>44373</v>
       </c>
       <c r="B933" t="s">
         <v>7</v>
@@ -7958,7 +7958,7 @@
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="1">
-        <v>44375</v>
+        <v>44374</v>
       </c>
       <c r="B934" t="s">
         <v>7</v>
@@ -7966,7 +7966,7 @@
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="1">
-        <v>44376</v>
+        <v>44375</v>
       </c>
       <c r="B935" t="s">
         <v>7</v>
@@ -7974,7 +7974,7 @@
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="1">
-        <v>44377</v>
+        <v>44376</v>
       </c>
       <c r="B936" t="s">
         <v>7</v>
@@ -7982,7 +7982,7 @@
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="1">
-        <v>44378</v>
+        <v>44377</v>
       </c>
       <c r="B937" t="s">
         <v>7</v>
@@ -7990,7 +7990,7 @@
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A938" s="1">
-        <v>44379</v>
+        <v>44378</v>
       </c>
       <c r="B938" t="s">
         <v>7</v>
@@ -7998,7 +7998,7 @@
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="1">
-        <v>44380</v>
+        <v>44379</v>
       </c>
       <c r="B939" t="s">
         <v>7</v>
@@ -8006,7 +8006,7 @@
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="1">
-        <v>44381</v>
+        <v>44380</v>
       </c>
       <c r="B940" t="s">
         <v>7</v>
@@ -8014,7 +8014,7 @@
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="1">
-        <v>44382</v>
+        <v>44381</v>
       </c>
       <c r="B941" t="s">
         <v>7</v>
@@ -8022,7 +8022,7 @@
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="1">
-        <v>44383</v>
+        <v>44382</v>
       </c>
       <c r="B942" t="s">
         <v>7</v>
@@ -8030,7 +8030,7 @@
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="1">
-        <v>44384</v>
+        <v>44383</v>
       </c>
       <c r="B943" t="s">
         <v>7</v>
@@ -8038,7 +8038,7 @@
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="1">
-        <v>44385</v>
+        <v>44384</v>
       </c>
       <c r="B944" t="s">
         <v>7</v>
@@ -8046,7 +8046,7 @@
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="1">
-        <v>44386</v>
+        <v>44385</v>
       </c>
       <c r="B945" t="s">
         <v>7</v>
@@ -8054,7 +8054,7 @@
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="1">
-        <v>44387</v>
+        <v>44386</v>
       </c>
       <c r="B946" t="s">
         <v>7</v>
@@ -8062,7 +8062,7 @@
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="1">
-        <v>44388</v>
+        <v>44387</v>
       </c>
       <c r="B947" t="s">
         <v>7</v>
@@ -8070,7 +8070,7 @@
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="1">
-        <v>44389</v>
+        <v>44388</v>
       </c>
       <c r="B948" t="s">
         <v>7</v>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="1">
-        <v>44390</v>
+        <v>44389</v>
       </c>
       <c r="B949" t="s">
         <v>7</v>
@@ -8086,7 +8086,7 @@
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A950" s="1">
-        <v>44391</v>
+        <v>44390</v>
       </c>
       <c r="B950" t="s">
         <v>7</v>
@@ -8094,7 +8094,7 @@
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A951" s="1">
-        <v>44392</v>
+        <v>44391</v>
       </c>
       <c r="B951" t="s">
         <v>7</v>
@@ -8102,7 +8102,7 @@
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A952" s="1">
-        <v>44393</v>
+        <v>44392</v>
       </c>
       <c r="B952" t="s">
         <v>7</v>
@@ -8110,7 +8110,7 @@
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A953" s="1">
-        <v>44394</v>
+        <v>44393</v>
       </c>
       <c r="B953" t="s">
         <v>7</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A954" s="1">
-        <v>44395</v>
+        <v>44394</v>
       </c>
       <c r="B954" t="s">
         <v>7</v>
@@ -8126,7 +8126,7 @@
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A955" s="1">
-        <v>44396</v>
+        <v>44395</v>
       </c>
       <c r="B955" t="s">
         <v>7</v>
@@ -8134,7 +8134,7 @@
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A956" s="1">
-        <v>44397</v>
+        <v>44396</v>
       </c>
       <c r="B956" t="s">
         <v>7</v>
@@ -8142,7 +8142,7 @@
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A957" s="1">
-        <v>44398</v>
+        <v>44397</v>
       </c>
       <c r="B957" t="s">
         <v>7</v>
@@ -8150,7 +8150,7 @@
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A958" s="1">
-        <v>44399</v>
+        <v>44398</v>
       </c>
       <c r="B958" t="s">
         <v>7</v>
@@ -8158,7 +8158,7 @@
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A959" s="1">
-        <v>44400</v>
+        <v>44399</v>
       </c>
       <c r="B959" t="s">
         <v>7</v>
@@ -8166,7 +8166,7 @@
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A960" s="1">
-        <v>44401</v>
+        <v>44400</v>
       </c>
       <c r="B960" t="s">
         <v>7</v>
@@ -8174,7 +8174,7 @@
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A961" s="1">
-        <v>44402</v>
+        <v>44401</v>
       </c>
       <c r="B961" t="s">
         <v>7</v>
@@ -8182,7 +8182,7 @@
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A962" s="1">
-        <v>44403</v>
+        <v>44402</v>
       </c>
       <c r="B962" t="s">
         <v>7</v>
@@ -8190,7 +8190,7 @@
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A963" s="1">
-        <v>44404</v>
+        <v>44403</v>
       </c>
       <c r="B963" t="s">
         <v>7</v>
@@ -8198,7 +8198,7 @@
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A964" s="1">
-        <v>44405</v>
+        <v>44404</v>
       </c>
       <c r="B964" t="s">
         <v>7</v>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A965" s="1">
-        <v>44406</v>
+        <v>44405</v>
       </c>
       <c r="B965" t="s">
         <v>7</v>
@@ -8214,7 +8214,7 @@
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A966" s="1">
-        <v>44407</v>
+        <v>44406</v>
       </c>
       <c r="B966" t="s">
         <v>7</v>
@@ -8222,7 +8222,7 @@
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A967" s="1">
-        <v>44408</v>
+        <v>44407</v>
       </c>
       <c r="B967" t="s">
         <v>7</v>
@@ -8230,15 +8230,15 @@
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A968" s="1">
-        <v>43848</v>
+        <v>44408</v>
       </c>
       <c r="B968" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A969" s="1">
-        <v>43849</v>
+        <v>43848</v>
       </c>
       <c r="B969" t="s">
         <v>5</v>
@@ -8246,7 +8246,7 @@
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A970" s="1">
-        <v>43850</v>
+        <v>43849</v>
       </c>
       <c r="B970" t="s">
         <v>5</v>
@@ -8254,7 +8254,7 @@
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A971" s="1">
-        <v>43851</v>
+        <v>43850</v>
       </c>
       <c r="B971" t="s">
         <v>5</v>
@@ -8262,7 +8262,7 @@
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A972" s="1">
-        <v>43852</v>
+        <v>43851</v>
       </c>
       <c r="B972" t="s">
         <v>5</v>
@@ -8270,7 +8270,7 @@
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A973" s="1">
-        <v>43853</v>
+        <v>43852</v>
       </c>
       <c r="B973" t="s">
         <v>5</v>
@@ -8278,7 +8278,7 @@
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="1">
-        <v>43855</v>
+        <v>43853</v>
       </c>
       <c r="B974" t="s">
         <v>5</v>
@@ -8286,7 +8286,7 @@
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="1">
-        <v>43856</v>
+        <v>43855</v>
       </c>
       <c r="B975" t="s">
         <v>5</v>
@@ -8294,7 +8294,7 @@
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="1">
-        <v>43857</v>
+        <v>43856</v>
       </c>
       <c r="B976" t="s">
         <v>5</v>
@@ -8302,7 +8302,7 @@
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="1">
-        <v>43858</v>
+        <v>43857</v>
       </c>
       <c r="B977" t="s">
         <v>5</v>
@@ -8310,7 +8310,7 @@
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="1">
-        <v>43859</v>
+        <v>43858</v>
       </c>
       <c r="B978" t="s">
         <v>5</v>
@@ -8318,7 +8318,7 @@
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="1">
-        <v>43860</v>
+        <v>43859</v>
       </c>
       <c r="B979" t="s">
         <v>5</v>
@@ -8326,7 +8326,7 @@
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="1">
-        <v>43861</v>
+        <v>43860</v>
       </c>
       <c r="B980" t="s">
         <v>5</v>
@@ -8334,7 +8334,7 @@
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="1">
-        <v>43862</v>
+        <v>43861</v>
       </c>
       <c r="B981" t="s">
         <v>5</v>
@@ -8342,7 +8342,7 @@
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A982" s="1">
-        <v>43863</v>
+        <v>43862</v>
       </c>
       <c r="B982" t="s">
         <v>5</v>
@@ -8350,7 +8350,7 @@
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="1">
-        <v>43864</v>
+        <v>43863</v>
       </c>
       <c r="B983" t="s">
         <v>5</v>
@@ -8358,7 +8358,7 @@
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="1">
-        <v>44232</v>
+        <v>43864</v>
       </c>
       <c r="B984" t="s">
         <v>5</v>
@@ -8366,7 +8366,7 @@
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A985" s="1">
-        <v>44233</v>
+        <v>44232</v>
       </c>
       <c r="B985" t="s">
         <v>5</v>
@@ -8374,7 +8374,7 @@
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="1">
-        <v>44234</v>
+        <v>44233</v>
       </c>
       <c r="B986" t="s">
         <v>5</v>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="1">
-        <v>44235</v>
+        <v>44234</v>
       </c>
       <c r="B987" t="s">
         <v>5</v>
@@ -8390,7 +8390,7 @@
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="1">
-        <v>44236</v>
+        <v>44235</v>
       </c>
       <c r="B988" t="s">
         <v>5</v>
@@ -8398,7 +8398,7 @@
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="1">
-        <v>44237</v>
+        <v>44236</v>
       </c>
       <c r="B989" t="s">
         <v>5</v>
@@ -8406,7 +8406,7 @@
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A990" s="1">
-        <v>44239</v>
+        <v>44237</v>
       </c>
       <c r="B990" t="s">
         <v>5</v>
@@ -8414,7 +8414,7 @@
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="1">
-        <v>44240</v>
+        <v>44239</v>
       </c>
       <c r="B991" t="s">
         <v>5</v>
@@ -8422,7 +8422,7 @@
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="1">
-        <v>44241</v>
+        <v>44240</v>
       </c>
       <c r="B992" t="s">
         <v>5</v>
@@ -8430,7 +8430,7 @@
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="1">
-        <v>44242</v>
+        <v>44241</v>
       </c>
       <c r="B993" t="s">
         <v>5</v>
@@ -8438,7 +8438,7 @@
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="1">
-        <v>44243</v>
+        <v>44242</v>
       </c>
       <c r="B994" t="s">
         <v>5</v>
@@ -8446,7 +8446,7 @@
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="1">
-        <v>44244</v>
+        <v>44243</v>
       </c>
       <c r="B995" t="s">
         <v>5</v>
@@ -8454,7 +8454,7 @@
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="1">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="B996" t="s">
         <v>5</v>
@@ -8462,7 +8462,7 @@
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="1">
-        <v>44246</v>
+        <v>44245</v>
       </c>
       <c r="B997" t="s">
         <v>5</v>
@@ -8470,7 +8470,7 @@
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A998" s="1">
-        <v>44247</v>
+        <v>44246</v>
       </c>
       <c r="B998" t="s">
         <v>5</v>
@@ -8478,13 +8478,22 @@
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A999" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B999" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1000" s="1">
         <v>44248</v>
       </c>
-      <c r="B999" t="s">
+      <c r="B1000" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1000" xr:uid="{DD25DBC2-16DB-4102-94CC-D4FC79081A1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjust holidays and update Mar23
</commit_message>
<xml_diff>
--- a/holidays.xlsx
+++ b/holidays.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namtrantuan\Desktop\passenger_forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11302D09-C452-4E68-B13E-9FAE56233BC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BB62BE-80D0-468C-BA50-C732083932B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C81195CF-3238-4C84-B228-279AE06B6B57}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="covid" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">covid!$A$1:$B$999</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">covid!$A$1:$B$997</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="9">
   <si>
     <t>covid_1</t>
   </si>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9708BE-FF7E-456D-97C7-E4E782A5149C}">
-  <dimension ref="A1:B999"/>
+  <dimension ref="A1:B997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A484" sqref="A484"/>
+      <selection activeCell="B478" sqref="B478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4405,7 +4405,7 @@
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A499" s="1">
-        <v>44593</v>
+        <v>44594</v>
       </c>
       <c r="B499" t="s">
         <v>5</v>
@@ -4413,7 +4413,7 @@
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A500" s="1">
-        <v>44594</v>
+        <v>44595</v>
       </c>
       <c r="B500" t="s">
         <v>5</v>
@@ -4421,7 +4421,7 @@
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A501" s="1">
-        <v>44595</v>
+        <v>44596</v>
       </c>
       <c r="B501" t="s">
         <v>5</v>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A502" s="1">
-        <v>44596</v>
+        <v>44597</v>
       </c>
       <c r="B502" t="s">
         <v>5</v>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A503" s="1">
-        <v>44597</v>
+        <v>44598</v>
       </c>
       <c r="B503" t="s">
         <v>5</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A504" s="1">
-        <v>44598</v>
+        <v>44599</v>
       </c>
       <c r="B504" t="s">
         <v>5</v>
@@ -4453,7 +4453,7 @@
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A505" s="1">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="B505" t="s">
         <v>5</v>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A506" s="1">
-        <v>44600</v>
+        <v>44601</v>
       </c>
       <c r="B506" t="s">
         <v>5</v>
@@ -4469,7 +4469,7 @@
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A507" s="1">
-        <v>44601</v>
+        <v>44602</v>
       </c>
       <c r="B507" t="s">
         <v>5</v>
@@ -4477,7 +4477,7 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A508" s="1">
-        <v>44602</v>
+        <v>42047</v>
       </c>
       <c r="B508" t="s">
         <v>5</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A509" s="1">
-        <v>42047</v>
+        <v>42048</v>
       </c>
       <c r="B509" t="s">
         <v>5</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" s="1">
-        <v>42048</v>
+        <v>42049</v>
       </c>
       <c r="B510" t="s">
         <v>5</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" s="1">
-        <v>42049</v>
+        <v>42050</v>
       </c>
       <c r="B511" t="s">
         <v>5</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A512" s="1">
-        <v>42050</v>
+        <v>42051</v>
       </c>
       <c r="B512" t="s">
         <v>5</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A513" s="1">
-        <v>42051</v>
+        <v>42052</v>
       </c>
       <c r="B513" t="s">
         <v>5</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A514" s="1">
-        <v>42052</v>
+        <v>42055</v>
       </c>
       <c r="B514" t="s">
         <v>5</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A515" s="1">
-        <v>42055</v>
+        <v>42056</v>
       </c>
       <c r="B515" t="s">
         <v>5</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A516" s="1">
-        <v>42056</v>
+        <v>42057</v>
       </c>
       <c r="B516" t="s">
         <v>5</v>
@@ -4549,7 +4549,7 @@
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A517" s="1">
-        <v>42057</v>
+        <v>42058</v>
       </c>
       <c r="B517" t="s">
         <v>5</v>
@@ -4557,7 +4557,7 @@
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A518" s="1">
-        <v>42058</v>
+        <v>42059</v>
       </c>
       <c r="B518" t="s">
         <v>5</v>
@@ -4565,7 +4565,7 @@
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A519" s="1">
-        <v>42059</v>
+        <v>42060</v>
       </c>
       <c r="B519" t="s">
         <v>5</v>
@@ -4573,7 +4573,7 @@
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A520" s="1">
-        <v>42060</v>
+        <v>42061</v>
       </c>
       <c r="B520" t="s">
         <v>5</v>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A521" s="1">
-        <v>42061</v>
+        <v>42062</v>
       </c>
       <c r="B521" t="s">
         <v>5</v>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A522" s="1">
-        <v>42062</v>
+        <v>42063</v>
       </c>
       <c r="B522" t="s">
         <v>5</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A523" s="1">
-        <v>42063</v>
+        <v>42064</v>
       </c>
       <c r="B523" t="s">
         <v>5</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A524" s="1">
-        <v>42064</v>
+        <v>42065</v>
       </c>
       <c r="B524" t="s">
         <v>5</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A525" s="1">
-        <v>42065</v>
+        <v>42402</v>
       </c>
       <c r="B525" t="s">
         <v>5</v>
@@ -4621,7 +4621,7 @@
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A526" s="1">
-        <v>42402</v>
+        <v>42403</v>
       </c>
       <c r="B526" t="s">
         <v>5</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A527" s="1">
-        <v>42403</v>
+        <v>42404</v>
       </c>
       <c r="B527" t="s">
         <v>5</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A528" s="1">
-        <v>42404</v>
+        <v>42405</v>
       </c>
       <c r="B528" t="s">
         <v>5</v>
@@ -4645,7 +4645,7 @@
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A529" s="1">
-        <v>42405</v>
+        <v>42406</v>
       </c>
       <c r="B529" t="s">
         <v>5</v>
@@ -4653,7 +4653,7 @@
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A530" s="1">
-        <v>42406</v>
+        <v>42409</v>
       </c>
       <c r="B530" t="s">
         <v>5</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A531" s="1">
-        <v>42409</v>
+        <v>42410</v>
       </c>
       <c r="B531" t="s">
         <v>5</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A532" s="1">
-        <v>42410</v>
+        <v>42411</v>
       </c>
       <c r="B532" t="s">
         <v>5</v>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A533" s="1">
-        <v>42411</v>
+        <v>42412</v>
       </c>
       <c r="B533" t="s">
         <v>5</v>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A534" s="1">
-        <v>42412</v>
+        <v>42413</v>
       </c>
       <c r="B534" t="s">
         <v>5</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A535" s="1">
-        <v>42413</v>
+        <v>42414</v>
       </c>
       <c r="B535" t="s">
         <v>5</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A536" s="1">
-        <v>42414</v>
+        <v>42415</v>
       </c>
       <c r="B536" t="s">
         <v>5</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A537" s="1">
-        <v>42415</v>
+        <v>42416</v>
       </c>
       <c r="B537" t="s">
         <v>5</v>
@@ -4717,7 +4717,7 @@
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A538" s="1">
-        <v>42416</v>
+        <v>42756</v>
       </c>
       <c r="B538" t="s">
         <v>5</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A539" s="1">
-        <v>42756</v>
+        <v>42757</v>
       </c>
       <c r="B539" t="s">
         <v>5</v>
@@ -4733,7 +4733,7 @@
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A540" s="1">
-        <v>42757</v>
+        <v>42758</v>
       </c>
       <c r="B540" t="s">
         <v>5</v>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A541" s="1">
-        <v>42758</v>
+        <v>42759</v>
       </c>
       <c r="B541" t="s">
         <v>5</v>
@@ -4749,7 +4749,7 @@
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A542" s="1">
-        <v>42759</v>
+        <v>42760</v>
       </c>
       <c r="B542" t="s">
         <v>5</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A543" s="1">
-        <v>42760</v>
+        <v>42761</v>
       </c>
       <c r="B543" t="s">
         <v>5</v>
@@ -4765,7 +4765,7 @@
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A544" s="1">
-        <v>42761</v>
+        <v>42764</v>
       </c>
       <c r="B544" t="s">
         <v>5</v>
@@ -4773,7 +4773,7 @@
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A545" s="1">
-        <v>42764</v>
+        <v>42765</v>
       </c>
       <c r="B545" t="s">
         <v>5</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A546" s="1">
-        <v>42765</v>
+        <v>42766</v>
       </c>
       <c r="B546" t="s">
         <v>5</v>
@@ -4789,7 +4789,7 @@
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A547" s="1">
-        <v>42766</v>
+        <v>42767</v>
       </c>
       <c r="B547" t="s">
         <v>5</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A548" s="1">
-        <v>42767</v>
+        <v>42768</v>
       </c>
       <c r="B548" t="s">
         <v>5</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A549" s="1">
-        <v>42768</v>
+        <v>42769</v>
       </c>
       <c r="B549" t="s">
         <v>5</v>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A550" s="1">
-        <v>42769</v>
+        <v>42770</v>
       </c>
       <c r="B550" t="s">
         <v>5</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A551" s="1">
-        <v>42770</v>
+        <v>42771</v>
       </c>
       <c r="B551" t="s">
         <v>5</v>
@@ -4829,7 +4829,7 @@
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A552" s="1">
-        <v>42771</v>
+        <v>42772</v>
       </c>
       <c r="B552" t="s">
         <v>5</v>
@@ -4837,7 +4837,7 @@
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A553" s="1">
-        <v>42772</v>
+        <v>43140</v>
       </c>
       <c r="B553" t="s">
         <v>5</v>
@@ -4845,7 +4845,8 @@
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A554" s="1">
-        <v>43140</v>
+        <f>A553+1</f>
+        <v>43141</v>
       </c>
       <c r="B554" t="s">
         <v>5</v>
@@ -4853,8 +4854,8 @@
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A555" s="1">
-        <f>A554+1</f>
-        <v>43141</v>
+        <f t="shared" ref="A555:A570" si="0">A554+1</f>
+        <v>43142</v>
       </c>
       <c r="B555" t="s">
         <v>5</v>
@@ -4862,8 +4863,8 @@
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A556" s="1">
-        <f t="shared" ref="A556:A571" si="0">A555+1</f>
-        <v>43142</v>
+        <f t="shared" si="0"/>
+        <v>43143</v>
       </c>
       <c r="B556" t="s">
         <v>5</v>
@@ -4872,7 +4873,7 @@
     <row r="557" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A557" s="1">
         <f t="shared" si="0"/>
-        <v>43143</v>
+        <v>43144</v>
       </c>
       <c r="B557" t="s">
         <v>5</v>
@@ -4881,7 +4882,7 @@
     <row r="558" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A558" s="1">
         <f t="shared" si="0"/>
-        <v>43144</v>
+        <v>43145</v>
       </c>
       <c r="B558" t="s">
         <v>5</v>
@@ -4889,8 +4890,7 @@
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A559" s="1">
-        <f t="shared" si="0"/>
-        <v>43145</v>
+        <v>43148</v>
       </c>
       <c r="B559" t="s">
         <v>5</v>
@@ -4898,7 +4898,8 @@
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A560" s="1">
-        <v>43148</v>
+        <f t="shared" si="0"/>
+        <v>43149</v>
       </c>
       <c r="B560" t="s">
         <v>5</v>
@@ -4907,7 +4908,7 @@
     <row r="561" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A561" s="1">
         <f t="shared" si="0"/>
-        <v>43149</v>
+        <v>43150</v>
       </c>
       <c r="B561" t="s">
         <v>5</v>
@@ -4916,7 +4917,7 @@
     <row r="562" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A562" s="1">
         <f t="shared" si="0"/>
-        <v>43150</v>
+        <v>43151</v>
       </c>
       <c r="B562" t="s">
         <v>5</v>
@@ -4925,7 +4926,7 @@
     <row r="563" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A563" s="1">
         <f t="shared" si="0"/>
-        <v>43151</v>
+        <v>43152</v>
       </c>
       <c r="B563" t="s">
         <v>5</v>
@@ -4934,7 +4935,7 @@
     <row r="564" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A564" s="1">
         <f t="shared" si="0"/>
-        <v>43152</v>
+        <v>43153</v>
       </c>
       <c r="B564" t="s">
         <v>5</v>
@@ -4943,7 +4944,7 @@
     <row r="565" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A565" s="1">
         <f t="shared" si="0"/>
-        <v>43153</v>
+        <v>43154</v>
       </c>
       <c r="B565" t="s">
         <v>5</v>
@@ -4952,7 +4953,7 @@
     <row r="566" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A566" s="1">
         <f t="shared" si="0"/>
-        <v>43154</v>
+        <v>43155</v>
       </c>
       <c r="B566" t="s">
         <v>5</v>
@@ -4961,7 +4962,7 @@
     <row r="567" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A567" s="1">
         <f t="shared" si="0"/>
-        <v>43155</v>
+        <v>43156</v>
       </c>
       <c r="B567" t="s">
         <v>5</v>
@@ -4970,7 +4971,7 @@
     <row r="568" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A568" s="1">
         <f t="shared" si="0"/>
-        <v>43156</v>
+        <v>43157</v>
       </c>
       <c r="B568" t="s">
         <v>5</v>
@@ -4979,7 +4980,7 @@
     <row r="569" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A569" s="1">
         <f t="shared" si="0"/>
-        <v>43157</v>
+        <v>43158</v>
       </c>
       <c r="B569" t="s">
         <v>5</v>
@@ -4988,7 +4989,7 @@
     <row r="570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A570" s="1">
         <f t="shared" si="0"/>
-        <v>43158</v>
+        <v>43159</v>
       </c>
       <c r="B570" t="s">
         <v>5</v>
@@ -4996,8 +4997,7 @@
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A571" s="1">
-        <f t="shared" si="0"/>
-        <v>43159</v>
+        <v>43494</v>
       </c>
       <c r="B571" t="s">
         <v>5</v>
@@ -5005,7 +5005,7 @@
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A572" s="1">
-        <v>43494</v>
+        <v>43495</v>
       </c>
       <c r="B572" t="s">
         <v>5</v>
@@ -5013,7 +5013,7 @@
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A573" s="1">
-        <v>43495</v>
+        <v>43496</v>
       </c>
       <c r="B573" t="s">
         <v>5</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A574" s="1">
-        <v>43496</v>
+        <v>43497</v>
       </c>
       <c r="B574" t="s">
         <v>5</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A575" s="1">
-        <v>43497</v>
+        <v>43498</v>
       </c>
       <c r="B575" t="s">
         <v>5</v>
@@ -5037,7 +5037,7 @@
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A576" s="1">
-        <v>43498</v>
+        <v>43499</v>
       </c>
       <c r="B576" t="s">
         <v>5</v>
@@ -5045,7 +5045,7 @@
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A577" s="1">
-        <v>43499</v>
+        <v>43502</v>
       </c>
       <c r="B577" t="s">
         <v>5</v>
@@ -5053,7 +5053,7 @@
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A578" s="1">
-        <v>43500</v>
+        <v>43503</v>
       </c>
       <c r="B578" t="s">
         <v>5</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A579" s="1">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="B579" t="s">
         <v>5</v>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A580" s="1">
-        <v>43503</v>
+        <v>43505</v>
       </c>
       <c r="B580" t="s">
         <v>5</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A581" s="1">
-        <v>43504</v>
+        <v>43506</v>
       </c>
       <c r="B581" t="s">
         <v>5</v>
@@ -5085,7 +5085,7 @@
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A582" s="1">
-        <v>43505</v>
+        <v>43507</v>
       </c>
       <c r="B582" t="s">
         <v>5</v>
@@ -5093,7 +5093,7 @@
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A583" s="1">
-        <v>43506</v>
+        <v>43508</v>
       </c>
       <c r="B583" t="s">
         <v>5</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A584" s="1">
-        <v>43507</v>
+        <v>43509</v>
       </c>
       <c r="B584" t="s">
         <v>5</v>
@@ -5109,7 +5109,7 @@
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A585" s="1">
-        <v>43508</v>
+        <v>43510</v>
       </c>
       <c r="B585" t="s">
         <v>5</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A586" s="1">
-        <v>43509</v>
+        <v>43511</v>
       </c>
       <c r="B586" t="s">
         <v>5</v>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A587" s="1">
-        <v>43510</v>
+        <v>43512</v>
       </c>
       <c r="B587" t="s">
         <v>5</v>
@@ -5133,24 +5133,26 @@
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A588" s="1">
-        <v>43511</v>
+        <f t="shared" ref="A588:A592" si="1">A589-1</f>
+        <v>42118</v>
       </c>
       <c r="B588" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A589" s="1">
-        <v>43512</v>
+        <f t="shared" si="1"/>
+        <v>42119</v>
       </c>
       <c r="B589" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A590" s="1">
-        <f t="shared" ref="A590:A594" si="1">A591-1</f>
-        <v>42118</v>
+        <f t="shared" si="1"/>
+        <v>42120</v>
       </c>
       <c r="B590" t="s">
         <v>6</v>
@@ -5159,7 +5161,7 @@
     <row r="591" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A591" s="1">
         <f t="shared" si="1"/>
-        <v>42119</v>
+        <v>42121</v>
       </c>
       <c r="B591" t="s">
         <v>6</v>
@@ -5168,7 +5170,7 @@
     <row r="592" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A592" s="1">
         <f t="shared" si="1"/>
-        <v>42120</v>
+        <v>42122</v>
       </c>
       <c r="B592" t="s">
         <v>6</v>
@@ -5176,8 +5178,8 @@
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A593" s="1">
-        <f t="shared" si="1"/>
-        <v>42121</v>
+        <f>A594-1</f>
+        <v>42123</v>
       </c>
       <c r="B593" t="s">
         <v>6</v>
@@ -5185,8 +5187,7 @@
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A594" s="1">
-        <f t="shared" si="1"/>
-        <v>42122</v>
+        <v>42124</v>
       </c>
       <c r="B594" t="s">
         <v>6</v>
@@ -5194,8 +5195,8 @@
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A595" s="1">
-        <f>A596-1</f>
-        <v>42123</v>
+        <f>A594+1</f>
+        <v>42125</v>
       </c>
       <c r="B595" t="s">
         <v>6</v>
@@ -5203,7 +5204,8 @@
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A596" s="1">
-        <v>42124</v>
+        <f t="shared" ref="A596:A598" si="2">A595+1</f>
+        <v>42126</v>
       </c>
       <c r="B596" t="s">
         <v>6</v>
@@ -5211,8 +5213,8 @@
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A597" s="1">
-        <f>A596+1</f>
-        <v>42125</v>
+        <f t="shared" si="2"/>
+        <v>42127</v>
       </c>
       <c r="B597" t="s">
         <v>6</v>
@@ -5220,8 +5222,8 @@
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A598" s="1">
-        <f t="shared" ref="A598:A600" si="2">A597+1</f>
-        <v>42126</v>
+        <f t="shared" si="2"/>
+        <v>42128</v>
       </c>
       <c r="B598" t="s">
         <v>6</v>
@@ -5229,8 +5231,8 @@
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A599" s="1">
-        <f t="shared" si="2"/>
-        <v>42127</v>
+        <f t="shared" ref="A599:A607" si="3">A600-1</f>
+        <v>42484</v>
       </c>
       <c r="B599" t="s">
         <v>6</v>
@@ -5238,8 +5240,8 @@
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A600" s="1">
-        <f t="shared" si="2"/>
-        <v>42128</v>
+        <f t="shared" si="3"/>
+        <v>42485</v>
       </c>
       <c r="B600" t="s">
         <v>6</v>
@@ -5247,8 +5249,8 @@
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" s="1">
-        <f t="shared" ref="A601:A609" si="3">A602-1</f>
-        <v>42484</v>
+        <f t="shared" si="3"/>
+        <v>42486</v>
       </c>
       <c r="B601" t="s">
         <v>6</v>
@@ -5257,7 +5259,7 @@
     <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A602" s="1">
         <f t="shared" si="3"/>
-        <v>42485</v>
+        <v>42487</v>
       </c>
       <c r="B602" t="s">
         <v>6</v>
@@ -5266,7 +5268,7 @@
     <row r="603" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A603" s="1">
         <f t="shared" si="3"/>
-        <v>42486</v>
+        <v>42488</v>
       </c>
       <c r="B603" t="s">
         <v>6</v>
@@ -5275,7 +5277,7 @@
     <row r="604" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A604" s="1">
         <f t="shared" si="3"/>
-        <v>42487</v>
+        <v>42489</v>
       </c>
       <c r="B604" t="s">
         <v>6</v>
@@ -5284,7 +5286,7 @@
     <row r="605" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A605" s="1">
         <f t="shared" si="3"/>
-        <v>42488</v>
+        <v>42490</v>
       </c>
       <c r="B605" t="s">
         <v>6</v>
@@ -5293,7 +5295,7 @@
     <row r="606" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A606" s="1">
         <f t="shared" si="3"/>
-        <v>42489</v>
+        <v>42491</v>
       </c>
       <c r="B606" t="s">
         <v>6</v>
@@ -5302,7 +5304,7 @@
     <row r="607" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A607" s="1">
         <f t="shared" si="3"/>
-        <v>42490</v>
+        <v>42492</v>
       </c>
       <c r="B607" t="s">
         <v>6</v>
@@ -5310,8 +5312,8 @@
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A608" s="1">
-        <f t="shared" si="3"/>
-        <v>42491</v>
+        <f>A609-1</f>
+        <v>42493</v>
       </c>
       <c r="B608" t="s">
         <v>6</v>
@@ -5319,8 +5321,7 @@
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A609" s="1">
-        <f t="shared" si="3"/>
-        <v>42492</v>
+        <v>42494</v>
       </c>
       <c r="B609" t="s">
         <v>6</v>
@@ -5328,8 +5329,8 @@
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A610" s="1">
-        <f>A611-1</f>
-        <v>42493</v>
+        <f t="shared" ref="A610:A616" si="4">A611-1</f>
+        <v>42851</v>
       </c>
       <c r="B610" t="s">
         <v>6</v>
@@ -5337,7 +5338,8 @@
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A611" s="1">
-        <v>42494</v>
+        <f t="shared" si="4"/>
+        <v>42852</v>
       </c>
       <c r="B611" t="s">
         <v>6</v>
@@ -5345,8 +5347,8 @@
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A612" s="1">
-        <f t="shared" ref="A612:A618" si="4">A613-1</f>
-        <v>42851</v>
+        <f t="shared" si="4"/>
+        <v>42853</v>
       </c>
       <c r="B612" t="s">
         <v>6</v>
@@ -5355,7 +5357,7 @@
     <row r="613" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A613" s="1">
         <f t="shared" si="4"/>
-        <v>42852</v>
+        <v>42854</v>
       </c>
       <c r="B613" t="s">
         <v>6</v>
@@ -5364,7 +5366,7 @@
     <row r="614" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A614" s="1">
         <f t="shared" si="4"/>
-        <v>42853</v>
+        <v>42855</v>
       </c>
       <c r="B614" t="s">
         <v>6</v>
@@ -5373,7 +5375,7 @@
     <row r="615" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A615" s="1">
         <f t="shared" si="4"/>
-        <v>42854</v>
+        <v>42856</v>
       </c>
       <c r="B615" t="s">
         <v>6</v>
@@ -5382,7 +5384,7 @@
     <row r="616" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A616" s="1">
         <f t="shared" si="4"/>
-        <v>42855</v>
+        <v>42857</v>
       </c>
       <c r="B616" t="s">
         <v>6</v>
@@ -5390,8 +5392,8 @@
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A617" s="1">
-        <f t="shared" si="4"/>
-        <v>42856</v>
+        <f>A618-1</f>
+        <v>42858</v>
       </c>
       <c r="B617" t="s">
         <v>6</v>
@@ -5399,8 +5401,7 @@
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A618" s="1">
-        <f t="shared" si="4"/>
-        <v>42857</v>
+        <v>42859</v>
       </c>
       <c r="B618" t="s">
         <v>6</v>
@@ -5408,8 +5409,7 @@
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A619" s="1">
-        <f>A620-1</f>
-        <v>42858</v>
+        <v>43217</v>
       </c>
       <c r="B619" t="s">
         <v>6</v>
@@ -5417,7 +5417,8 @@
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A620" s="1">
-        <v>42859</v>
+        <f>A619+1</f>
+        <v>43218</v>
       </c>
       <c r="B620" t="s">
         <v>6</v>
@@ -5425,7 +5426,8 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A621" s="1">
-        <v>43217</v>
+        <f t="shared" ref="A621:A624" si="5">A620+1</f>
+        <v>43219</v>
       </c>
       <c r="B621" t="s">
         <v>6</v>
@@ -5433,8 +5435,8 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A622" s="1">
-        <f>A621+1</f>
-        <v>43218</v>
+        <f t="shared" si="5"/>
+        <v>43220</v>
       </c>
       <c r="B622" t="s">
         <v>6</v>
@@ -5442,8 +5444,8 @@
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A623" s="1">
-        <f t="shared" ref="A623:A626" si="5">A622+1</f>
-        <v>43219</v>
+        <f t="shared" si="5"/>
+        <v>43221</v>
       </c>
       <c r="B623" t="s">
         <v>6</v>
@@ -5452,7 +5454,7 @@
     <row r="624" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A624" s="1">
         <f t="shared" si="5"/>
-        <v>43220</v>
+        <v>43222</v>
       </c>
       <c r="B624" t="s">
         <v>6</v>
@@ -5460,8 +5462,7 @@
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A625" s="1">
-        <f t="shared" si="5"/>
-        <v>43221</v>
+        <v>43581</v>
       </c>
       <c r="B625" t="s">
         <v>6</v>
@@ -5469,8 +5470,8 @@
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A626" s="1">
-        <f t="shared" si="5"/>
-        <v>43222</v>
+        <f>A625+1</f>
+        <v>43582</v>
       </c>
       <c r="B626" t="s">
         <v>6</v>
@@ -5478,7 +5479,8 @@
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A627" s="1">
-        <v>43581</v>
+        <f t="shared" ref="A627:A631" si="6">A626+1</f>
+        <v>43583</v>
       </c>
       <c r="B627" t="s">
         <v>6</v>
@@ -5486,8 +5488,8 @@
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A628" s="1">
-        <f>A627+1</f>
-        <v>43582</v>
+        <f t="shared" si="6"/>
+        <v>43584</v>
       </c>
       <c r="B628" t="s">
         <v>6</v>
@@ -5495,8 +5497,8 @@
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A629" s="1">
-        <f t="shared" ref="A629:A633" si="6">A628+1</f>
-        <v>43583</v>
+        <f t="shared" si="6"/>
+        <v>43585</v>
       </c>
       <c r="B629" t="s">
         <v>6</v>
@@ -5505,7 +5507,7 @@
     <row r="630" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A630" s="1">
         <f t="shared" si="6"/>
-        <v>43584</v>
+        <v>43586</v>
       </c>
       <c r="B630" t="s">
         <v>6</v>
@@ -5514,7 +5516,7 @@
     <row r="631" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A631" s="1">
         <f t="shared" si="6"/>
-        <v>43585</v>
+        <v>43587</v>
       </c>
       <c r="B631" t="s">
         <v>6</v>
@@ -5522,8 +5524,7 @@
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A632" s="1">
-        <f t="shared" si="6"/>
-        <v>43586</v>
+        <v>45046</v>
       </c>
       <c r="B632" t="s">
         <v>6</v>
@@ -5531,8 +5532,7 @@
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A633" s="1">
-        <f t="shared" si="6"/>
-        <v>43587</v>
+        <v>45047</v>
       </c>
       <c r="B633" t="s">
         <v>6</v>
@@ -5540,23 +5540,23 @@
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A634" s="1">
-        <v>45046</v>
+        <v>42180</v>
       </c>
       <c r="B634" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A635" s="1">
-        <v>45047</v>
+        <v>42181</v>
       </c>
       <c r="B635" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A636" s="1">
-        <v>42180</v>
+        <v>42182</v>
       </c>
       <c r="B636" t="s">
         <v>7</v>
@@ -5564,7 +5564,7 @@
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A637" s="1">
-        <v>42181</v>
+        <v>42183</v>
       </c>
       <c r="B637" t="s">
         <v>7</v>
@@ -5572,7 +5572,7 @@
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A638" s="1">
-        <v>42182</v>
+        <v>42184</v>
       </c>
       <c r="B638" t="s">
         <v>7</v>
@@ -5580,7 +5580,7 @@
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A639" s="1">
-        <v>42183</v>
+        <v>42185</v>
       </c>
       <c r="B639" t="s">
         <v>7</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A640" s="1">
-        <v>42184</v>
+        <v>42186</v>
       </c>
       <c r="B640" t="s">
         <v>7</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A641" s="1">
-        <v>42185</v>
+        <v>42187</v>
       </c>
       <c r="B641" t="s">
         <v>7</v>
@@ -5604,7 +5604,7 @@
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A642" s="1">
-        <v>42186</v>
+        <v>42188</v>
       </c>
       <c r="B642" t="s">
         <v>7</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A643" s="1">
-        <v>42187</v>
+        <v>42189</v>
       </c>
       <c r="B643" t="s">
         <v>7</v>
@@ -5620,7 +5620,7 @@
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A644" s="1">
-        <v>42188</v>
+        <v>42190</v>
       </c>
       <c r="B644" t="s">
         <v>7</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A645" s="1">
-        <v>42189</v>
+        <v>42191</v>
       </c>
       <c r="B645" t="s">
         <v>7</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A646" s="1">
-        <v>42190</v>
+        <v>42192</v>
       </c>
       <c r="B646" t="s">
         <v>7</v>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A647" s="1">
-        <v>42191</v>
+        <v>42193</v>
       </c>
       <c r="B647" t="s">
         <v>7</v>
@@ -5652,7 +5652,7 @@
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A648" s="1">
-        <v>42192</v>
+        <v>42194</v>
       </c>
       <c r="B648" t="s">
         <v>7</v>
@@ -5660,7 +5660,7 @@
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A649" s="1">
-        <v>42193</v>
+        <v>42195</v>
       </c>
       <c r="B649" t="s">
         <v>7</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A650" s="1">
-        <v>42194</v>
+        <v>42196</v>
       </c>
       <c r="B650" t="s">
         <v>7</v>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A651" s="1">
-        <v>42195</v>
+        <v>42197</v>
       </c>
       <c r="B651" t="s">
         <v>7</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A652" s="1">
-        <v>42196</v>
+        <v>42198</v>
       </c>
       <c r="B652" t="s">
         <v>7</v>
@@ -5692,7 +5692,7 @@
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A653" s="1">
-        <v>42197</v>
+        <v>42199</v>
       </c>
       <c r="B653" t="s">
         <v>7</v>
@@ -5700,7 +5700,7 @@
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A654" s="1">
-        <v>42198</v>
+        <v>42200</v>
       </c>
       <c r="B654" t="s">
         <v>7</v>
@@ -5708,7 +5708,7 @@
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A655" s="1">
-        <v>42199</v>
+        <v>42201</v>
       </c>
       <c r="B655" t="s">
         <v>7</v>
@@ -5716,7 +5716,7 @@
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A656" s="1">
-        <v>42200</v>
+        <v>42202</v>
       </c>
       <c r="B656" t="s">
         <v>7</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A657" s="1">
-        <v>42201</v>
+        <v>42203</v>
       </c>
       <c r="B657" t="s">
         <v>7</v>
@@ -5732,7 +5732,7 @@
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A658" s="1">
-        <v>42202</v>
+        <v>42204</v>
       </c>
       <c r="B658" t="s">
         <v>7</v>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A659" s="1">
-        <v>42203</v>
+        <v>42205</v>
       </c>
       <c r="B659" t="s">
         <v>7</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A660" s="1">
-        <v>42204</v>
+        <v>42206</v>
       </c>
       <c r="B660" t="s">
         <v>7</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A661" s="1">
-        <v>42205</v>
+        <v>42207</v>
       </c>
       <c r="B661" t="s">
         <v>7</v>
@@ -5764,7 +5764,7 @@
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A662" s="1">
-        <v>42206</v>
+        <v>42208</v>
       </c>
       <c r="B662" t="s">
         <v>7</v>
@@ -5772,7 +5772,7 @@
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A663" s="1">
-        <v>42207</v>
+        <v>42209</v>
       </c>
       <c r="B663" t="s">
         <v>7</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A664" s="1">
-        <v>42208</v>
+        <v>42210</v>
       </c>
       <c r="B664" t="s">
         <v>7</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A665" s="1">
-        <v>42209</v>
+        <v>42211</v>
       </c>
       <c r="B665" t="s">
         <v>7</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A666" s="1">
-        <v>42210</v>
+        <v>42212</v>
       </c>
       <c r="B666" t="s">
         <v>7</v>
@@ -5804,7 +5804,7 @@
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A667" s="1">
-        <v>42211</v>
+        <v>42213</v>
       </c>
       <c r="B667" t="s">
         <v>7</v>
@@ -5812,7 +5812,7 @@
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A668" s="1">
-        <v>42212</v>
+        <v>42214</v>
       </c>
       <c r="B668" t="s">
         <v>7</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A669" s="1">
-        <v>42213</v>
+        <v>42215</v>
       </c>
       <c r="B669" t="s">
         <v>7</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A670" s="1">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B670" t="s">
         <v>7</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A671" s="1">
-        <v>42215</v>
+        <v>42217</v>
       </c>
       <c r="B671" t="s">
         <v>7</v>
@@ -5844,7 +5844,7 @@
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A672" s="1">
-        <v>42216</v>
+        <v>42218</v>
       </c>
       <c r="B672" t="s">
         <v>7</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A673" s="1">
-        <v>42217</v>
+        <v>42219</v>
       </c>
       <c r="B673" t="s">
         <v>7</v>
@@ -5860,7 +5860,7 @@
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A674" s="1">
-        <v>42218</v>
+        <v>42220</v>
       </c>
       <c r="B674" t="s">
         <v>7</v>
@@ -5868,7 +5868,7 @@
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A675" s="1">
-        <v>42219</v>
+        <v>42221</v>
       </c>
       <c r="B675" t="s">
         <v>7</v>
@@ -5876,7 +5876,7 @@
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A676" s="1">
-        <v>42220</v>
+        <v>42222</v>
       </c>
       <c r="B676" t="s">
         <v>7</v>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A677" s="1">
-        <v>42221</v>
+        <v>42223</v>
       </c>
       <c r="B677" t="s">
         <v>7</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A678" s="1">
-        <v>42222</v>
+        <v>42224</v>
       </c>
       <c r="B678" t="s">
         <v>7</v>
@@ -5900,7 +5900,7 @@
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A679" s="1">
-        <v>42223</v>
+        <v>42225</v>
       </c>
       <c r="B679" t="s">
         <v>7</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A680" s="1">
-        <v>42224</v>
+        <v>42546</v>
       </c>
       <c r="B680" t="s">
         <v>7</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A681" s="1">
-        <v>42225</v>
+        <v>42547</v>
       </c>
       <c r="B681" t="s">
         <v>7</v>
@@ -5924,7 +5924,7 @@
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A682" s="1">
-        <v>42546</v>
+        <v>42548</v>
       </c>
       <c r="B682" t="s">
         <v>7</v>
@@ -5932,7 +5932,7 @@
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A683" s="1">
-        <v>42547</v>
+        <v>42549</v>
       </c>
       <c r="B683" t="s">
         <v>7</v>
@@ -5940,7 +5940,7 @@
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A684" s="1">
-        <v>42548</v>
+        <v>42550</v>
       </c>
       <c r="B684" t="s">
         <v>7</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A685" s="1">
-        <v>42549</v>
+        <v>42551</v>
       </c>
       <c r="B685" t="s">
         <v>7</v>
@@ -5956,7 +5956,7 @@
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A686" s="1">
-        <v>42550</v>
+        <v>42552</v>
       </c>
       <c r="B686" t="s">
         <v>7</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A687" s="1">
-        <v>42551</v>
+        <v>42553</v>
       </c>
       <c r="B687" t="s">
         <v>7</v>
@@ -5972,7 +5972,7 @@
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A688" s="1">
-        <v>42552</v>
+        <v>42554</v>
       </c>
       <c r="B688" t="s">
         <v>7</v>
@@ -5980,7 +5980,7 @@
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A689" s="1">
-        <v>42553</v>
+        <v>42555</v>
       </c>
       <c r="B689" t="s">
         <v>7</v>
@@ -5988,7 +5988,7 @@
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A690" s="1">
-        <v>42554</v>
+        <v>42556</v>
       </c>
       <c r="B690" t="s">
         <v>7</v>
@@ -5996,7 +5996,7 @@
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A691" s="1">
-        <v>42555</v>
+        <v>42557</v>
       </c>
       <c r="B691" t="s">
         <v>7</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A692" s="1">
-        <v>42556</v>
+        <v>42558</v>
       </c>
       <c r="B692" t="s">
         <v>7</v>
@@ -6012,7 +6012,7 @@
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A693" s="1">
-        <v>42557</v>
+        <v>42559</v>
       </c>
       <c r="B693" t="s">
         <v>7</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A694" s="1">
-        <v>42558</v>
+        <v>42560</v>
       </c>
       <c r="B694" t="s">
         <v>7</v>
@@ -6028,7 +6028,7 @@
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A695" s="1">
-        <v>42559</v>
+        <v>42561</v>
       </c>
       <c r="B695" t="s">
         <v>7</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A696" s="1">
-        <v>42560</v>
+        <v>42562</v>
       </c>
       <c r="B696" t="s">
         <v>7</v>
@@ -6044,7 +6044,7 @@
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A697" s="1">
-        <v>42561</v>
+        <v>42563</v>
       </c>
       <c r="B697" t="s">
         <v>7</v>
@@ -6052,7 +6052,7 @@
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A698" s="1">
-        <v>42562</v>
+        <v>42564</v>
       </c>
       <c r="B698" t="s">
         <v>7</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A699" s="1">
-        <v>42563</v>
+        <v>42565</v>
       </c>
       <c r="B699" t="s">
         <v>7</v>
@@ -6068,7 +6068,7 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A700" s="1">
-        <v>42564</v>
+        <v>42566</v>
       </c>
       <c r="B700" t="s">
         <v>7</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A701" s="1">
-        <v>42565</v>
+        <v>42567</v>
       </c>
       <c r="B701" t="s">
         <v>7</v>
@@ -6084,7 +6084,7 @@
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A702" s="1">
-        <v>42566</v>
+        <v>42568</v>
       </c>
       <c r="B702" t="s">
         <v>7</v>
@@ -6092,7 +6092,7 @@
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A703" s="1">
-        <v>42567</v>
+        <v>42569</v>
       </c>
       <c r="B703" t="s">
         <v>7</v>
@@ -6100,7 +6100,7 @@
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A704" s="1">
-        <v>42568</v>
+        <v>42570</v>
       </c>
       <c r="B704" t="s">
         <v>7</v>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A705" s="1">
-        <v>42569</v>
+        <v>42571</v>
       </c>
       <c r="B705" t="s">
         <v>7</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A706" s="1">
-        <v>42570</v>
+        <v>42572</v>
       </c>
       <c r="B706" t="s">
         <v>7</v>
@@ -6124,7 +6124,7 @@
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A707" s="1">
-        <v>42571</v>
+        <v>42573</v>
       </c>
       <c r="B707" t="s">
         <v>7</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A708" s="1">
-        <v>42572</v>
+        <v>42574</v>
       </c>
       <c r="B708" t="s">
         <v>7</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A709" s="1">
-        <v>42573</v>
+        <v>42575</v>
       </c>
       <c r="B709" t="s">
         <v>7</v>
@@ -6148,7 +6148,7 @@
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A710" s="1">
-        <v>42574</v>
+        <v>42576</v>
       </c>
       <c r="B710" t="s">
         <v>7</v>
@@ -6156,7 +6156,7 @@
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A711" s="1">
-        <v>42575</v>
+        <v>42577</v>
       </c>
       <c r="B711" t="s">
         <v>7</v>
@@ -6164,7 +6164,7 @@
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A712" s="1">
-        <v>42576</v>
+        <v>42578</v>
       </c>
       <c r="B712" t="s">
         <v>7</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A713" s="1">
-        <v>42577</v>
+        <v>42579</v>
       </c>
       <c r="B713" t="s">
         <v>7</v>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A714" s="1">
-        <v>42578</v>
+        <v>42580</v>
       </c>
       <c r="B714" t="s">
         <v>7</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A715" s="1">
-        <v>42579</v>
+        <v>42581</v>
       </c>
       <c r="B715" t="s">
         <v>7</v>
@@ -6196,7 +6196,7 @@
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A716" s="1">
-        <v>42580</v>
+        <v>42582</v>
       </c>
       <c r="B716" t="s">
         <v>7</v>
@@ -6204,7 +6204,7 @@
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A717" s="1">
-        <v>42581</v>
+        <v>42583</v>
       </c>
       <c r="B717" t="s">
         <v>7</v>
@@ -6212,7 +6212,7 @@
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A718" s="1">
-        <v>42582</v>
+        <v>42584</v>
       </c>
       <c r="B718" t="s">
         <v>7</v>
@@ -6220,7 +6220,7 @@
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A719" s="1">
-        <v>42583</v>
+        <v>42585</v>
       </c>
       <c r="B719" t="s">
         <v>7</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A720" s="1">
-        <v>42584</v>
+        <v>42586</v>
       </c>
       <c r="B720" t="s">
         <v>7</v>
@@ -6236,7 +6236,7 @@
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A721" s="1">
-        <v>42585</v>
+        <v>42587</v>
       </c>
       <c r="B721" t="s">
         <v>7</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" s="1">
-        <v>42586</v>
+        <v>42588</v>
       </c>
       <c r="B722" t="s">
         <v>7</v>
@@ -6252,7 +6252,7 @@
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A723" s="1">
-        <v>42587</v>
+        <v>42589</v>
       </c>
       <c r="B723" t="s">
         <v>7</v>
@@ -6260,7 +6260,7 @@
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A724" s="1">
-        <v>42588</v>
+        <v>42590</v>
       </c>
       <c r="B724" t="s">
         <v>7</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A725" s="1">
-        <v>42589</v>
+        <v>42911</v>
       </c>
       <c r="B725" t="s">
         <v>7</v>
@@ -6276,7 +6276,7 @@
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A726" s="1">
-        <v>42590</v>
+        <v>42912</v>
       </c>
       <c r="B726" t="s">
         <v>7</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A727" s="1">
-        <v>42911</v>
+        <v>42913</v>
       </c>
       <c r="B727" t="s">
         <v>7</v>
@@ -6292,7 +6292,7 @@
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A728" s="1">
-        <v>42912</v>
+        <v>42914</v>
       </c>
       <c r="B728" t="s">
         <v>7</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A729" s="1">
-        <v>42913</v>
+        <v>42915</v>
       </c>
       <c r="B729" t="s">
         <v>7</v>
@@ -6308,7 +6308,7 @@
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A730" s="1">
-        <v>42914</v>
+        <v>42916</v>
       </c>
       <c r="B730" t="s">
         <v>7</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A731" s="1">
-        <v>42915</v>
+        <v>42917</v>
       </c>
       <c r="B731" t="s">
         <v>7</v>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A732" s="1">
-        <v>42916</v>
+        <v>42918</v>
       </c>
       <c r="B732" t="s">
         <v>7</v>
@@ -6332,7 +6332,7 @@
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A733" s="1">
-        <v>42917</v>
+        <v>42919</v>
       </c>
       <c r="B733" t="s">
         <v>7</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A734" s="1">
-        <v>42918</v>
+        <v>42920</v>
       </c>
       <c r="B734" t="s">
         <v>7</v>
@@ -6348,7 +6348,7 @@
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A735" s="1">
-        <v>42919</v>
+        <v>42921</v>
       </c>
       <c r="B735" t="s">
         <v>7</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A736" s="1">
-        <v>42920</v>
+        <v>42922</v>
       </c>
       <c r="B736" t="s">
         <v>7</v>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A737" s="1">
-        <v>42921</v>
+        <v>42923</v>
       </c>
       <c r="B737" t="s">
         <v>7</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A738" s="1">
-        <v>42922</v>
+        <v>42924</v>
       </c>
       <c r="B738" t="s">
         <v>7</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A739" s="1">
-        <v>42923</v>
+        <v>42925</v>
       </c>
       <c r="B739" t="s">
         <v>7</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A740" s="1">
-        <v>42924</v>
+        <v>42926</v>
       </c>
       <c r="B740" t="s">
         <v>7</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A741" s="1">
-        <v>42925</v>
+        <v>42927</v>
       </c>
       <c r="B741" t="s">
         <v>7</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A742" s="1">
-        <v>42926</v>
+        <v>42928</v>
       </c>
       <c r="B742" t="s">
         <v>7</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A743" s="1">
-        <v>42927</v>
+        <v>42929</v>
       </c>
       <c r="B743" t="s">
         <v>7</v>
@@ -6420,7 +6420,7 @@
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A744" s="1">
-        <v>42928</v>
+        <v>42930</v>
       </c>
       <c r="B744" t="s">
         <v>7</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A745" s="1">
-        <v>42929</v>
+        <v>42931</v>
       </c>
       <c r="B745" t="s">
         <v>7</v>
@@ -6436,7 +6436,7 @@
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A746" s="1">
-        <v>42930</v>
+        <v>42932</v>
       </c>
       <c r="B746" t="s">
         <v>7</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A747" s="1">
-        <v>42931</v>
+        <v>42933</v>
       </c>
       <c r="B747" t="s">
         <v>7</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A748" s="1">
-        <v>42932</v>
+        <v>42934</v>
       </c>
       <c r="B748" t="s">
         <v>7</v>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A749" s="1">
-        <v>42933</v>
+        <v>42935</v>
       </c>
       <c r="B749" t="s">
         <v>7</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A750" s="1">
-        <v>42934</v>
+        <v>42936</v>
       </c>
       <c r="B750" t="s">
         <v>7</v>
@@ -6476,7 +6476,7 @@
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A751" s="1">
-        <v>42935</v>
+        <v>42937</v>
       </c>
       <c r="B751" t="s">
         <v>7</v>
@@ -6484,7 +6484,7 @@
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A752" s="1">
-        <v>42936</v>
+        <v>42938</v>
       </c>
       <c r="B752" t="s">
         <v>7</v>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A753" s="1">
-        <v>42937</v>
+        <v>42939</v>
       </c>
       <c r="B753" t="s">
         <v>7</v>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A754" s="1">
-        <v>42938</v>
+        <v>42940</v>
       </c>
       <c r="B754" t="s">
         <v>7</v>
@@ -6508,7 +6508,7 @@
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A755" s="1">
-        <v>42939</v>
+        <v>42941</v>
       </c>
       <c r="B755" t="s">
         <v>7</v>
@@ -6516,7 +6516,7 @@
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A756" s="1">
-        <v>42940</v>
+        <v>42942</v>
       </c>
       <c r="B756" t="s">
         <v>7</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A757" s="1">
-        <v>42941</v>
+        <v>42943</v>
       </c>
       <c r="B757" t="s">
         <v>7</v>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A758" s="1">
-        <v>42942</v>
+        <v>42944</v>
       </c>
       <c r="B758" t="s">
         <v>7</v>
@@ -6540,7 +6540,7 @@
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A759" s="1">
-        <v>42943</v>
+        <v>42945</v>
       </c>
       <c r="B759" t="s">
         <v>7</v>
@@ -6548,7 +6548,7 @@
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A760" s="1">
-        <v>42944</v>
+        <v>42946</v>
       </c>
       <c r="B760" t="s">
         <v>7</v>
@@ -6556,7 +6556,7 @@
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A761" s="1">
-        <v>42945</v>
+        <v>43276</v>
       </c>
       <c r="B761" t="s">
         <v>7</v>
@@ -6564,7 +6564,7 @@
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A762" s="1">
-        <v>42946</v>
+        <v>43277</v>
       </c>
       <c r="B762" t="s">
         <v>7</v>
@@ -6572,7 +6572,7 @@
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A763" s="1">
-        <v>43276</v>
+        <v>43278</v>
       </c>
       <c r="B763" t="s">
         <v>7</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A764" s="1">
-        <v>43277</v>
+        <v>43279</v>
       </c>
       <c r="B764" t="s">
         <v>7</v>
@@ -6588,7 +6588,7 @@
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A765" s="1">
-        <v>43278</v>
+        <v>43280</v>
       </c>
       <c r="B765" t="s">
         <v>7</v>
@@ -6596,7 +6596,7 @@
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A766" s="1">
-        <v>43279</v>
+        <v>43281</v>
       </c>
       <c r="B766" t="s">
         <v>7</v>
@@ -6604,7 +6604,7 @@
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A767" s="1">
-        <v>43280</v>
+        <v>43282</v>
       </c>
       <c r="B767" t="s">
         <v>7</v>
@@ -6612,7 +6612,7 @@
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A768" s="1">
-        <v>43281</v>
+        <v>43283</v>
       </c>
       <c r="B768" t="s">
         <v>7</v>
@@ -6620,7 +6620,7 @@
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A769" s="1">
-        <v>43282</v>
+        <v>43284</v>
       </c>
       <c r="B769" t="s">
         <v>7</v>
@@ -6628,7 +6628,7 @@
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A770" s="1">
-        <v>43283</v>
+        <v>43285</v>
       </c>
       <c r="B770" t="s">
         <v>7</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A771" s="1">
-        <v>43284</v>
+        <v>43286</v>
       </c>
       <c r="B771" t="s">
         <v>7</v>
@@ -6644,7 +6644,7 @@
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A772" s="1">
-        <v>43285</v>
+        <v>43287</v>
       </c>
       <c r="B772" t="s">
         <v>7</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A773" s="1">
-        <v>43286</v>
+        <v>43288</v>
       </c>
       <c r="B773" t="s">
         <v>7</v>
@@ -6660,7 +6660,7 @@
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A774" s="1">
-        <v>43287</v>
+        <v>43289</v>
       </c>
       <c r="B774" t="s">
         <v>7</v>
@@ -6668,7 +6668,7 @@
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A775" s="1">
-        <v>43288</v>
+        <v>43290</v>
       </c>
       <c r="B775" t="s">
         <v>7</v>
@@ -6676,7 +6676,7 @@
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A776" s="1">
-        <v>43289</v>
+        <v>43291</v>
       </c>
       <c r="B776" t="s">
         <v>7</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A777" s="1">
-        <v>43290</v>
+        <v>43292</v>
       </c>
       <c r="B777" t="s">
         <v>7</v>
@@ -6692,7 +6692,7 @@
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A778" s="1">
-        <v>43291</v>
+        <v>43293</v>
       </c>
       <c r="B778" t="s">
         <v>7</v>
@@ -6700,7 +6700,7 @@
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A779" s="1">
-        <v>43292</v>
+        <v>43294</v>
       </c>
       <c r="B779" t="s">
         <v>7</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A780" s="1">
-        <v>43293</v>
+        <v>43295</v>
       </c>
       <c r="B780" t="s">
         <v>7</v>
@@ -6716,7 +6716,7 @@
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A781" s="1">
-        <v>43294</v>
+        <v>43296</v>
       </c>
       <c r="B781" t="s">
         <v>7</v>
@@ -6724,7 +6724,7 @@
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A782" s="1">
-        <v>43295</v>
+        <v>43297</v>
       </c>
       <c r="B782" t="s">
         <v>7</v>
@@ -6732,7 +6732,7 @@
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A783" s="1">
-        <v>43296</v>
+        <v>43298</v>
       </c>
       <c r="B783" t="s">
         <v>7</v>
@@ -6740,7 +6740,7 @@
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A784" s="1">
-        <v>43297</v>
+        <v>43299</v>
       </c>
       <c r="B784" t="s">
         <v>7</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A785" s="1">
-        <v>43298</v>
+        <v>43300</v>
       </c>
       <c r="B785" t="s">
         <v>7</v>
@@ -6756,7 +6756,7 @@
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A786" s="1">
-        <v>43299</v>
+        <v>43301</v>
       </c>
       <c r="B786" t="s">
         <v>7</v>
@@ -6764,7 +6764,7 @@
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A787" s="1">
-        <v>43300</v>
+        <v>43302</v>
       </c>
       <c r="B787" t="s">
         <v>7</v>
@@ -6772,7 +6772,7 @@
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A788" s="1">
-        <v>43301</v>
+        <v>43303</v>
       </c>
       <c r="B788" t="s">
         <v>7</v>
@@ -6780,7 +6780,7 @@
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A789" s="1">
-        <v>43302</v>
+        <v>43304</v>
       </c>
       <c r="B789" t="s">
         <v>7</v>
@@ -6788,7 +6788,7 @@
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A790" s="1">
-        <v>43303</v>
+        <v>43305</v>
       </c>
       <c r="B790" t="s">
         <v>7</v>
@@ -6796,7 +6796,7 @@
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A791" s="1">
-        <v>43304</v>
+        <v>43306</v>
       </c>
       <c r="B791" t="s">
         <v>7</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A792" s="1">
-        <v>43305</v>
+        <v>43307</v>
       </c>
       <c r="B792" t="s">
         <v>7</v>
@@ -6812,7 +6812,7 @@
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A793" s="1">
-        <v>43306</v>
+        <v>43308</v>
       </c>
       <c r="B793" t="s">
         <v>7</v>
@@ -6820,7 +6820,7 @@
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A794" s="1">
-        <v>43307</v>
+        <v>43309</v>
       </c>
       <c r="B794" t="s">
         <v>7</v>
@@ -6828,7 +6828,7 @@
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A795" s="1">
-        <v>43308</v>
+        <v>43310</v>
       </c>
       <c r="B795" t="s">
         <v>7</v>
@@ -6836,7 +6836,7 @@
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A796" s="1">
-        <v>43309</v>
+        <v>43311</v>
       </c>
       <c r="B796" t="s">
         <v>7</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A797" s="1">
-        <v>43310</v>
+        <v>43312</v>
       </c>
       <c r="B797" t="s">
         <v>7</v>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A798" s="1">
-        <v>43311</v>
+        <v>43641</v>
       </c>
       <c r="B798" t="s">
         <v>7</v>
@@ -6860,7 +6860,7 @@
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A799" s="1">
-        <v>43312</v>
+        <v>43642</v>
       </c>
       <c r="B799" t="s">
         <v>7</v>
@@ -6868,7 +6868,7 @@
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A800" s="1">
-        <v>43641</v>
+        <v>43643</v>
       </c>
       <c r="B800" t="s">
         <v>7</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A801" s="1">
-        <v>43642</v>
+        <v>43644</v>
       </c>
       <c r="B801" t="s">
         <v>7</v>
@@ -6884,7 +6884,7 @@
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A802" s="1">
-        <v>43643</v>
+        <v>43645</v>
       </c>
       <c r="B802" t="s">
         <v>7</v>
@@ -6892,7 +6892,7 @@
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A803" s="1">
-        <v>43644</v>
+        <v>43646</v>
       </c>
       <c r="B803" t="s">
         <v>7</v>
@@ -6900,7 +6900,7 @@
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A804" s="1">
-        <v>43645</v>
+        <v>43647</v>
       </c>
       <c r="B804" t="s">
         <v>7</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A805" s="1">
-        <v>43646</v>
+        <v>43648</v>
       </c>
       <c r="B805" t="s">
         <v>7</v>
@@ -6916,7 +6916,7 @@
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A806" s="1">
-        <v>43647</v>
+        <v>43649</v>
       </c>
       <c r="B806" t="s">
         <v>7</v>
@@ -6924,7 +6924,7 @@
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A807" s="1">
-        <v>43648</v>
+        <v>43650</v>
       </c>
       <c r="B807" t="s">
         <v>7</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A808" s="1">
-        <v>43649</v>
+        <v>43651</v>
       </c>
       <c r="B808" t="s">
         <v>7</v>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A809" s="1">
-        <v>43650</v>
+        <v>43652</v>
       </c>
       <c r="B809" t="s">
         <v>7</v>
@@ -6948,7 +6948,7 @@
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A810" s="1">
-        <v>43651</v>
+        <v>43653</v>
       </c>
       <c r="B810" t="s">
         <v>7</v>
@@ -6956,7 +6956,7 @@
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A811" s="1">
-        <v>43652</v>
+        <v>43654</v>
       </c>
       <c r="B811" t="s">
         <v>7</v>
@@ -6964,7 +6964,7 @@
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A812" s="1">
-        <v>43653</v>
+        <v>43655</v>
       </c>
       <c r="B812" t="s">
         <v>7</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A813" s="1">
-        <v>43654</v>
+        <v>43656</v>
       </c>
       <c r="B813" t="s">
         <v>7</v>
@@ -6980,7 +6980,7 @@
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A814" s="1">
-        <v>43655</v>
+        <v>43657</v>
       </c>
       <c r="B814" t="s">
         <v>7</v>
@@ -6988,7 +6988,7 @@
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A815" s="1">
-        <v>43656</v>
+        <v>43658</v>
       </c>
       <c r="B815" t="s">
         <v>7</v>
@@ -6996,7 +6996,7 @@
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A816" s="1">
-        <v>43657</v>
+        <v>43659</v>
       </c>
       <c r="B816" t="s">
         <v>7</v>
@@ -7004,7 +7004,7 @@
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A817" s="1">
-        <v>43658</v>
+        <v>43660</v>
       </c>
       <c r="B817" t="s">
         <v>7</v>
@@ -7012,7 +7012,7 @@
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A818" s="1">
-        <v>43659</v>
+        <v>43661</v>
       </c>
       <c r="B818" t="s">
         <v>7</v>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A819" s="1">
-        <v>43660</v>
+        <v>43662</v>
       </c>
       <c r="B819" t="s">
         <v>7</v>
@@ -7028,7 +7028,7 @@
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A820" s="1">
-        <v>43661</v>
+        <v>43663</v>
       </c>
       <c r="B820" t="s">
         <v>7</v>
@@ -7036,7 +7036,7 @@
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A821" s="1">
-        <v>43662</v>
+        <v>43664</v>
       </c>
       <c r="B821" t="s">
         <v>7</v>
@@ -7044,7 +7044,7 @@
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A822" s="1">
-        <v>43663</v>
+        <v>43665</v>
       </c>
       <c r="B822" t="s">
         <v>7</v>
@@ -7052,7 +7052,7 @@
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A823" s="1">
-        <v>43664</v>
+        <v>43666</v>
       </c>
       <c r="B823" t="s">
         <v>7</v>
@@ -7060,7 +7060,7 @@
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A824" s="1">
-        <v>43665</v>
+        <v>43667</v>
       </c>
       <c r="B824" t="s">
         <v>7</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A825" s="1">
-        <v>43666</v>
+        <v>43668</v>
       </c>
       <c r="B825" t="s">
         <v>7</v>
@@ -7076,7 +7076,7 @@
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A826" s="1">
-        <v>43667</v>
+        <v>43669</v>
       </c>
       <c r="B826" t="s">
         <v>7</v>
@@ -7084,7 +7084,7 @@
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A827" s="1">
-        <v>43668</v>
+        <v>43670</v>
       </c>
       <c r="B827" t="s">
         <v>7</v>
@@ -7092,7 +7092,7 @@
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A828" s="1">
-        <v>43669</v>
+        <v>43671</v>
       </c>
       <c r="B828" t="s">
         <v>7</v>
@@ -7100,7 +7100,7 @@
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A829" s="1">
-        <v>43670</v>
+        <v>43672</v>
       </c>
       <c r="B829" t="s">
         <v>7</v>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A830" s="1">
-        <v>43671</v>
+        <v>43673</v>
       </c>
       <c r="B830" t="s">
         <v>7</v>
@@ -7116,7 +7116,7 @@
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A831" s="1">
-        <v>43672</v>
+        <v>43674</v>
       </c>
       <c r="B831" t="s">
         <v>7</v>
@@ -7124,7 +7124,7 @@
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A832" s="1">
-        <v>43673</v>
+        <v>43675</v>
       </c>
       <c r="B832" t="s">
         <v>7</v>
@@ -7132,7 +7132,7 @@
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A833" s="1">
-        <v>43674</v>
+        <v>43676</v>
       </c>
       <c r="B833" t="s">
         <v>7</v>
@@ -7140,7 +7140,7 @@
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="1">
-        <v>43675</v>
+        <v>44737</v>
       </c>
       <c r="B834" t="s">
         <v>7</v>
@@ -7148,7 +7148,7 @@
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="1">
-        <v>43676</v>
+        <v>44738</v>
       </c>
       <c r="B835" t="s">
         <v>7</v>
@@ -7156,7 +7156,7 @@
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="1">
-        <v>44737</v>
+        <v>44739</v>
       </c>
       <c r="B836" t="s">
         <v>7</v>
@@ -7164,7 +7164,7 @@
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A837" s="1">
-        <v>44738</v>
+        <v>44740</v>
       </c>
       <c r="B837" t="s">
         <v>7</v>
@@ -7172,7 +7172,7 @@
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A838" s="1">
-        <v>44739</v>
+        <v>44741</v>
       </c>
       <c r="B838" t="s">
         <v>7</v>
@@ -7180,7 +7180,7 @@
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A839" s="1">
-        <v>44740</v>
+        <v>44742</v>
       </c>
       <c r="B839" t="s">
         <v>7</v>
@@ -7188,7 +7188,7 @@
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="1">
-        <v>44741</v>
+        <v>44743</v>
       </c>
       <c r="B840" t="s">
         <v>7</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A841" s="1">
-        <v>44742</v>
+        <v>44744</v>
       </c>
       <c r="B841" t="s">
         <v>7</v>
@@ -7204,7 +7204,7 @@
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="1">
-        <v>44743</v>
+        <v>44745</v>
       </c>
       <c r="B842" t="s">
         <v>7</v>
@@ -7212,7 +7212,7 @@
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A843" s="1">
-        <v>44744</v>
+        <v>44746</v>
       </c>
       <c r="B843" t="s">
         <v>7</v>
@@ -7220,7 +7220,7 @@
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A844" s="1">
-        <v>44745</v>
+        <v>44747</v>
       </c>
       <c r="B844" t="s">
         <v>7</v>
@@ -7228,7 +7228,7 @@
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A845" s="1">
-        <v>44746</v>
+        <v>44748</v>
       </c>
       <c r="B845" t="s">
         <v>7</v>
@@ -7236,7 +7236,7 @@
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="1">
-        <v>44747</v>
+        <v>44749</v>
       </c>
       <c r="B846" t="s">
         <v>7</v>
@@ -7244,7 +7244,7 @@
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A847" s="1">
-        <v>44748</v>
+        <v>44750</v>
       </c>
       <c r="B847" t="s">
         <v>7</v>
@@ -7252,7 +7252,7 @@
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A848" s="1">
-        <v>44749</v>
+        <v>44751</v>
       </c>
       <c r="B848" t="s">
         <v>7</v>
@@ -7260,7 +7260,7 @@
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A849" s="1">
-        <v>44750</v>
+        <v>44752</v>
       </c>
       <c r="B849" t="s">
         <v>7</v>
@@ -7268,7 +7268,7 @@
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="1">
-        <v>44751</v>
+        <v>44753</v>
       </c>
       <c r="B850" t="s">
         <v>7</v>
@@ -7276,7 +7276,7 @@
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="1">
-        <v>44752</v>
+        <v>44754</v>
       </c>
       <c r="B851" t="s">
         <v>7</v>
@@ -7284,7 +7284,7 @@
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="1">
-        <v>44753</v>
+        <v>44755</v>
       </c>
       <c r="B852" t="s">
         <v>7</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="1">
-        <v>44754</v>
+        <v>44756</v>
       </c>
       <c r="B853" t="s">
         <v>7</v>
@@ -7300,7 +7300,7 @@
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="1">
-        <v>44755</v>
+        <v>44757</v>
       </c>
       <c r="B854" t="s">
         <v>7</v>
@@ -7308,7 +7308,7 @@
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="1">
-        <v>44756</v>
+        <v>44758</v>
       </c>
       <c r="B855" t="s">
         <v>7</v>
@@ -7316,7 +7316,7 @@
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="1">
-        <v>44757</v>
+        <v>44759</v>
       </c>
       <c r="B856" t="s">
         <v>7</v>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A857" s="1">
-        <v>44758</v>
+        <v>44760</v>
       </c>
       <c r="B857" t="s">
         <v>7</v>
@@ -7332,7 +7332,7 @@
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="1">
-        <v>44759</v>
+        <v>44761</v>
       </c>
       <c r="B858" t="s">
         <v>7</v>
@@ -7340,7 +7340,7 @@
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="1">
-        <v>44760</v>
+        <v>44762</v>
       </c>
       <c r="B859" t="s">
         <v>7</v>
@@ -7348,7 +7348,7 @@
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="1">
-        <v>44761</v>
+        <v>44763</v>
       </c>
       <c r="B860" t="s">
         <v>7</v>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="1">
-        <v>44762</v>
+        <v>44764</v>
       </c>
       <c r="B861" t="s">
         <v>7</v>
@@ -7364,7 +7364,7 @@
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="1">
-        <v>44763</v>
+        <v>44765</v>
       </c>
       <c r="B862" t="s">
         <v>7</v>
@@ -7372,7 +7372,7 @@
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="1">
-        <v>44764</v>
+        <v>44766</v>
       </c>
       <c r="B863" t="s">
         <v>7</v>
@@ -7380,7 +7380,7 @@
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="1">
-        <v>44765</v>
+        <v>44767</v>
       </c>
       <c r="B864" t="s">
         <v>7</v>
@@ -7388,7 +7388,7 @@
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="1">
-        <v>44766</v>
+        <v>44768</v>
       </c>
       <c r="B865" t="s">
         <v>7</v>
@@ -7396,7 +7396,7 @@
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="1">
-        <v>44767</v>
+        <v>44769</v>
       </c>
       <c r="B866" t="s">
         <v>7</v>
@@ -7404,7 +7404,7 @@
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="1">
-        <v>44768</v>
+        <v>44770</v>
       </c>
       <c r="B867" t="s">
         <v>7</v>
@@ -7412,7 +7412,7 @@
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="1">
-        <v>44769</v>
+        <v>44771</v>
       </c>
       <c r="B868" t="s">
         <v>7</v>
@@ -7420,7 +7420,7 @@
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="1">
-        <v>44770</v>
+        <v>44772</v>
       </c>
       <c r="B869" t="s">
         <v>7</v>
@@ -7428,7 +7428,7 @@
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="1">
-        <v>44771</v>
+        <v>44773</v>
       </c>
       <c r="B870" t="s">
         <v>7</v>
@@ -7436,23 +7436,25 @@
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="1">
-        <v>44772</v>
+        <v>44677</v>
       </c>
       <c r="B871" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="1">
-        <v>44773</v>
+        <f>A871+1</f>
+        <v>44678</v>
       </c>
       <c r="B872" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="1">
-        <v>44677</v>
+        <f t="shared" ref="A873:A877" si="7">A872+1</f>
+        <v>44679</v>
       </c>
       <c r="B873" t="s">
         <v>6</v>
@@ -7460,8 +7462,8 @@
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="1">
-        <f>A873+1</f>
-        <v>44678</v>
+        <f t="shared" si="7"/>
+        <v>44680</v>
       </c>
       <c r="B874" t="s">
         <v>6</v>
@@ -7469,8 +7471,8 @@
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="1">
-        <f t="shared" ref="A875:A879" si="7">A874+1</f>
-        <v>44679</v>
+        <f t="shared" si="7"/>
+        <v>44681</v>
       </c>
       <c r="B875" t="s">
         <v>6</v>
@@ -7479,7 +7481,7 @@
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="1">
         <f t="shared" si="7"/>
-        <v>44680</v>
+        <v>44682</v>
       </c>
       <c r="B876" t="s">
         <v>6</v>
@@ -7488,7 +7490,7 @@
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="1">
         <f t="shared" si="7"/>
-        <v>44681</v>
+        <v>44683</v>
       </c>
       <c r="B877" t="s">
         <v>6</v>
@@ -7496,8 +7498,7 @@
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="1">
-        <f t="shared" si="7"/>
-        <v>44682</v>
+        <v>44312</v>
       </c>
       <c r="B878" t="s">
         <v>6</v>
@@ -7505,8 +7506,8 @@
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="1">
-        <f t="shared" si="7"/>
-        <v>44683</v>
+        <f>A878+1</f>
+        <v>44313</v>
       </c>
       <c r="B879" t="s">
         <v>6</v>
@@ -7514,7 +7515,8 @@
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="1">
-        <v>44312</v>
+        <f t="shared" ref="A880:A884" si="8">A879+1</f>
+        <v>44314</v>
       </c>
       <c r="B880" t="s">
         <v>6</v>
@@ -7522,8 +7524,8 @@
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="1">
-        <f>A880+1</f>
-        <v>44313</v>
+        <f t="shared" si="8"/>
+        <v>44315</v>
       </c>
       <c r="B881" t="s">
         <v>6</v>
@@ -7531,8 +7533,8 @@
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="1">
-        <f t="shared" ref="A882:A886" si="8">A881+1</f>
-        <v>44314</v>
+        <f t="shared" si="8"/>
+        <v>44316</v>
       </c>
       <c r="B882" t="s">
         <v>6</v>
@@ -7541,7 +7543,7 @@
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="1">
         <f t="shared" si="8"/>
-        <v>44315</v>
+        <v>44317</v>
       </c>
       <c r="B883" t="s">
         <v>6</v>
@@ -7550,7 +7552,7 @@
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="1">
         <f t="shared" si="8"/>
-        <v>44316</v>
+        <v>44318</v>
       </c>
       <c r="B884" t="s">
         <v>6</v>
@@ -7558,8 +7560,7 @@
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="1">
-        <f t="shared" si="8"/>
-        <v>44317</v>
+        <v>43947</v>
       </c>
       <c r="B885" t="s">
         <v>6</v>
@@ -7567,8 +7568,8 @@
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="1">
-        <f t="shared" si="8"/>
-        <v>44318</v>
+        <f>A885+1</f>
+        <v>43948</v>
       </c>
       <c r="B886" t="s">
         <v>6</v>
@@ -7576,7 +7577,8 @@
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="1">
-        <v>43947</v>
+        <f t="shared" ref="A887:A891" si="9">A886+1</f>
+        <v>43949</v>
       </c>
       <c r="B887" t="s">
         <v>6</v>
@@ -7584,8 +7586,8 @@
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="1">
-        <f>A887+1</f>
-        <v>43948</v>
+        <f t="shared" si="9"/>
+        <v>43950</v>
       </c>
       <c r="B888" t="s">
         <v>6</v>
@@ -7593,8 +7595,8 @@
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="1">
-        <f t="shared" ref="A889:A893" si="9">A888+1</f>
-        <v>43949</v>
+        <f t="shared" si="9"/>
+        <v>43951</v>
       </c>
       <c r="B889" t="s">
         <v>6</v>
@@ -7603,7 +7605,7 @@
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="1">
         <f t="shared" si="9"/>
-        <v>43950</v>
+        <v>43952</v>
       </c>
       <c r="B890" t="s">
         <v>6</v>
@@ -7612,7 +7614,7 @@
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="1">
         <f t="shared" si="9"/>
-        <v>43951</v>
+        <v>43953</v>
       </c>
       <c r="B891" t="s">
         <v>6</v>
@@ -7620,25 +7622,23 @@
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="1">
-        <f t="shared" si="9"/>
-        <v>43952</v>
+        <v>44007</v>
       </c>
       <c r="B892" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A893" s="1">
-        <f t="shared" si="9"/>
-        <v>43953</v>
+        <v>44008</v>
       </c>
       <c r="B893" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="1">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="B894" t="s">
         <v>7</v>
@@ -7646,7 +7646,7 @@
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="1">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="B895" t="s">
         <v>7</v>
@@ -7654,7 +7654,7 @@
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="1">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="B896" t="s">
         <v>7</v>
@@ -7662,7 +7662,7 @@
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="1">
-        <v>44010</v>
+        <v>44012</v>
       </c>
       <c r="B897" t="s">
         <v>7</v>
@@ -7670,7 +7670,7 @@
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A898" s="1">
-        <v>44011</v>
+        <v>44013</v>
       </c>
       <c r="B898" t="s">
         <v>7</v>
@@ -7678,7 +7678,7 @@
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="1">
-        <v>44012</v>
+        <v>44014</v>
       </c>
       <c r="B899" t="s">
         <v>7</v>
@@ -7686,7 +7686,7 @@
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="1">
-        <v>44013</v>
+        <v>44015</v>
       </c>
       <c r="B900" t="s">
         <v>7</v>
@@ -7694,7 +7694,7 @@
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="1">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="B901" t="s">
         <v>7</v>
@@ -7702,7 +7702,7 @@
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="1">
-        <v>44015</v>
+        <v>44017</v>
       </c>
       <c r="B902" t="s">
         <v>7</v>
@@ -7710,7 +7710,7 @@
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="1">
-        <v>44016</v>
+        <v>44018</v>
       </c>
       <c r="B903" t="s">
         <v>7</v>
@@ -7718,7 +7718,7 @@
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="1">
-        <v>44017</v>
+        <v>44019</v>
       </c>
       <c r="B904" t="s">
         <v>7</v>
@@ -7726,7 +7726,7 @@
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="1">
-        <v>44018</v>
+        <v>44020</v>
       </c>
       <c r="B905" t="s">
         <v>7</v>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="1">
-        <v>44019</v>
+        <v>44021</v>
       </c>
       <c r="B906" t="s">
         <v>7</v>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="1">
-        <v>44020</v>
+        <v>44022</v>
       </c>
       <c r="B907" t="s">
         <v>7</v>
@@ -7750,7 +7750,7 @@
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="1">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="B908" t="s">
         <v>7</v>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A909" s="1">
-        <v>44022</v>
+        <v>44024</v>
       </c>
       <c r="B909" t="s">
         <v>7</v>
@@ -7766,7 +7766,7 @@
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="1">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="B910" t="s">
         <v>7</v>
@@ -7774,7 +7774,7 @@
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="1">
-        <v>44024</v>
+        <v>44026</v>
       </c>
       <c r="B911" t="s">
         <v>7</v>
@@ -7782,7 +7782,7 @@
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="1">
-        <v>44025</v>
+        <v>44027</v>
       </c>
       <c r="B912" t="s">
         <v>7</v>
@@ -7790,7 +7790,7 @@
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="1">
-        <v>44026</v>
+        <v>44028</v>
       </c>
       <c r="B913" t="s">
         <v>7</v>
@@ -7798,7 +7798,7 @@
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A914" s="1">
-        <v>44027</v>
+        <v>44029</v>
       </c>
       <c r="B914" t="s">
         <v>7</v>
@@ -7806,7 +7806,7 @@
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="1">
-        <v>44028</v>
+        <v>44030</v>
       </c>
       <c r="B915" t="s">
         <v>7</v>
@@ -7814,7 +7814,7 @@
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="1">
-        <v>44029</v>
+        <v>44031</v>
       </c>
       <c r="B916" t="s">
         <v>7</v>
@@ -7822,7 +7822,7 @@
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="1">
-        <v>44030</v>
+        <v>44032</v>
       </c>
       <c r="B917" t="s">
         <v>7</v>
@@ -7830,7 +7830,7 @@
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="1">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="B918" t="s">
         <v>7</v>
@@ -7838,7 +7838,7 @@
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A919" s="1">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="B919" t="s">
         <v>7</v>
@@ -7846,7 +7846,7 @@
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="1">
-        <v>44033</v>
+        <v>44035</v>
       </c>
       <c r="B920" t="s">
         <v>7</v>
@@ -7854,7 +7854,7 @@
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="1">
-        <v>44034</v>
+        <v>44036</v>
       </c>
       <c r="B921" t="s">
         <v>7</v>
@@ -7862,7 +7862,7 @@
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="1">
-        <v>44035</v>
+        <v>44037</v>
       </c>
       <c r="B922" t="s">
         <v>7</v>
@@ -7870,7 +7870,7 @@
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="1">
-        <v>44036</v>
+        <v>44038</v>
       </c>
       <c r="B923" t="s">
         <v>7</v>
@@ -7878,7 +7878,7 @@
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="1">
-        <v>44037</v>
+        <v>44039</v>
       </c>
       <c r="B924" t="s">
         <v>7</v>
@@ -7886,7 +7886,7 @@
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="1">
-        <v>44038</v>
+        <v>44040</v>
       </c>
       <c r="B925" t="s">
         <v>7</v>
@@ -7894,7 +7894,7 @@
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="1">
-        <v>44039</v>
+        <v>44041</v>
       </c>
       <c r="B926" t="s">
         <v>7</v>
@@ -7902,7 +7902,7 @@
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="1">
-        <v>44040</v>
+        <v>44042</v>
       </c>
       <c r="B927" t="s">
         <v>7</v>
@@ -7910,7 +7910,7 @@
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="1">
-        <v>44041</v>
+        <v>44043</v>
       </c>
       <c r="B928" t="s">
         <v>7</v>
@@ -7918,7 +7918,7 @@
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="1">
-        <v>44042</v>
+        <v>44372</v>
       </c>
       <c r="B929" t="s">
         <v>7</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="1">
-        <v>44043</v>
+        <v>44373</v>
       </c>
       <c r="B930" t="s">
         <v>7</v>
@@ -7934,7 +7934,7 @@
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="1">
-        <v>44372</v>
+        <v>44374</v>
       </c>
       <c r="B931" t="s">
         <v>7</v>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="1">
-        <v>44373</v>
+        <v>44375</v>
       </c>
       <c r="B932" t="s">
         <v>7</v>
@@ -7950,7 +7950,7 @@
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A933" s="1">
-        <v>44374</v>
+        <v>44376</v>
       </c>
       <c r="B933" t="s">
         <v>7</v>
@@ -7958,7 +7958,7 @@
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="1">
-        <v>44375</v>
+        <v>44377</v>
       </c>
       <c r="B934" t="s">
         <v>7</v>
@@ -7966,7 +7966,7 @@
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="1">
-        <v>44376</v>
+        <v>44378</v>
       </c>
       <c r="B935" t="s">
         <v>7</v>
@@ -7974,7 +7974,7 @@
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="1">
-        <v>44377</v>
+        <v>44379</v>
       </c>
       <c r="B936" t="s">
         <v>7</v>
@@ -7982,7 +7982,7 @@
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="1">
-        <v>44378</v>
+        <v>44380</v>
       </c>
       <c r="B937" t="s">
         <v>7</v>
@@ -7990,7 +7990,7 @@
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A938" s="1">
-        <v>44379</v>
+        <v>44381</v>
       </c>
       <c r="B938" t="s">
         <v>7</v>
@@ -7998,7 +7998,7 @@
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="1">
-        <v>44380</v>
+        <v>44382</v>
       </c>
       <c r="B939" t="s">
         <v>7</v>
@@ -8006,7 +8006,7 @@
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="1">
-        <v>44381</v>
+        <v>44383</v>
       </c>
       <c r="B940" t="s">
         <v>7</v>
@@ -8014,7 +8014,7 @@
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="1">
-        <v>44382</v>
+        <v>44384</v>
       </c>
       <c r="B941" t="s">
         <v>7</v>
@@ -8022,7 +8022,7 @@
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="1">
-        <v>44383</v>
+        <v>44385</v>
       </c>
       <c r="B942" t="s">
         <v>7</v>
@@ -8030,7 +8030,7 @@
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="1">
-        <v>44384</v>
+        <v>44386</v>
       </c>
       <c r="B943" t="s">
         <v>7</v>
@@ -8038,7 +8038,7 @@
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="1">
-        <v>44385</v>
+        <v>44387</v>
       </c>
       <c r="B944" t="s">
         <v>7</v>
@@ -8046,7 +8046,7 @@
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="1">
-        <v>44386</v>
+        <v>44388</v>
       </c>
       <c r="B945" t="s">
         <v>7</v>
@@ -8054,7 +8054,7 @@
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="1">
-        <v>44387</v>
+        <v>44389</v>
       </c>
       <c r="B946" t="s">
         <v>7</v>
@@ -8062,7 +8062,7 @@
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="1">
-        <v>44388</v>
+        <v>44390</v>
       </c>
       <c r="B947" t="s">
         <v>7</v>
@@ -8070,7 +8070,7 @@
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="1">
-        <v>44389</v>
+        <v>44391</v>
       </c>
       <c r="B948" t="s">
         <v>7</v>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="1">
-        <v>44390</v>
+        <v>44392</v>
       </c>
       <c r="B949" t="s">
         <v>7</v>
@@ -8086,7 +8086,7 @@
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A950" s="1">
-        <v>44391</v>
+        <v>44393</v>
       </c>
       <c r="B950" t="s">
         <v>7</v>
@@ -8094,7 +8094,7 @@
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A951" s="1">
-        <v>44392</v>
+        <v>44394</v>
       </c>
       <c r="B951" t="s">
         <v>7</v>
@@ -8102,7 +8102,7 @@
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A952" s="1">
-        <v>44393</v>
+        <v>44395</v>
       </c>
       <c r="B952" t="s">
         <v>7</v>
@@ -8110,7 +8110,7 @@
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A953" s="1">
-        <v>44394</v>
+        <v>44396</v>
       </c>
       <c r="B953" t="s">
         <v>7</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A954" s="1">
-        <v>44395</v>
+        <v>44397</v>
       </c>
       <c r="B954" t="s">
         <v>7</v>
@@ -8126,7 +8126,7 @@
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A955" s="1">
-        <v>44396</v>
+        <v>44398</v>
       </c>
       <c r="B955" t="s">
         <v>7</v>
@@ -8134,7 +8134,7 @@
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A956" s="1">
-        <v>44397</v>
+        <v>44399</v>
       </c>
       <c r="B956" t="s">
         <v>7</v>
@@ -8142,7 +8142,7 @@
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A957" s="1">
-        <v>44398</v>
+        <v>44400</v>
       </c>
       <c r="B957" t="s">
         <v>7</v>
@@ -8150,7 +8150,7 @@
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A958" s="1">
-        <v>44399</v>
+        <v>44401</v>
       </c>
       <c r="B958" t="s">
         <v>7</v>
@@ -8158,7 +8158,7 @@
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A959" s="1">
-        <v>44400</v>
+        <v>44402</v>
       </c>
       <c r="B959" t="s">
         <v>7</v>
@@ -8166,7 +8166,7 @@
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A960" s="1">
-        <v>44401</v>
+        <v>44403</v>
       </c>
       <c r="B960" t="s">
         <v>7</v>
@@ -8174,7 +8174,7 @@
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A961" s="1">
-        <v>44402</v>
+        <v>44404</v>
       </c>
       <c r="B961" t="s">
         <v>7</v>
@@ -8182,7 +8182,7 @@
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A962" s="1">
-        <v>44403</v>
+        <v>44405</v>
       </c>
       <c r="B962" t="s">
         <v>7</v>
@@ -8190,7 +8190,7 @@
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A963" s="1">
-        <v>44404</v>
+        <v>44406</v>
       </c>
       <c r="B963" t="s">
         <v>7</v>
@@ -8198,7 +8198,7 @@
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A964" s="1">
-        <v>44405</v>
+        <v>44407</v>
       </c>
       <c r="B964" t="s">
         <v>7</v>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A965" s="1">
-        <v>44406</v>
+        <v>44408</v>
       </c>
       <c r="B965" t="s">
         <v>7</v>
@@ -8214,23 +8214,23 @@
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A966" s="1">
-        <v>44407</v>
+        <v>43848</v>
       </c>
       <c r="B966" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A967" s="1">
-        <v>44408</v>
+        <v>43849</v>
       </c>
       <c r="B967" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A968" s="1">
-        <v>43848</v>
+        <v>43850</v>
       </c>
       <c r="B968" t="s">
         <v>5</v>
@@ -8238,7 +8238,7 @@
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A969" s="1">
-        <v>43849</v>
+        <v>43851</v>
       </c>
       <c r="B969" t="s">
         <v>5</v>
@@ -8246,7 +8246,7 @@
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A970" s="1">
-        <v>43850</v>
+        <v>43852</v>
       </c>
       <c r="B970" t="s">
         <v>5</v>
@@ -8254,7 +8254,7 @@
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A971" s="1">
-        <v>43851</v>
+        <v>43853</v>
       </c>
       <c r="B971" t="s">
         <v>5</v>
@@ -8262,7 +8262,7 @@
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A972" s="1">
-        <v>43852</v>
+        <v>43855</v>
       </c>
       <c r="B972" t="s">
         <v>5</v>
@@ -8270,7 +8270,7 @@
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A973" s="1">
-        <v>43853</v>
+        <v>43856</v>
       </c>
       <c r="B973" t="s">
         <v>5</v>
@@ -8278,7 +8278,7 @@
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="1">
-        <v>43855</v>
+        <v>43857</v>
       </c>
       <c r="B974" t="s">
         <v>5</v>
@@ -8286,7 +8286,7 @@
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="1">
-        <v>43856</v>
+        <v>43858</v>
       </c>
       <c r="B975" t="s">
         <v>5</v>
@@ -8294,7 +8294,7 @@
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="1">
-        <v>43857</v>
+        <v>43859</v>
       </c>
       <c r="B976" t="s">
         <v>5</v>
@@ -8302,7 +8302,7 @@
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="1">
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="B977" t="s">
         <v>5</v>
@@ -8310,7 +8310,7 @@
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="1">
-        <v>43859</v>
+        <v>43861</v>
       </c>
       <c r="B978" t="s">
         <v>5</v>
@@ -8318,7 +8318,7 @@
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="1">
-        <v>43860</v>
+        <v>43862</v>
       </c>
       <c r="B979" t="s">
         <v>5</v>
@@ -8326,7 +8326,7 @@
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="1">
-        <v>43861</v>
+        <v>43863</v>
       </c>
       <c r="B980" t="s">
         <v>5</v>
@@ -8334,7 +8334,7 @@
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="1">
-        <v>43862</v>
+        <v>43864</v>
       </c>
       <c r="B981" t="s">
         <v>5</v>
@@ -8342,7 +8342,7 @@
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A982" s="1">
-        <v>43863</v>
+        <v>44232</v>
       </c>
       <c r="B982" t="s">
         <v>5</v>
@@ -8350,7 +8350,7 @@
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="1">
-        <v>43864</v>
+        <v>44233</v>
       </c>
       <c r="B983" t="s">
         <v>5</v>
@@ -8358,7 +8358,7 @@
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="1">
-        <v>44232</v>
+        <v>44234</v>
       </c>
       <c r="B984" t="s">
         <v>5</v>
@@ -8366,7 +8366,7 @@
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A985" s="1">
-        <v>44233</v>
+        <v>44235</v>
       </c>
       <c r="B985" t="s">
         <v>5</v>
@@ -8374,7 +8374,7 @@
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="1">
-        <v>44234</v>
+        <v>44236</v>
       </c>
       <c r="B986" t="s">
         <v>5</v>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="1">
-        <v>44235</v>
+        <v>44237</v>
       </c>
       <c r="B987" t="s">
         <v>5</v>
@@ -8390,7 +8390,7 @@
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="1">
-        <v>44236</v>
+        <v>44239</v>
       </c>
       <c r="B988" t="s">
         <v>5</v>
@@ -8398,7 +8398,7 @@
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="1">
-        <v>44237</v>
+        <v>44240</v>
       </c>
       <c r="B989" t="s">
         <v>5</v>
@@ -8406,7 +8406,7 @@
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A990" s="1">
-        <v>44239</v>
+        <v>44241</v>
       </c>
       <c r="B990" t="s">
         <v>5</v>
@@ -8414,7 +8414,7 @@
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="1">
-        <v>44240</v>
+        <v>44242</v>
       </c>
       <c r="B991" t="s">
         <v>5</v>
@@ -8422,7 +8422,7 @@
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="1">
-        <v>44241</v>
+        <v>44243</v>
       </c>
       <c r="B992" t="s">
         <v>5</v>
@@ -8430,7 +8430,7 @@
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="1">
-        <v>44242</v>
+        <v>44244</v>
       </c>
       <c r="B993" t="s">
         <v>5</v>
@@ -8438,7 +8438,7 @@
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="1">
-        <v>44243</v>
+        <v>44245</v>
       </c>
       <c r="B994" t="s">
         <v>5</v>
@@ -8446,7 +8446,7 @@
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="1">
-        <v>44244</v>
+        <v>44246</v>
       </c>
       <c r="B995" t="s">
         <v>5</v>
@@ -8454,7 +8454,7 @@
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="1">
-        <v>44245</v>
+        <v>44247</v>
       </c>
       <c r="B996" t="s">
         <v>5</v>
@@ -8462,30 +8462,14 @@
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="1">
-        <v>44246</v>
+        <v>44248</v>
       </c>
       <c r="B997" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="998" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A998" s="1">
-        <v>44247</v>
-      </c>
-      <c r="B998" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="999" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A999" s="1">
-        <v>44248</v>
-      </c>
-      <c r="B999" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B999" xr:uid="{DD25DBC2-16DB-4102-94CC-D4FC79081A1B}"/>
+  <autoFilter ref="A1:B997" xr:uid="{DD25DBC2-16DB-4102-94CC-D4FC79081A1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>